<commit_message>
Updated code on timestamp:   23-09-2021 - 17:26:37.27
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B528BC45-220F-42E5-AF90-B46409799871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DAA4A6-34F0-4845-A74D-085B5E1EAFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6274,8 +6274,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6293,6 +6293,7 @@
     <col min="11" max="11" width="30" style="10" customWidth="1"/>
     <col min="12" max="12" width="29.42578125" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" customWidth="1"/>
+    <col min="14" max="14" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 18:10:35.65
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DAA4A6-34F0-4845-A74D-085B5E1EAFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D705B0-57D0-452F-9232-F61B5FD1D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="871">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3067,6 +3067,129 @@
   </si>
   <si>
     <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/recursion-with-backtracking/n-queens-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java</t>
+  </si>
+  <si>
+    <t> Normal Queue Easy</t>
+  </si>
+  <si>
+    <t> Dynamic Queue Easy</t>
+  </si>
+  <si>
+    <t> Queue To Stack Adapter - Push Efficient Easy</t>
+  </si>
+  <si>
+    <t> Queue To Stack Adapter - Pop Efficient Easy</t>
+  </si>
+  <si>
+    <t> Stack To Queue Adapter - Add Efficient Easy</t>
+  </si>
+  <si>
+    <t> Stack To Queue Adapter - Remove Efficient Easy</t>
+  </si>
+  <si>
+    <t> Two Stacks In An Array</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/duplicate-brackets-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/balanced-brackets-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/next-greater-element-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stock-span-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/lah-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/sliding-window=maximum-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-evaluation-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-conversions-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/postfix-evaluation-conversions-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/prefix-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/celebrity-problem-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/merge-overlapping-interval-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/smallest-number-following-pattern-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-stack-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-stack-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/minimum-stack-i-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/min-stack-ii-official/ojquestion</t>
   </si>
 </sst>
 </file>
@@ -3954,12 +4077,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="14" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -3998,6 +4115,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="16" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Accent1" xfId="9" builtinId="30"/>
@@ -4409,10 +4532,10 @@
       <c r="C2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="157" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="141"/>
+      <c r="G2" s="157"/>
       <c r="J2" s="90" t="s">
         <v>294</v>
       </c>
@@ -6274,8 +6397,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6348,10 +6471,10 @@
       <c r="K3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="154" t="s">
+      <c r="L3" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="155" t="s">
+      <c r="M3" s="153" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6362,10 +6485,10 @@
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="147" t="s">
+      <c r="D4" s="145" t="s">
         <v>801</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="146" t="s">
         <v>800</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -6386,7 +6509,7 @@
       <c r="L4" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="156" t="s">
+      <c r="M4" s="154" t="s">
         <v>745</v>
       </c>
       <c r="N4" t="str">
@@ -6404,7 +6527,7 @@
       <c r="D5" s="140" t="s">
         <v>738</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="147" t="s">
         <v>802</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -6425,7 +6548,7 @@
       <c r="L5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="157" t="s">
+      <c r="M5" s="155" t="s">
         <v>746</v>
       </c>
       <c r="N5" t="str">
@@ -6443,7 +6566,7 @@
       <c r="D6" s="140" t="s">
         <v>739</v>
       </c>
-      <c r="E6" s="149" t="s">
+      <c r="E6" s="147" t="s">
         <v>803</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -6464,7 +6587,7 @@
       <c r="L6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="157" t="s">
+      <c r="M6" s="155" t="s">
         <v>747</v>
       </c>
       <c r="N6" t="str">
@@ -6482,7 +6605,7 @@
       <c r="D7" s="140" t="s">
         <v>740</v>
       </c>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="147" t="s">
         <v>804</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -6503,7 +6626,7 @@
       <c r="L7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="157" t="s">
+      <c r="M7" s="155" t="s">
         <v>748</v>
       </c>
       <c r="N7" t="str">
@@ -6521,7 +6644,7 @@
       <c r="D8" s="140" t="s">
         <v>741</v>
       </c>
-      <c r="E8" s="149" t="s">
+      <c r="E8" s="147" t="s">
         <v>805</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -6542,7 +6665,7 @@
       <c r="L8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="157" t="s">
+      <c r="M8" s="155" t="s">
         <v>749</v>
       </c>
       <c r="N8" t="str">
@@ -6557,7 +6680,7 @@
       <c r="D9" s="140" t="s">
         <v>742</v>
       </c>
-      <c r="E9" s="149" t="s">
+      <c r="E9" s="147" t="s">
         <v>806</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -6575,7 +6698,7 @@
       <c r="L9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="157" t="s">
+      <c r="M9" s="155" t="s">
         <v>750</v>
       </c>
       <c r="N9" t="str">
@@ -6593,7 +6716,7 @@
       <c r="D10" s="140" t="s">
         <v>743</v>
       </c>
-      <c r="E10" s="149" t="s">
+      <c r="E10" s="147" t="s">
         <v>807</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -6617,7 +6740,7 @@
       <c r="L10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="157" t="s">
+      <c r="M10" s="155" t="s">
         <v>751</v>
       </c>
       <c r="N10" t="str">
@@ -6635,7 +6758,7 @@
       <c r="D11" s="140" t="s">
         <v>744</v>
       </c>
-      <c r="E11" s="149" t="s">
+      <c r="E11" s="147" t="s">
         <v>808</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -6659,7 +6782,7 @@
       <c r="L11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="157" t="s">
+      <c r="M11" s="155" t="s">
         <v>752</v>
       </c>
       <c r="N11" t="str">
@@ -6674,10 +6797,10 @@
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="143" t="s">
+      <c r="D12" s="141" t="s">
         <v>776</v>
       </c>
-      <c r="E12" s="150" t="s">
+      <c r="E12" s="148" t="s">
         <v>809</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -6695,7 +6818,7 @@
       <c r="L12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="157" t="s">
+      <c r="M12" s="155" t="s">
         <v>753</v>
       </c>
       <c r="N12" t="str">
@@ -6710,10 +6833,10 @@
       <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="143" t="s">
+      <c r="D13" s="141" t="s">
         <v>777</v>
       </c>
-      <c r="E13" s="150" t="s">
+      <c r="E13" s="148" t="s">
         <v>810</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -6734,7 +6857,7 @@
       <c r="L13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="157" t="s">
+      <c r="M13" s="155" t="s">
         <v>754</v>
       </c>
       <c r="N13" t="str">
@@ -6749,10 +6872,10 @@
       <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="143" t="s">
+      <c r="D14" s="141" t="s">
         <v>778</v>
       </c>
-      <c r="E14" s="150" t="s">
+      <c r="E14" s="148" t="s">
         <v>811</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -6773,7 +6896,7 @@
       <c r="L14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="157" t="s">
+      <c r="M14" s="155" t="s">
         <v>755</v>
       </c>
       <c r="N14" t="str">
@@ -6788,10 +6911,10 @@
       <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="143" t="s">
+      <c r="D15" s="141" t="s">
         <v>779</v>
       </c>
-      <c r="E15" s="150" t="s">
+      <c r="E15" s="148" t="s">
         <v>812</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -6806,7 +6929,7 @@
       <c r="L15" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="M15" s="157" t="s">
+      <c r="M15" s="155" t="s">
         <v>756</v>
       </c>
       <c r="N15" t="str">
@@ -6821,10 +6944,10 @@
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="143" t="s">
+      <c r="D16" s="141" t="s">
         <v>780</v>
       </c>
-      <c r="E16" s="150" t="s">
+      <c r="E16" s="148" t="s">
         <v>813</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -6839,7 +6962,7 @@
       <c r="L16" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="M16" s="157" t="s">
+      <c r="M16" s="155" t="s">
         <v>757</v>
       </c>
       <c r="N16" t="str">
@@ -6854,10 +6977,10 @@
       <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="143" t="s">
+      <c r="D17" s="141" t="s">
         <v>781</v>
       </c>
-      <c r="E17" s="150" t="s">
+      <c r="E17" s="148" t="s">
         <v>814</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -6875,7 +6998,7 @@
       <c r="L17" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="M17" s="157" t="s">
+      <c r="M17" s="155" t="s">
         <v>758</v>
       </c>
       <c r="N17" t="str">
@@ -6890,10 +7013,10 @@
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="145" t="s">
+      <c r="D18" s="143" t="s">
         <v>782</v>
       </c>
-      <c r="E18" s="151" t="s">
+      <c r="E18" s="149" t="s">
         <v>815</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -6911,7 +7034,7 @@
       <c r="L18" s="16" t="s">
         <v>641</v>
       </c>
-      <c r="M18" s="157" t="s">
+      <c r="M18" s="155" t="s">
         <v>759</v>
       </c>
       <c r="N18" t="str">
@@ -6926,10 +7049,10 @@
       <c r="B19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="145" t="s">
+      <c r="D19" s="143" t="s">
         <v>783</v>
       </c>
-      <c r="E19" s="151" t="s">
+      <c r="E19" s="149" t="s">
         <v>816</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -6944,7 +7067,7 @@
       <c r="L19" s="16" t="s">
         <v>642</v>
       </c>
-      <c r="M19" s="157" t="s">
+      <c r="M19" s="155" t="s">
         <v>760</v>
       </c>
       <c r="N19" t="str">
@@ -6959,10 +7082,10 @@
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="145" t="s">
+      <c r="D20" s="143" t="s">
         <v>784</v>
       </c>
-      <c r="E20" s="151" t="s">
+      <c r="E20" s="149" t="s">
         <v>817</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -6977,7 +7100,7 @@
       <c r="L20" s="16" t="s">
         <v>640</v>
       </c>
-      <c r="M20" s="157" t="s">
+      <c r="M20" s="155" t="s">
         <v>761</v>
       </c>
       <c r="N20" t="str">
@@ -6992,10 +7115,10 @@
       <c r="B21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="145" t="s">
+      <c r="D21" s="143" t="s">
         <v>785</v>
       </c>
-      <c r="E21" s="151" t="s">
+      <c r="E21" s="149" t="s">
         <v>818</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -7010,7 +7133,7 @@
       <c r="L21" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="M21" s="157" t="s">
+      <c r="M21" s="155" t="s">
         <v>762</v>
       </c>
       <c r="N21" t="str">
@@ -7025,10 +7148,10 @@
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="145" t="s">
+      <c r="D22" s="143" t="s">
         <v>786</v>
       </c>
-      <c r="E22" s="151" t="s">
+      <c r="E22" s="149" t="s">
         <v>819</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -7043,7 +7166,7 @@
       <c r="L22" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="M22" s="157" t="s">
+      <c r="M22" s="155" t="s">
         <v>763</v>
       </c>
       <c r="N22" t="str">
@@ -7058,10 +7181,10 @@
       <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="144" t="s">
+      <c r="D23" s="142" t="s">
         <v>787</v>
       </c>
-      <c r="E23" s="152" t="s">
+      <c r="E23" s="150" t="s">
         <v>820</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -7082,7 +7205,7 @@
       <c r="L23" s="16" t="s">
         <v>637</v>
       </c>
-      <c r="M23" s="157" t="s">
+      <c r="M23" s="155" t="s">
         <v>764</v>
       </c>
       <c r="N23" t="str">
@@ -7097,10 +7220,10 @@
       <c r="B24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="144" t="s">
+      <c r="D24" s="142" t="s">
         <v>788</v>
       </c>
-      <c r="E24" s="152" t="s">
+      <c r="E24" s="150" t="s">
         <v>821</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -7121,7 +7244,7 @@
       <c r="L24" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="M24" s="157" t="s">
+      <c r="M24" s="155" t="s">
         <v>765</v>
       </c>
       <c r="N24" t="str">
@@ -7136,10 +7259,10 @@
       <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="144" t="s">
+      <c r="D25" s="142" t="s">
         <v>789</v>
       </c>
-      <c r="E25" s="152" t="s">
+      <c r="E25" s="150" t="s">
         <v>822</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -7157,7 +7280,7 @@
       <c r="L25" s="16" t="s">
         <v>633</v>
       </c>
-      <c r="M25" s="157" t="s">
+      <c r="M25" s="155" t="s">
         <v>766</v>
       </c>
       <c r="N25" t="str">
@@ -7172,10 +7295,10 @@
       <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="144" t="s">
+      <c r="D26" s="142" t="s">
         <v>790</v>
       </c>
-      <c r="E26" s="152" t="s">
+      <c r="E26" s="150" t="s">
         <v>823</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -7193,7 +7316,7 @@
       <c r="L26" s="16" t="s">
         <v>634</v>
       </c>
-      <c r="M26" s="157" t="s">
+      <c r="M26" s="155" t="s">
         <v>767</v>
       </c>
       <c r="N26" t="str">
@@ -7208,10 +7331,10 @@
       <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="144" t="s">
+      <c r="D27" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="E27" s="152" t="s">
+      <c r="E27" s="150" t="s">
         <v>824</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -7232,7 +7355,7 @@
       <c r="L27" s="16" t="s">
         <v>635</v>
       </c>
-      <c r="M27" s="157" t="s">
+      <c r="M27" s="155" t="s">
         <v>768</v>
       </c>
       <c r="N27" t="str">
@@ -7247,10 +7370,10 @@
       <c r="B28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="144" t="s">
+      <c r="D28" s="142" t="s">
         <v>792</v>
       </c>
-      <c r="E28" s="152" t="s">
+      <c r="E28" s="150" t="s">
         <v>825</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -7268,7 +7391,7 @@
       <c r="L28" s="16" t="s">
         <v>636</v>
       </c>
-      <c r="M28" s="157" t="s">
+      <c r="M28" s="155" t="s">
         <v>769</v>
       </c>
       <c r="N28" t="str">
@@ -7283,10 +7406,10 @@
       <c r="B29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="144" t="s">
+      <c r="D29" s="142" t="s">
         <v>793</v>
       </c>
-      <c r="E29" s="152" t="s">
+      <c r="E29" s="150" t="s">
         <v>826</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -7307,7 +7430,7 @@
       <c r="L29" s="16" t="s">
         <v>631</v>
       </c>
-      <c r="M29" s="157" t="s">
+      <c r="M29" s="155" t="s">
         <v>770</v>
       </c>
       <c r="N29" t="str">
@@ -7322,10 +7445,10 @@
       <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="146" t="s">
+      <c r="D30" s="144" t="s">
         <v>794</v>
       </c>
-      <c r="E30" s="153" t="s">
+      <c r="E30" s="151" t="s">
         <v>827</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7346,7 +7469,7 @@
       <c r="L30" s="16" t="s">
         <v>626</v>
       </c>
-      <c r="M30" s="157" t="s">
+      <c r="M30" s="155" t="s">
         <v>771</v>
       </c>
       <c r="N30" t="str">
@@ -7361,10 +7484,10 @@
       <c r="B31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="146" t="s">
+      <c r="D31" s="144" t="s">
         <v>795</v>
       </c>
-      <c r="E31" s="153" t="s">
+      <c r="E31" s="151" t="s">
         <v>828</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -7385,7 +7508,7 @@
       <c r="L31" s="16" t="s">
         <v>630</v>
       </c>
-      <c r="M31" s="157" t="s">
+      <c r="M31" s="155" t="s">
         <v>772</v>
       </c>
       <c r="N31" t="str">
@@ -7400,10 +7523,10 @@
       <c r="B32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="146" t="s">
+      <c r="D32" s="144" t="s">
         <v>796</v>
       </c>
-      <c r="E32" s="153" t="s">
+      <c r="E32" s="151" t="s">
         <v>829</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -7424,7 +7547,7 @@
       <c r="L32" s="16" t="s">
         <v>629</v>
       </c>
-      <c r="M32" s="157" t="s">
+      <c r="M32" s="155" t="s">
         <v>773</v>
       </c>
       <c r="N32" t="str">
@@ -7433,10 +7556,10 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="146" t="s">
+      <c r="D33" s="144" t="s">
         <v>797</v>
       </c>
-      <c r="E33" s="153" t="s">
+      <c r="E33" s="151" t="s">
         <v>829</v>
       </c>
       <c r="H33" s="2">
@@ -7448,7 +7571,7 @@
       <c r="L33" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="M33" s="157" t="s">
+      <c r="M33" s="155" t="s">
         <v>774</v>
       </c>
       <c r="N33" t="str">
@@ -7463,10 +7586,10 @@
       <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="146" t="s">
+      <c r="D34" s="144" t="s">
         <v>799</v>
       </c>
-      <c r="E34" s="153" t="s">
+      <c r="E34" s="151" t="s">
         <v>798</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -7487,7 +7610,7 @@
       <c r="L34" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="M34" s="158" t="s">
+      <c r="M34" s="156" t="s">
         <v>775</v>
       </c>
       <c r="N34" t="str">
@@ -8181,829 +8304,1046 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="39" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="8"/>
+    <col min="2" max="3" width="52.85546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="44.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="39" style="11" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>387</v>
       </c>
-      <c r="I1"/>
-    </row>
-    <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="106" t="s">
         <v>542</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="106"/>
+      <c r="D2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:12" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
       <c r="B3" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="32"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:12" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="16" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="16" t="s">
+        <v>830</v>
+      </c>
+      <c r="L5" t="str">
+        <f>CONCATENATE("|[",B5,"](",C5,")|[Solution](",J5,")|")</f>
+        <v>|[Duplicate Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/duplicate-brackets-official/ojquestion)|[Solution](CP/Duplicatebracket.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="K6" s="16" t="s">
+        <v>831</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L21" si="0">CONCATENATE("|[",B6,"](",C6,")|[Solution](",J6,")|")</f>
+        <v>|[Balanced Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/balanced-brackets-official/ojquestion)|[Solution](CP/BalancedBracket.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="K7" s="16" t="s">
+        <v>832</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Next Greater Element to right](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/next-greater-element-official/ojquestion)|[Solution](CP/NGETR.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
       <c r="B8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="C8" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="K8" s="16" t="s">
+        <v>833</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Stock span](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stock-span-official/ojquestion)|[Solution](CP/StockSpan.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
       <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="C9" s="12" t="s">
+        <v>858</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="16" t="s">
+        <v>834</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Largest Are Histogram](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/lah-official/ojquestion)|[Solution](CP/LargestAreaHistogram.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>6</v>
       </c>
       <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58">
-        <v>5</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="C10" s="12" t="s">
+        <v>859</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58">
+        <v>5</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="K10" s="16" t="s">
+        <v>835</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Sliding Window Maximam](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/sliding-window=maximum-official/ojquestion)|[Solution](CP/SlidingWindowMax.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
       <c r="B11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11" s="12" t="s">
+        <v>860</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
         <v>3</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="16" t="s">
+        <v>836</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Infix evaluation](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-evaluation-official/ojquestion)|[Solution](CP/InfixEvaluation.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="C12" s="12" t="s">
+        <v>861</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>837</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>|[infix conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-conversions-official/ojquestion)|[Solution](CP/InfixConversion.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="C13" s="12" t="s">
+        <v>862</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="16" t="s">
+        <v>838</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Postfix evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/postfix-evaluation-conversions-official/ojquestion)|[Solution](CP/PostFixEvaluationConversion.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>10</v>
       </c>
       <c r="B14" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58">
+      <c r="C14" s="12" t="s">
+        <v>863</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="57"/>
+      <c r="F14" s="58">
         <v>3</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="K14" s="16" t="s">
+        <v>839</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Prefix Evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/prefix-official/ojquestion)|[Solution](CP/PrefixEvaluationConversion.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
       <c r="B15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="C15" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
         <v>3</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="I15" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="J15" s="16" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="K15" s="16" t="s">
+        <v>840</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Celebrity Problem](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/celebrity-problem-official/ojquestion)|[Solution](CP/CelebrityProblem.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
       <c r="B16" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="C16" s="12" t="s">
+        <v>865</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
         <v>3</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="J16" s="16" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>841</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Merge Overlapping interval](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/merge-overlapping-interval-official/ojquestion)|[Solution](CP/Merge_Overlapping_Interval.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
       <c r="B17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="C17" s="12" t="s">
+        <v>866</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="J17" s="16" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="16" t="s">
+        <v>842</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Smallest Number Following pattern](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/smallest-number-following-pattern-official/ojquestion)|[Solution](CP/Smallest_Number_Following_Pattern.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="C18" s="12" t="s">
+        <v>867</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
         <v>3</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="J18" s="16" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Normal stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-stack-official/ojquestion)|[Solution](CP/NormalStack.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="C19" s="12" t="s">
+        <v>868</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
         <v>3</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="J19" s="16" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K19" s="16" t="s">
+        <v>844</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Dynamic stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-stack-official/ojquestion)|[Solution](CP/DynamicStack.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="C20" s="12" t="s">
+        <v>869</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
         <v>3</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="16" t="s">
+        <v>845</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Minimum Stack  -1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/minimum-stack-i-official/ojquestion)|[Solution](CP/MinimumStack.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>17</v>
       </c>
       <c r="B21" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55">
+      <c r="C21" s="12" t="s">
+        <v>870</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55">
         <v>3</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="J21" s="16" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="16" t="s">
+        <v>846</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Minimum Stack  - constant space](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/min-stack-ii-official/ojquestion)|[Solution](CP/MinimumStackConstantSpace.java at main · spartan4cs/CP (github.com))|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C28" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
-    </row>
-    <row r="33" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="18"/>
+    </row>
+    <row r="33" spans="1:10" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="32"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="35"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>1</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="E34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="2">
         <v>0</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J34" s="31"/>
+    </row>
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="31"/>
+      <c r="D35" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="E35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="H35" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="31"/>
+    </row>
+    <row r="36" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>3</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="31"/>
       <c r="D36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="2">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="2">
         <v>0</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="I36" s="31"/>
-    </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J36" s="31"/>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>4</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="31"/>
+      <c r="D37" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="E37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="H37" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="H37" s="47"/>
-      <c r="I37" s="31"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="47"/>
+      <c r="J37" s="31"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>5</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="31"/>
+      <c r="D38" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="2">
+      <c r="E38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="2">
         <v>0</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="H38" s="47"/>
-      <c r="I38" s="31"/>
-    </row>
-    <row r="39" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="47"/>
+      <c r="J38" s="31"/>
+    </row>
+    <row r="39" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>6</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="31"/>
+      <c r="D39" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="E39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="2">
         <v>0</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="G39" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="H39" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="I39" s="31"/>
-    </row>
-    <row r="40" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="31"/>
+    </row>
+    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>7</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="21"/>
+      <c r="D40" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="2">
+      <c r="E40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="G40" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="I40" s="31"/>
-    </row>
-    <row r="41" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="J40" s="31"/>
+    </row>
+    <row r="41" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>8</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="2">
+      <c r="E41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="2">
         <v>0</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="G41" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="H41" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J41" s="31"/>
+    </row>
+    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>9</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="E42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="2">
         <v>0</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="H42" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="I42" s="31"/>
-    </row>
-    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J42" s="31"/>
+    </row>
+    <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>10</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="21"/>
+      <c r="D43" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="2">
+      <c r="E43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="2">
         <v>0</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="H43" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="I43" s="31"/>
-    </row>
-    <row r="44" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="31"/>
+    </row>
+    <row r="44" spans="1:10" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>11</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="21"/>
+      <c r="D44" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="2">
+      <c r="E44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="2">
         <v>0</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="G44" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="H44" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="I44" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="I44" s="31"/>
-    </row>
-    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="J44" s="31"/>
+    </row>
+    <row r="45" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>12</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="21"/>
+      <c r="D45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="E45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="2">
         <v>0</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="G45" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="H45" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="H45" s="25" t="s">
+      <c r="I45" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="I45" s="21"/>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>13</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C46" s="16"/>
       <c r="D46" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="2">
+        <v>5</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="2">
         <v>0</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="G46" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="H46" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="I46" s="16"/>
-    </row>
-    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J46" s="16"/>
+    </row>
+    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>14</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="C47" s="16"/>
+      <c r="I47" s="10" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="16"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="16"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="16"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>558</v>
       </c>
+      <c r="C51" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
     <hyperlink ref="B34" r:id="rId2" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
     <hyperlink ref="B35" r:id="rId3" display="https://leetcode.com/problems/next-greater-element-ii/" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
     <hyperlink ref="B36" r:id="rId4" display="https://leetcode.com/problems/next-greater-element-i/" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
@@ -9018,304 +9358,372 @@
     <hyperlink ref="B45" r:id="rId13" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string-ii/" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
     <hyperlink ref="B46" r:id="rId14" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
     <hyperlink ref="B47" r:id="rId15" display="https://leetcode.com/problems/maximum-frequency-stack/" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="H20" r:id="rId16" display="https://leetcode.com/problems/min-stack/" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="I20" r:id="rId16" display="https://leetcode.com/problems/min-stack/" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
     <hyperlink ref="B48" r:id="rId17" display="https://leetcode.com/problems/trapping-rain-water/" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
     <hyperlink ref="B49" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
-    <hyperlink ref="G1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
-    <hyperlink ref="I5" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="I8" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="I9" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="I10" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="I6" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="I15" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="I16" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
-    <hyperlink ref="I13" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
-    <hyperlink ref="I14" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
-    <hyperlink ref="I11" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
-    <hyperlink ref="I12" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
-    <hyperlink ref="I17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
-    <hyperlink ref="I18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
-    <hyperlink ref="I19" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
-    <hyperlink ref="I20" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
-    <hyperlink ref="I21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="H1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="J5" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="J8" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="J9" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="J10" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="J6" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="J15" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="J16" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="J13" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="J14" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="J11" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="J12" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="J17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="J18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="J19" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="J20" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="J21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
     <hyperlink ref="B50" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
-    <hyperlink ref="I7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="J7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
     <hyperlink ref="B51" r:id="rId38" display="https://leetcode.com/problems/validate-stack-sequences/" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
+    <hyperlink ref="K5" r:id="rId39" xr:uid="{C5DA77CE-BF5F-471B-BD15-FD12434C8866}"/>
+    <hyperlink ref="K8" r:id="rId40" xr:uid="{88688B35-7028-4B07-AF64-DEB6121F2E50}"/>
+    <hyperlink ref="K9" r:id="rId41" xr:uid="{A2887BC4-2D33-48D0-91CA-2E9DC8873CEE}"/>
+    <hyperlink ref="K10" r:id="rId42" xr:uid="{C08C34BC-FDC8-46A2-B8E4-12118592AFCC}"/>
+    <hyperlink ref="K6" r:id="rId43" xr:uid="{2784DED9-6DAC-439F-AC5B-7D178ADF003E}"/>
+    <hyperlink ref="K15" r:id="rId44" xr:uid="{8FE340F2-6D35-4CCD-9306-219A0FA38768}"/>
+    <hyperlink ref="K16" r:id="rId45" xr:uid="{C4D28745-BBE5-4EEC-9746-1D859885A2E9}"/>
+    <hyperlink ref="K13" r:id="rId46" xr:uid="{7673294E-2743-4364-AD88-1A125513F98E}"/>
+    <hyperlink ref="K14" r:id="rId47" xr:uid="{41B8ED56-0876-4334-8AED-9B99785ED675}"/>
+    <hyperlink ref="K11" r:id="rId48" xr:uid="{AD064460-E725-4427-B16B-FABF21A77A63}"/>
+    <hyperlink ref="K12" r:id="rId49" xr:uid="{9097970C-F4C5-4F23-935C-F05DB88649DB}"/>
+    <hyperlink ref="K17" r:id="rId50" xr:uid="{8E8AB80B-7564-416A-B3B8-FBB5AAE26F78}"/>
+    <hyperlink ref="K18" r:id="rId51" xr:uid="{0E84154A-F5F4-403B-BA6C-2DF598AAAD28}"/>
+    <hyperlink ref="K19" r:id="rId52" xr:uid="{56C77BA2-89C4-445B-8A50-B9B58F0CEE02}"/>
+    <hyperlink ref="K20" r:id="rId53" xr:uid="{824CF2BD-1F69-4277-AB6B-F7D76F558D39}"/>
+    <hyperlink ref="K21" r:id="rId54" xr:uid="{1D2D55A4-C68D-4891-921E-8C87B27471FA}"/>
+    <hyperlink ref="K7" r:id="rId55" xr:uid="{D3DEBC72-F3AE-44FB-BAB9-3A0044AB73EC}"/>
+    <hyperlink ref="C5" r:id="rId56" xr:uid="{874E0623-8FFB-4179-BA39-AF74487F60A1}"/>
+    <hyperlink ref="C6" r:id="rId57" xr:uid="{AA94A7F2-7E66-4F17-8786-21965F4A0C77}"/>
+    <hyperlink ref="C7" r:id="rId58" xr:uid="{BB8C6D39-CA91-41FF-8799-2E439F8AEEA2}"/>
+    <hyperlink ref="C8" r:id="rId59" xr:uid="{D4098828-B819-438E-AA1D-53B157AB3918}"/>
+    <hyperlink ref="C9" r:id="rId60" xr:uid="{2C880774-255A-4D47-86CB-6CA5F4C81333}"/>
+    <hyperlink ref="C10" r:id="rId61" xr:uid="{78B238FE-92AF-4EB6-8304-111489859ADD}"/>
+    <hyperlink ref="C11" r:id="rId62" xr:uid="{FAB35DEE-9D13-46C5-BA95-82E6172923D5}"/>
+    <hyperlink ref="C12" r:id="rId63" xr:uid="{42920AE1-703A-4C58-8EC1-9772E52D21B3}"/>
+    <hyperlink ref="C13" r:id="rId64" xr:uid="{A1A26E47-EAB3-4E04-B174-47496607FFF4}"/>
+    <hyperlink ref="C14" r:id="rId65" xr:uid="{056B63C3-D159-4F75-A944-FC9F661E399B}"/>
+    <hyperlink ref="C15" r:id="rId66" xr:uid="{86F53A88-369F-4D35-94CC-51E65189C39E}"/>
+    <hyperlink ref="C16" r:id="rId67" xr:uid="{2A22302A-6F88-4A90-8160-07ED92C4CEA2}"/>
+    <hyperlink ref="C17" r:id="rId68" xr:uid="{104539CA-065F-4863-95B4-D19FC109B4E9}"/>
+    <hyperlink ref="C18" r:id="rId69" xr:uid="{C624F35C-C88A-42EA-8048-B15545102627}"/>
+    <hyperlink ref="C19" r:id="rId70" xr:uid="{AE3D143E-5AC7-4BF5-9353-22217A91A1DA}"/>
+    <hyperlink ref="C20" r:id="rId71" xr:uid="{52B49247-3BFE-4087-A275-D517E72935CE}"/>
+    <hyperlink ref="C21" r:id="rId72" xr:uid="{71E90A70-1B5E-40F0-80BC-2081B9FE995F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId39"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="42" customWidth="1"/>
-    <col min="7" max="7" width="49.42578125" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" customWidth="1"/>
-    <col min="9" max="9" width="39.7109375" customWidth="1"/>
+    <col min="2" max="3" width="46.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" customWidth="1"/>
+    <col min="10" max="10" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="142" t="s">
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="158" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="I2" s="61"/>
-    </row>
-    <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="J2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="E3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="F3" s="59" t="s">
         <v>455</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="64" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2">
+      <c r="C4" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="16" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="12" t="s">
+        <v>848</v>
+      </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="10"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="16" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2">
+      <c r="C6" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="16" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2">
+      <c r="C7" s="12" t="s">
+        <v>850</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="16" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="16" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2">
+      <c r="C8" s="12" t="s">
+        <v>851</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="16" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="16" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2">
+      <c r="C9" s="12" t="s">
+        <v>852</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="16" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="16" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2">
+      <c r="C10" s="12" t="s">
+        <v>853</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="65" t="s">
         <v>412</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="11"/>
+      <c r="J10" s="16" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="62" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="62" t="s">
         <v>375</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>414</v>
       </c>
+      <c r="C15" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://auth.geeksforgeeks.org/?to=https%3A%2F%2Fpractice.geeksforgeeks.org%2Fproblems%2Fgenerate-binary-numbers-1587115620%2F1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="C1" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="I4" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="I6" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="I8" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="G10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="D1" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="J5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="J4" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="J11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="J6" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="J10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="J9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="J8" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="H10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
     <hyperlink ref="B14" r:id="rId12" display="https://www.geeksforgeeks.org/kth-smallestlargest-element-unsorted-array/" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
     <hyperlink ref="B15" r:id="rId13" display="https://practice.geeksforgeeks.org/problems/minimize-the-heights3351/1" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="C4" r:id="rId14" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion" xr:uid="{580FDDDC-9D3D-412C-A5EB-BCC7C6A67C5F}"/>
+    <hyperlink ref="C5" r:id="rId15" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion" xr:uid="{8FD8EAB7-49A4-4493-A4B3-095A76C47BFE}"/>
+    <hyperlink ref="C6" r:id="rId16" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-push-efficient-official/ojquestion" xr:uid="{E419515B-FDD7-4D25-84A6-1896C7EA4868}"/>
+    <hyperlink ref="C7" r:id="rId17" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-pop-efficient/ojquestion" xr:uid="{D62EF7CF-5E2E-431E-949C-D9C168D794C9}"/>
+    <hyperlink ref="C8" r:id="rId18" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-add-efficient-official/ojquestion" xr:uid="{11F21342-3293-4284-9968-7156404D1806}"/>
+    <hyperlink ref="C9" r:id="rId19" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-remove-efficient-official/ojquestion" xr:uid="{A4D6BBC3-0800-460D-A724-A5ECB367332B}"/>
+    <hyperlink ref="C10" r:id="rId20" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/two-stacks-official/ojquestion" xr:uid="{A7E9C8E1-2442-431D-8938-F2CFEF3D2718}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 18:15:48.32
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D705B0-57D0-452F-9232-F61B5FD1D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF341B3-5911-405A-91BC-65020DCFE591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="879">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3120,27 +3120,6 @@
     <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java</t>
   </si>
   <si>
-    <t> Normal Queue Easy</t>
-  </si>
-  <si>
-    <t> Dynamic Queue Easy</t>
-  </si>
-  <si>
-    <t> Queue To Stack Adapter - Push Efficient Easy</t>
-  </si>
-  <si>
-    <t> Queue To Stack Adapter - Pop Efficient Easy</t>
-  </si>
-  <si>
-    <t> Stack To Queue Adapter - Add Efficient Easy</t>
-  </si>
-  <si>
-    <t> Stack To Queue Adapter - Remove Efficient Easy</t>
-  </si>
-  <si>
-    <t> Two Stacks In An Array</t>
-  </si>
-  <si>
     <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/duplicate-brackets-official/ojquestion</t>
   </si>
   <si>
@@ -3190,6 +3169,51 @@
   </si>
   <si>
     <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/min-stack-ii-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-push-efficient-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-pop-efficient/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-add-efficient-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-remove-efficient-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/two-stacks-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java</t>
   </si>
 </sst>
 </file>
@@ -3707,7 +3731,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4121,6 +4145,14 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Accent1" xfId="9" builtinId="30"/>
@@ -8306,14 +8338,15 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="5" customWidth="1"/>
-    <col min="2" max="3" width="52.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
@@ -8342,7 +8375,7 @@
       <c r="B2" s="106" t="s">
         <v>542</v>
       </c>
-      <c r="C2" s="106"/>
+      <c r="C2" s="159"/>
       <c r="D2" s="16"/>
       <c r="H2" s="16"/>
       <c r="J2"/>
@@ -8352,7 +8385,7 @@
       <c r="B3" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="160"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="34"/>
@@ -8368,7 +8401,7 @@
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -8398,8 +8431,8 @@
       <c r="B5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>854</v>
+      <c r="C5" s="31" t="s">
+        <v>847</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
@@ -8420,8 +8453,8 @@
         <v>830</v>
       </c>
       <c r="L5" t="str">
-        <f>CONCATENATE("|[",B5,"](",C5,")|[Solution](",J5,")|")</f>
-        <v>|[Duplicate Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/duplicate-brackets-official/ojquestion)|[Solution](CP/Duplicatebracket.java at main · spartan4cs/CP (github.com))|</v>
+        <f>CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
+        <v>|[Duplicate Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/duplicate-brackets-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java)|</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -8431,8 +8464,8 @@
       <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>855</v>
+      <c r="C6" s="31" t="s">
+        <v>848</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -8453,8 +8486,8 @@
         <v>831</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" ref="L6:L21" si="0">CONCATENATE("|[",B6,"](",C6,")|[Solution](",J6,")|")</f>
-        <v>|[Balanced Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/balanced-brackets-official/ojquestion)|[Solution](CP/BalancedBracket.java at main · spartan4cs/CP (github.com))|</v>
+        <f t="shared" ref="L6:L21" si="0">CONCATENATE("|[",B6,"](",C6,")|[Solution](",K6,")|")</f>
+        <v>|[Balanced Bracket](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/balanced-brackets-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java)|</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
@@ -8464,8 +8497,8 @@
       <c r="B7" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>856</v>
+      <c r="C7" s="31" t="s">
+        <v>849</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -8487,7 +8520,7 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>|[Next Greater Element to right](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/next-greater-element-official/ojquestion)|[Solution](CP/NGETR.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Next Greater Element to right](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/next-greater-element-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java)|</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
@@ -8497,8 +8530,8 @@
       <c r="B8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>857</v>
+      <c r="C8" s="31" t="s">
+        <v>850</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -8520,7 +8553,7 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>|[Stock span](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stock-span-official/ojquestion)|[Solution](CP/StockSpan.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Stock span](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stock-span-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java)|</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -8530,8 +8563,8 @@
       <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>858</v>
+      <c r="C9" s="31" t="s">
+        <v>851</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -8550,7 +8583,7 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>|[Largest Are Histogram](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/lah-official/ojquestion)|[Solution](CP/LargestAreaHistogram.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Largest Are Histogram](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/lah-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java)|</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8560,8 +8593,8 @@
       <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>859</v>
+      <c r="C10" s="31" t="s">
+        <v>852</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>5</v>
@@ -8581,7 +8614,7 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>|[Sliding Window Maximam](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/sliding-window=maximum-official/ojquestion)|[Solution](CP/SlidingWindowMax.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Sliding Window Maximam](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/sliding-window=maximum-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java)|</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -8591,8 +8624,8 @@
       <c r="B11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>860</v>
+      <c r="C11" s="31" t="s">
+        <v>853</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
@@ -8617,7 +8650,7 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>|[Infix evaluation](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-evaluation-official/ojquestion)|[Solution](CP/InfixEvaluation.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Infix evaluation](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-evaluation-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java)|</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -8627,8 +8660,8 @@
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>861</v>
+      <c r="C12" s="31" t="s">
+        <v>854</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -8650,7 +8683,7 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>|[infix conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-conversions-official/ojquestion)|[Solution](CP/InfixConversion.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[infix conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/infix-conversions-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java)|</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8660,8 +8693,8 @@
       <c r="B13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>862</v>
+      <c r="C13" s="31" t="s">
+        <v>855</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -8683,7 +8716,7 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>|[Postfix evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/postfix-evaluation-conversions-official/ojquestion)|[Solution](CP/PostFixEvaluationConversion.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Postfix evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/postfix-evaluation-conversions-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java)|</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8693,8 +8726,8 @@
       <c r="B14" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>863</v>
+      <c r="C14" s="31" t="s">
+        <v>856</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>5</v>
@@ -8717,7 +8750,7 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>|[Prefix Evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/prefix-official/ojquestion)|[Solution](CP/PrefixEvaluationConversion.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Prefix Evaluation and conversion](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/prefix-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java)|</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -8727,8 +8760,8 @@
       <c r="B15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>864</v>
+      <c r="C15" s="31" t="s">
+        <v>857</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -8750,7 +8783,7 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>|[Celebrity Problem](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/celebrity-problem-official/ojquestion)|[Solution](CP/CelebrityProblem.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Celebrity Problem](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/celebrity-problem-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java)|</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -8760,8 +8793,8 @@
       <c r="B16" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>865</v>
+      <c r="C16" s="31" t="s">
+        <v>858</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -8780,18 +8813,18 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>|[Merge Overlapping interval](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/merge-overlapping-interval-official/ojquestion)|[Solution](CP/Merge_Overlapping_Interval.java at main · spartan4cs/CP (github.com))|</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>|[Merge Overlapping interval](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/merge-overlapping-interval-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java)|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
       <c r="B17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>866</v>
+      <c r="C17" s="31" t="s">
+        <v>859</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
@@ -8810,7 +8843,7 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>|[Smallest Number Following pattern](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/smallest-number-following-pattern-official/ojquestion)|[Solution](CP/Smallest_Number_Following_Pattern.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Smallest Number Following pattern](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/smallest-number-following-pattern-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java)|</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8820,8 +8853,8 @@
       <c r="B18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>867</v>
+      <c r="C18" s="31" t="s">
+        <v>860</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -8840,18 +8873,18 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>|[Normal stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-stack-official/ojquestion)|[Solution](CP/NormalStack.java at main · spartan4cs/CP (github.com))|</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>|[Normal stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-stack-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java)|</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>868</v>
+      <c r="C19" s="31" t="s">
+        <v>861</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
@@ -8867,18 +8900,18 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>|[Dynamic stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-stack-official/ojquestion)|[Solution](CP/DynamicStack.java at main · spartan4cs/CP (github.com))|</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>|[Dynamic stack ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-stack-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java)|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>869</v>
+      <c r="C20" s="31" t="s">
+        <v>862</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
@@ -8903,18 +8936,18 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>|[Minimum Stack  -1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/minimum-stack-i-official/ojquestion)|[Solution](CP/MinimumStack.java at main · spartan4cs/CP (github.com))|</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>|[Minimum Stack  -1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/minimum-stack-i-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java)|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>17</v>
       </c>
       <c r="B21" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>870</v>
+      <c r="C21" s="31" t="s">
+        <v>863</v>
       </c>
       <c r="D21" s="53" t="s">
         <v>5</v>
@@ -8934,48 +8967,48 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
-        <v>|[Minimum Stack  - constant space](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/min-stack-ii-official/ojquestion)|[Solution](CP/MinimumStackConstantSpace.java at main · spartan4cs/CP (github.com))|</v>
+        <v>|[Minimum Stack  - constant space](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/min-stack-ii-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java)|</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="12"/>
+      <c r="C22" s="31"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="12"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="12"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="12"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="12"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="12"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="12"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
+      <c r="C30" s="161"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
+      <c r="C31" s="161"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
+      <c r="C32" s="161"/>
     </row>
     <row r="33" spans="1:10" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C33" s="38"/>
+      <c r="C33" s="160"/>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="34"/>
@@ -9287,7 +9320,7 @@
       <c r="B46" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="162"/>
       <c r="D46" s="5" t="s">
         <v>5</v>
       </c>
@@ -9312,7 +9345,7 @@
       <c r="B47" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="162"/>
       <c r="I47" s="10" t="s">
         <v>363</v>
       </c>
@@ -9321,25 +9354,25 @@
       <c r="B48" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="162"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="162"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="C50" s="16"/>
+      <c r="C50" s="162"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="C51" s="16"/>
+      <c r="C51" s="162"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9424,10 +9457,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9440,7 +9473,7 @@
     <col min="10" max="10" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>87</v>
       </c>
@@ -9450,7 +9483,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:12" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="158" t="s">
         <v>315</v>
       </c>
@@ -9463,7 +9496,7 @@
       <c r="H2" s="158"/>
       <c r="J2" s="61"/>
     </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
@@ -9493,7 +9526,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -9501,7 +9534,7 @@
         <v>379</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>847</v>
+        <v>864</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -9518,8 +9551,15 @@
       <c r="J4" s="16" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="16" t="s">
+        <v>871</v>
+      </c>
+      <c r="L4" t="str">
+        <f>CONCATENATE("|[",B4,"](",C4,")|[Solution](",K4,")|")</f>
+        <v>|[Normal queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java)|</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -9527,7 +9567,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>848</v>
+        <v>865</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -9538,8 +9578,15 @@
       <c r="J5" s="16" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="16" t="s">
+        <v>872</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" ref="L5:L11" si="0">CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
+        <v>|[Dynamic Queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java)|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -9547,7 +9594,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>849</v>
+        <v>866</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -9562,8 +9609,15 @@
       <c r="J6" s="16" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="16" t="s">
+        <v>873</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Queue to Stack Adapter- push efficient ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-push-efficient-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java)|</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -9571,7 +9625,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>850</v>
+        <v>867</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -9586,8 +9640,15 @@
       <c r="J7" s="16" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="16" t="s">
+        <v>874</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Queue to Stack Adapter- pop efficient ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-pop-efficient/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java)|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -9595,7 +9656,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>851</v>
+        <v>868</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -9610,8 +9671,15 @@
       <c r="J8" s="16" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="16" t="s">
+        <v>875</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Stack to Queue Adapter-Add efficient](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-add-efficient-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java)|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -9619,7 +9687,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>852</v>
+        <v>869</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -9634,8 +9702,15 @@
       <c r="J9" s="16" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="16" t="s">
+        <v>876</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Stack to Queue Adapter-Remove efficient](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-remove-efficient-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java)|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -9643,7 +9718,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>853</v>
+        <v>870</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
@@ -9660,8 +9735,15 @@
       <c r="J10" s="16" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="16" t="s">
+        <v>877</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Two Stacks in an Array ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/two-stacks-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java)|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -9686,14 +9768,21 @@
       <c r="J11" s="16" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="16" t="s">
+        <v>878</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Generate Binary Numbers ]()|[Solution](https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java)|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>413</v>
       </c>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>414</v>
       </c>
@@ -9717,13 +9806,21 @@
     <hyperlink ref="H10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
     <hyperlink ref="B14" r:id="rId12" display="https://www.geeksforgeeks.org/kth-smallestlargest-element-unsorted-array/" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
     <hyperlink ref="B15" r:id="rId13" display="https://practice.geeksforgeeks.org/problems/minimize-the-heights3351/1" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="C4" r:id="rId14" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion" xr:uid="{580FDDDC-9D3D-412C-A5EB-BCC7C6A67C5F}"/>
-    <hyperlink ref="C5" r:id="rId15" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion" xr:uid="{8FD8EAB7-49A4-4493-A4B3-095A76C47BFE}"/>
-    <hyperlink ref="C6" r:id="rId16" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-push-efficient-official/ojquestion" xr:uid="{E419515B-FDD7-4D25-84A6-1896C7EA4868}"/>
-    <hyperlink ref="C7" r:id="rId17" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-pop-efficient/ojquestion" xr:uid="{D62EF7CF-5E2E-431E-949C-D9C168D794C9}"/>
-    <hyperlink ref="C8" r:id="rId18" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-add-efficient-official/ojquestion" xr:uid="{11F21342-3293-4284-9968-7156404D1806}"/>
-    <hyperlink ref="C9" r:id="rId19" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-remove-efficient-official/ojquestion" xr:uid="{A4D6BBC3-0800-460D-A724-A5ECB367332B}"/>
-    <hyperlink ref="C10" r:id="rId20" display="https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/two-stacks-official/ojquestion" xr:uid="{A7E9C8E1-2442-431D-8938-F2CFEF3D2718}"/>
+    <hyperlink ref="C4" r:id="rId14" xr:uid="{580FDDDC-9D3D-412C-A5EB-BCC7C6A67C5F}"/>
+    <hyperlink ref="C5" r:id="rId15" xr:uid="{8FD8EAB7-49A4-4493-A4B3-095A76C47BFE}"/>
+    <hyperlink ref="C6" r:id="rId16" xr:uid="{E419515B-FDD7-4D25-84A6-1896C7EA4868}"/>
+    <hyperlink ref="C7" r:id="rId17" xr:uid="{D62EF7CF-5E2E-431E-949C-D9C168D794C9}"/>
+    <hyperlink ref="C8" r:id="rId18" xr:uid="{11F21342-3293-4284-9968-7156404D1806}"/>
+    <hyperlink ref="C9" r:id="rId19" xr:uid="{A4D6BBC3-0800-460D-A724-A5ECB367332B}"/>
+    <hyperlink ref="C10" r:id="rId20" xr:uid="{A7E9C8E1-2442-431D-8938-F2CFEF3D2718}"/>
+    <hyperlink ref="K5" r:id="rId21" xr:uid="{071BA520-9648-4DD0-AE0E-A750D6B2F8EC}"/>
+    <hyperlink ref="K4" r:id="rId22" xr:uid="{712248B5-69CF-41F3-9618-13846E4396FD}"/>
+    <hyperlink ref="K11" r:id="rId23" xr:uid="{4B1E7EB2-C820-4222-BA27-73040EDF7600}"/>
+    <hyperlink ref="K7" r:id="rId24" xr:uid="{FC2A0DA3-AF65-451C-B29C-330A4B8CF2E3}"/>
+    <hyperlink ref="K6" r:id="rId25" xr:uid="{5C7E613E-04CB-4A03-9E1B-6532697710FC}"/>
+    <hyperlink ref="K10" r:id="rId26" xr:uid="{EDC3D542-AF08-4D54-858F-A4D5F6BF7EF9}"/>
+    <hyperlink ref="K9" r:id="rId27" xr:uid="{1D1441BA-B450-4337-BDEC-391B92DC621E}"/>
+    <hyperlink ref="K8" r:id="rId28" xr:uid="{8CEA5E56-E83A-480F-A33F-3C5ED550F365}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 19:01:39.44
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF341B3-5911-405A-91BC-65020DCFE591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7F42D5-0AE0-4770-9549-A4E03BAE05F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="924">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3214,6 +3214,141 @@
   </si>
   <si>
     <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-last-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-first-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/get-in-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-first-in-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-at-index-in-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-last-in-linked-list/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-at-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-di-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-pi-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linkedlist-to-stack-adapter-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linked-list-to-queue-adapter-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kth-from-last-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mid-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/merge-two-sorted-linked-lists-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mergesort-linkedlist-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-duplicates-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/odd-even-linked-list-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kreverse-linkedlist-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-reverse-linkedlist-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-linkedlist-pr-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/is-linkedlist-palindromic-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/fold-linkedlist-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-two-linkedlists-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/intersection-of-linked-lists-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/copy-linkedlist-with-random-pointers/ojquestion</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java</t>
   </si>
 </sst>
 </file>
@@ -9459,8 +9594,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L11"/>
+    <sheetView topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10441,18 +10576,17 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="4" width="51.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="56" customWidth="1"/>
@@ -10461,59 +10595,63 @@
     <col min="11" max="11" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="87" t="s">
+      <c r="C1" s="87" t="s">
         <v>511</v>
       </c>
+      <c r="D1" s="87"/>
       <c r="E1" s="5">
         <v>0</v>
       </c>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="88" t="s">
+      <c r="C2" s="88" t="s">
         <v>512</v>
       </c>
+      <c r="D2" s="88"/>
       <c r="E2" s="88" t="s">
         <v>513</v>
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="87"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4"/>
+      <c r="C4" s="87"/>
       <c r="D4" s="87"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="87"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6"/>
+      <c r="C6" s="87"/>
       <c r="D6" s="87"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
+      <c r="D7" s="24"/>
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
@@ -10536,17 +10674,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="16" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="C9" s="81" t="s">
         <v>209</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>879</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -10557,13 +10698,23 @@
       <c r="K9" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M9" t="str">
+        <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",L9,")|")</f>
+        <v>|[ Add Last In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-last-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>2</v>
       </c>
-      <c r="D10" s="82" t="s">
+      <c r="C10" s="82" t="s">
         <v>210</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>880</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -10574,13 +10725,23 @@
       <c r="K10" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ref="M10:M34" si="0">CONCATENATE("|[",C10,"](",D10,")|[Solution](",L10,")|")</f>
+        <v>|[ Display A Linkedlist ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="C11" s="82" t="s">
         <v>211</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>881</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -10591,13 +10752,23 @@
       <c r="K11" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Remove First In Linkedlist ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-first-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="C12" s="82" t="s">
         <v>212</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>882</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -10608,13 +10779,23 @@
       <c r="K12" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Get Value In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/get-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="82" t="s">
+      <c r="C13" s="82" t="s">
         <v>213</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>883</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -10625,13 +10806,23 @@
       <c r="K13" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Add First In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-first-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="C14" s="82" t="s">
         <v>214</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>884</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -10642,13 +10833,23 @@
       <c r="K14" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Add At Index In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-at-index-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="C15" s="82" t="s">
         <v>215</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>885</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -10659,13 +10860,23 @@
       <c r="K15" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Remove Last In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-last-in-linked-list/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="82" t="s">
         <v>216</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>886</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -10676,13 +10887,23 @@
       <c r="K16" s="16" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Remove At Index In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-at-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="C17" s="82" t="s">
         <v>217</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>887</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -10699,13 +10920,23 @@
       <c r="K17" s="16" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="16" t="s">
+        <v>906</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Reverse A Linked List (data Iterative) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-di-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java)|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>10</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="C18" s="83" t="s">
         <v>218</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>888</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -10719,13 +10950,23 @@
       <c r="K18" s="16" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="16" t="s">
+        <v>907</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Reverse Linked List (pointer Iterative) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-pi-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java)|</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="85" t="s">
+      <c r="C19" s="85" t="s">
         <v>219</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>889</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -10739,13 +10980,23 @@
       <c r="K19" s="16" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="16" t="s">
+        <v>908</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Linked List To Stack Adapter ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linkedlist-to-stack-adapter-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java)|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>12</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="C20" s="39" t="s">
         <v>220</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>890</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -10759,13 +11010,23 @@
       <c r="K20" s="16" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="16" t="s">
+        <v>909</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Linked List To Queue Adapter ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linked-list-to-queue-adapter-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java)|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>13</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="C21" s="39" t="s">
         <v>221</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>891</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -10779,13 +11040,23 @@
       <c r="K21" s="16" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="16" t="s">
+        <v>910</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Kth Node From End Of Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kth-from-last-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java)|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>14</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="C22" s="39" t="s">
         <v>222</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>892</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -10799,13 +11070,23 @@
       <c r="K22" s="16" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L22" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Mid Of Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mid-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java)|</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D23" s="85" t="s">
+      <c r="C23" s="85" t="s">
         <v>223</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>893</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -10825,13 +11106,23 @@
       <c r="K23" s="16" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="16" t="s">
+        <v>912</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Merge Two Sorted Linked Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/merge-two-sorted-linked-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java)|</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>16</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="C24" s="39" t="s">
         <v>224</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>894</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -10842,13 +11133,23 @@
       <c r="K24" s="16" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Merge Sort A Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mergesort-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java)|</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>17</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="C25" s="39" t="s">
         <v>225</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>895</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -10862,13 +11163,23 @@
       <c r="K25" s="16" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="16" t="s">
+        <v>914</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Remove Duplicates In A Sorted Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-duplicates-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java)|</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>18</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="C26" s="39" t="s">
         <v>178</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>896</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -10879,13 +11190,23 @@
       <c r="K26" s="16" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="16" t="s">
+        <v>915</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Odd Even Linked List Medium](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/odd-even-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java)|</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>19</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="C27" s="39" t="s">
         <v>226</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>897</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -10896,13 +11217,23 @@
       <c r="K27" s="16" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="16" t="s">
+        <v>916</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ K Reverse In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kreverse-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java)|</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>20</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="C28" s="39" t="s">
         <v>227</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>898</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
@@ -10913,13 +11244,23 @@
       <c r="K28" s="16" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="16" t="s">
+        <v>917</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Display Reverse (recursive) - Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-reverse-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java)|</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="C29" s="105" t="s">
         <v>228</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>899</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -10930,13 +11271,23 @@
       <c r="K29" s="16" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L29" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Reverse Linked List (pointer - Recursive) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-linkedlist-pr-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java)|</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="92" t="s">
+      <c r="C30" s="92" t="s">
         <v>229</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>900</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -10950,13 +11301,23 @@
       <c r="K30" s="16" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="L30" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Is Linked List A Palindrome? ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/is-linkedlist-palindromic-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java)|</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="C31" s="91" t="s">
         <v>230</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>901</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -10976,13 +11337,23 @@
       <c r="K31" s="16" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="L31" s="16" t="s">
+        <v>920</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Fold A Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/fold-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java)|</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="C32" s="91" t="s">
         <v>231</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>902</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -10999,13 +11370,23 @@
       <c r="K32" s="16" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="16" t="s">
+        <v>921</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Add Two Linked Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-two-linkedlists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java)|</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="93" t="s">
+      <c r="C33" s="93" t="s">
         <v>179</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>903</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -11019,16 +11400,26 @@
       <c r="K33" s="16" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L33" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Intersection Point Of Linked Lists](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/intersection-of-linked-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java)|</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>26</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="D34" s="86" t="s">
+      <c r="C34" s="86" t="s">
         <v>505</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>904</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -11042,21 +11433,30 @@
       <c r="K34" s="16" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="16" t="s">
+        <v>923</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="0"/>
+        <v>|[Copy Linkedlist With Random Pointers ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/copy-linkedlist-with-random-pointers/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java)|</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:11" s="76" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="36" spans="1:13" s="76" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A36" s="75"/>
-      <c r="D36" s="77" t="s">
+      <c r="C36" s="77" t="s">
         <v>474</v>
       </c>
+      <c r="D36" s="77"/>
       <c r="G36" s="78"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="16" t="s">
         <v>472</v>
       </c>
+      <c r="D38" s="16"/>
       <c r="F38" t="s">
         <v>6</v>
       </c>
@@ -11064,15 +11464,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="16" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="16" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="16" t="s">
+      <c r="D39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="16" t="s">
         <v>465</v>
       </c>
+      <c r="D40" s="16"/>
       <c r="F40" t="s">
         <v>6</v>
       </c>
@@ -11080,10 +11482,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="16" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="16" t="s">
         <v>473</v>
       </c>
+      <c r="D41" s="16"/>
       <c r="F41" t="s">
         <v>6</v>
       </c>
@@ -11091,10 +11494,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="16" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="16" t="s">
         <v>475</v>
       </c>
+      <c r="D42" s="16"/>
       <c r="F42" t="s">
         <v>6</v>
       </c>
@@ -11102,10 +11506,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="16" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C43" s="16" t="s">
         <v>477</v>
       </c>
+      <c r="D43" s="16"/>
       <c r="F43" t="s">
         <v>6</v>
       </c>
@@ -11117,10 +11522,11 @@
       </c>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="16" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="16" t="s">
         <v>469</v>
       </c>
+      <c r="D44" s="16"/>
       <c r="F44" t="s">
         <v>6</v>
       </c>
@@ -11128,10 +11534,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="16" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="16" t="s">
         <v>478</v>
       </c>
+      <c r="D45" s="16"/>
       <c r="F45" t="s">
         <v>6</v>
       </c>
@@ -11139,10 +11546,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D46" s="16" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C46" s="16" t="s">
         <v>470</v>
       </c>
+      <c r="D46" s="16"/>
       <c r="F46" t="s">
         <v>6</v>
       </c>
@@ -11150,21 +11558,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C47" s="5" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="C47" s="16" t="s">
         <v>471</v>
       </c>
+      <c r="D47" s="16"/>
       <c r="G47" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D48" s="16" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C48" s="16" t="s">
         <v>507</v>
       </c>
+      <c r="D48" s="16"/>
       <c r="F48" t="s">
         <v>6</v>
       </c>
@@ -11172,10 +11582,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="16" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="16" t="s">
         <v>506</v>
       </c>
+      <c r="D49" s="16"/>
       <c r="F49" t="s">
         <v>6</v>
       </c>
@@ -11198,16 +11609,16 @@
     <hyperlink ref="K23" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
     <hyperlink ref="K24" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
     <hyperlink ref="H25" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{00000000-0004-0000-0700-00000C000000}"/>
-    <hyperlink ref="D47" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/" xr:uid="{00000000-0004-0000-0700-00000D000000}"/>
+    <hyperlink ref="C47" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/" xr:uid="{00000000-0004-0000-0700-00000D000000}"/>
     <hyperlink ref="I17" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{00000000-0004-0000-0700-00000E000000}"/>
-    <hyperlink ref="D44" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{00000000-0004-0000-0700-00000F000000}"/>
-    <hyperlink ref="D40" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/" xr:uid="{00000000-0004-0000-0700-000010000000}"/>
-    <hyperlink ref="D38" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{00000000-0004-0000-0700-000011000000}"/>
-    <hyperlink ref="D42" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/" xr:uid="{00000000-0004-0000-0700-000012000000}"/>
-    <hyperlink ref="D43" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/" xr:uid="{00000000-0004-0000-0700-000013000000}"/>
-    <hyperlink ref="D46" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{00000000-0004-0000-0700-000014000000}"/>
-    <hyperlink ref="D41" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/" xr:uid="{00000000-0004-0000-0700-000015000000}"/>
-    <hyperlink ref="D45" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/" xr:uid="{00000000-0004-0000-0700-000016000000}"/>
+    <hyperlink ref="C44" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{00000000-0004-0000-0700-00000F000000}"/>
+    <hyperlink ref="C40" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/" xr:uid="{00000000-0004-0000-0700-000010000000}"/>
+    <hyperlink ref="C38" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{00000000-0004-0000-0700-000011000000}"/>
+    <hyperlink ref="C42" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/" xr:uid="{00000000-0004-0000-0700-000012000000}"/>
+    <hyperlink ref="C43" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/" xr:uid="{00000000-0004-0000-0700-000013000000}"/>
+    <hyperlink ref="C46" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{00000000-0004-0000-0700-000014000000}"/>
+    <hyperlink ref="C41" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/" xr:uid="{00000000-0004-0000-0700-000015000000}"/>
+    <hyperlink ref="C45" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/" xr:uid="{00000000-0004-0000-0700-000016000000}"/>
     <hyperlink ref="H43" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs" xr:uid="{00000000-0004-0000-0700-000017000000}"/>
     <hyperlink ref="K26" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java" xr:uid="{00000000-0004-0000-0700-000018000000}"/>
     <hyperlink ref="K25" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java" xr:uid="{00000000-0004-0000-0700-000019000000}"/>
@@ -11222,15 +11633,67 @@
     <hyperlink ref="K29" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
     <hyperlink ref="K30" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
     <hyperlink ref="K31" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
-    <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
-    <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
+    <hyperlink ref="C49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
+    <hyperlink ref="C48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
+    <hyperlink ref="C39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
     <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
     <hyperlink ref="K33" r:id="rId42" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
     <hyperlink ref="K34" r:id="rId43" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
+    <hyperlink ref="D9" r:id="rId44" xr:uid="{1250C759-2AC2-46FB-9436-FB01033AF6AE}"/>
+    <hyperlink ref="D10" r:id="rId45" xr:uid="{7FDFFB02-F70F-48A7-BD1A-150D962F6262}"/>
+    <hyperlink ref="D11" r:id="rId46" xr:uid="{BDB20524-3FD5-4444-99D2-DB1E9985E7EB}"/>
+    <hyperlink ref="D12" r:id="rId47" xr:uid="{2A75017D-0F7C-407D-BF3A-1B4BE02BE715}"/>
+    <hyperlink ref="D13" r:id="rId48" xr:uid="{D92B3973-866A-4AB9-809B-F68188EB72F4}"/>
+    <hyperlink ref="D14" r:id="rId49" xr:uid="{60424F70-EE4F-4F7A-91B3-C916B7DEAB7C}"/>
+    <hyperlink ref="D15" r:id="rId50" xr:uid="{8A853E80-54F2-4580-8E07-7CF5919A12F1}"/>
+    <hyperlink ref="D16" r:id="rId51" xr:uid="{80A981A4-3B1C-4CB1-B86E-468D2288FF99}"/>
+    <hyperlink ref="D17" r:id="rId52" xr:uid="{65992DF2-7BA6-4C55-83AF-B355A8A1193C}"/>
+    <hyperlink ref="D18" r:id="rId53" xr:uid="{A3506C47-CEF5-4AF0-838F-965E452E3ED4}"/>
+    <hyperlink ref="D19" r:id="rId54" xr:uid="{E7E5E194-EB37-4E24-BB5B-CA56A6CF696D}"/>
+    <hyperlink ref="D20" r:id="rId55" xr:uid="{29BA3650-8503-4640-8478-FE5F54E111D6}"/>
+    <hyperlink ref="D21" r:id="rId56" xr:uid="{5080F8D4-9535-42B5-A49C-89F41B7A9E79}"/>
+    <hyperlink ref="D22" r:id="rId57" xr:uid="{00B22C2E-386B-4997-BC2A-A440225348F2}"/>
+    <hyperlink ref="D23" r:id="rId58" xr:uid="{1935545E-9977-4C52-9F44-BFD42A079AC3}"/>
+    <hyperlink ref="D24" r:id="rId59" xr:uid="{12AB7105-A00B-4B2C-AD80-C9FDB4F21945}"/>
+    <hyperlink ref="D25" r:id="rId60" xr:uid="{4137AFD8-A3C1-4137-A978-D63CFBFCF44A}"/>
+    <hyperlink ref="D26" r:id="rId61" xr:uid="{25C4FD9B-4CD7-4CB8-8225-C8DBD1221855}"/>
+    <hyperlink ref="D27" r:id="rId62" xr:uid="{92572E17-78DE-4FD5-9461-FE24B092ED70}"/>
+    <hyperlink ref="D28" r:id="rId63" xr:uid="{DAFCF42C-BBCA-4299-98F6-EB3557BF2C4D}"/>
+    <hyperlink ref="D29" r:id="rId64" xr:uid="{738ED242-83B3-4DC9-B821-AE1A6CA9DBDF}"/>
+    <hyperlink ref="D30" r:id="rId65" xr:uid="{B9A096E1-2603-4E28-8A6E-1D70DE870018}"/>
+    <hyperlink ref="D31" r:id="rId66" xr:uid="{3AEC6811-EF8C-459F-821B-D896EE9AD1E0}"/>
+    <hyperlink ref="D32" r:id="rId67" xr:uid="{7063D5B7-28AD-4A5E-A596-8ACFDE39F7BD}"/>
+    <hyperlink ref="D33" r:id="rId68" xr:uid="{2CA5AA48-63A0-4EE2-9F90-BDC4D361AA9B}"/>
+    <hyperlink ref="D34" r:id="rId69" xr:uid="{B916335A-F62D-401B-BCAA-76DFFDACAFE9}"/>
+    <hyperlink ref="L9" r:id="rId70" xr:uid="{62190C63-5411-433A-989E-A9EDAD81C386}"/>
+    <hyperlink ref="L10" r:id="rId71" xr:uid="{C02034B0-525E-49A9-BAA6-3E9D7F41C850}"/>
+    <hyperlink ref="L11" r:id="rId72" xr:uid="{3AEF378E-45D0-47CE-9ACA-BAE51B13EDF5}"/>
+    <hyperlink ref="L12" r:id="rId73" xr:uid="{C3805017-3824-4A8F-9A83-4CBAC3AFDD66}"/>
+    <hyperlink ref="L13" r:id="rId74" xr:uid="{E68830A5-0849-4BCE-AFE6-2F4D77248205}"/>
+    <hyperlink ref="L14" r:id="rId75" xr:uid="{CCA99896-FABE-448E-B5AA-259959B088D1}"/>
+    <hyperlink ref="L15" r:id="rId76" xr:uid="{8AF1F30B-365B-4E27-9F5A-90183C58A31A}"/>
+    <hyperlink ref="L16" r:id="rId77" xr:uid="{B43A9E44-23AD-4A29-9E9E-01A1F5D5CEF9}"/>
+    <hyperlink ref="L23" r:id="rId78" xr:uid="{02AD8B83-FE0B-4C21-BFE5-98C1653F4741}"/>
+    <hyperlink ref="L24" r:id="rId79" xr:uid="{075A2DC3-2334-4398-839F-AEA1943F02F2}"/>
+    <hyperlink ref="L26" r:id="rId80" xr:uid="{8CDE4FB3-AE33-40B2-BDA3-CC72C5208311}"/>
+    <hyperlink ref="L25" r:id="rId81" xr:uid="{0D45CF61-657B-4FEF-A2EB-C6631FCD1A96}"/>
+    <hyperlink ref="L19" r:id="rId82" xr:uid="{F98754B5-4890-4132-8FB0-FAF4562FC5C6}"/>
+    <hyperlink ref="L20" r:id="rId83" xr:uid="{E2413C66-0F5D-4A18-90E0-D6E42C354ABD}"/>
+    <hyperlink ref="L21" r:id="rId84" xr:uid="{B4E66D75-EC36-4CF5-8FBC-496BD9DF1007}"/>
+    <hyperlink ref="L22" r:id="rId85" xr:uid="{3022FF93-B693-4F0A-9661-5547871B21D9}"/>
+    <hyperlink ref="L17" r:id="rId86" xr:uid="{EA063804-E37B-4F76-A980-C63B027E4FBD}"/>
+    <hyperlink ref="L18" r:id="rId87" xr:uid="{920FF6EE-8A33-4786-90E4-B0BE51323F8A}"/>
+    <hyperlink ref="L27" r:id="rId88" xr:uid="{DC39154B-83C5-4286-922E-EB6443BD6B64}"/>
+    <hyperlink ref="L28" r:id="rId89" xr:uid="{9DC41B85-5E51-43F8-B7CE-708E211DB6EE}"/>
+    <hyperlink ref="L29" r:id="rId90" xr:uid="{481806EA-5EEF-4E02-8838-C5946624CCAE}"/>
+    <hyperlink ref="L30" r:id="rId91" xr:uid="{8710AC91-E243-4C79-BD82-F3F56ABCE737}"/>
+    <hyperlink ref="L31" r:id="rId92" xr:uid="{1C181866-A257-4535-AFEB-E093DD934F05}"/>
+    <hyperlink ref="L32" r:id="rId93" xr:uid="{D724434B-CC4F-443A-BC6D-4D3ACBBB3923}"/>
+    <hyperlink ref="L33" r:id="rId94" xr:uid="{4C96ED4F-3A66-4DF7-BCF9-687BCA6D4E5C}"/>
+    <hyperlink ref="L34" r:id="rId95" xr:uid="{8C55AFC1-3023-4ABB-963B-F668100A2067}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId96"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 23:06:50.20
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7F42D5-0AE0-4770-9549-A4E03BAE05F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB2974-5AB1-4FCD-9AE3-C946044D1278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10578,7 +10578,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M9" sqref="M9:M34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 23:16:27.59
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB2974-5AB1-4FCD-9AE3-C946044D1278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7B9329-5908-435B-9943-627CB0E6A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="981">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3349,6 +3349,177 @@
   </si>
   <si>
     <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/generic-trees-intro-official/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/generic-tree-const-official/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/display-generic-tree/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/size-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/max-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/height-of-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/traversals-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/level-order-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/levelorder-linewise-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/levelorder-linewise-zigzag-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/level-order-traversal-alternates/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/mirror-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/remove-leaves-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/linearize-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/linearize-gt-efficient/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/find-in-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/node-to-root-path-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/lca-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/distance-between-nodes-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-generic-trees-similar-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-trees-mirror-in-shape-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/is-generic-tree-symmetric-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/multisolver-gt/video</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/pred-succ-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/ceil-and-floor-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/kth-largest-element-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/node-with-maximum-subtree-sum-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/diameter-of-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/iterative-preorder-postorder-generic-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/iterable-iterator-official/video</t>
+  </si>
+  <si>
+    <t>Iterable and Iterator - YouTube</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MirrorAGT.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/RemoveLeavesInGT.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/FindElementInGenericTree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/NodeToRootPath.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LowestCommonAncestor.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Distancebetween2Nodes.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesSimilarInShape.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreeSymmetric.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Multisolver.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/PredessorAndSuccessorElement.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/CeilAndFloor.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/KthLargestInGT.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxSumSubtree.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/DiameterGT.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/IterativePreorderPostorderGT.java</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t4IKNhNBTdo&amp;list=TLGGXv0lFdWAQ5EyMzA5MjAyMQ</t>
   </si>
 </sst>
 </file>
@@ -4275,12 +4446,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
@@ -4288,6 +4453,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Accent1" xfId="9" builtinId="30"/>
@@ -4699,10 +4870,10 @@
       <c r="C2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="157" t="s">
+      <c r="F2" s="161" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="157"/>
+      <c r="G2" s="161"/>
       <c r="J2" s="90" t="s">
         <v>294</v>
       </c>
@@ -8510,7 +8681,7 @@
       <c r="B2" s="106" t="s">
         <v>542</v>
       </c>
-      <c r="C2" s="159"/>
+      <c r="C2" s="157"/>
       <c r="D2" s="16"/>
       <c r="H2" s="16"/>
       <c r="J2"/>
@@ -8520,7 +8691,7 @@
       <c r="B3" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="160"/>
+      <c r="C3" s="158"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="34"/>
@@ -9128,22 +9299,22 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
-      <c r="C30" s="161"/>
+      <c r="C30" s="159"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
-      <c r="C31" s="161"/>
+      <c r="C31" s="159"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
-      <c r="C32" s="161"/>
+      <c r="C32" s="159"/>
     </row>
     <row r="33" spans="1:10" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C33" s="160"/>
+      <c r="C33" s="158"/>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="34"/>
@@ -9455,7 +9626,7 @@
       <c r="B46" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="C46" s="162"/>
+      <c r="C46" s="160"/>
       <c r="D46" s="5" t="s">
         <v>5</v>
       </c>
@@ -9480,7 +9651,7 @@
       <c r="B47" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="C47" s="162"/>
+      <c r="C47" s="160"/>
       <c r="I47" s="10" t="s">
         <v>363</v>
       </c>
@@ -9489,25 +9660,25 @@
       <c r="B48" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="C48" s="162"/>
+      <c r="C48" s="160"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="C49" s="162"/>
+      <c r="C49" s="160"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="C50" s="162"/>
+      <c r="C50" s="160"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="C51" s="162"/>
+      <c r="C51" s="160"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9619,16 +9790,16 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:12" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="162" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="158"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
       <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:12" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10578,7 +10749,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M9" sqref="M9:M34"/>
     </sheetView>
   </sheetViews>
@@ -10586,7 +10757,8 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="56" customWidth="1"/>
@@ -11700,23 +11872,24 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="3" max="3" width="45.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="42.28515625" customWidth="1"/>
     <col min="8" max="8" width="46.7109375" customWidth="1"/>
     <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" t="s">
         <v>673</v>
@@ -11725,14 +11898,14 @@
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="C2"/>
       <c r="G2" s="18" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
@@ -11764,7 +11937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>1</v>
       </c>
@@ -11773,13 +11946,19 @@
       </c>
       <c r="C4" s="97" t="s">
         <v>180</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>924</v>
       </c>
       <c r="F4" s="89"/>
       <c r="J4" s="16" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="16" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -11788,19 +11967,28 @@
       </c>
       <c r="C5" s="98" t="s">
         <v>181</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>925</v>
       </c>
       <c r="F5" s="89"/>
       <c r="J5" s="16" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="16" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>3</v>
       </c>
       <c r="C6" s="99" t="s">
         <v>182</v>
       </c>
+      <c r="D6" s="12" t="s">
+        <v>926</v>
+      </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
@@ -11819,14 +12007,20 @@
       <c r="J6" s="16" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="16" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
       <c r="C7" s="99" t="s">
         <v>183</v>
       </c>
+      <c r="D7" s="12" t="s">
+        <v>927</v>
+      </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
@@ -11842,14 +12036,20 @@
       <c r="J7" s="16" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="16" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
       <c r="C8" s="99" t="s">
         <v>184</v>
       </c>
+      <c r="D8" s="12" t="s">
+        <v>928</v>
+      </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -11865,14 +12065,20 @@
       <c r="J8" s="16" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="16" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
       <c r="C9" s="99" t="s">
         <v>185</v>
       </c>
+      <c r="D9" s="12" t="s">
+        <v>929</v>
+      </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
@@ -11888,14 +12094,20 @@
       <c r="J9" s="16" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="16" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>7</v>
       </c>
       <c r="C10" s="82" t="s">
         <v>186</v>
       </c>
+      <c r="D10" s="12" t="s">
+        <v>930</v>
+      </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
@@ -11914,14 +12126,20 @@
       <c r="J10" s="16" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="16" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
       <c r="C11" s="99" t="s">
         <v>187</v>
       </c>
+      <c r="D11" s="12" t="s">
+        <v>931</v>
+      </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
@@ -11940,8 +12158,11 @@
       <c r="J11" s="16" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="K11" s="16" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -11951,6 +12172,9 @@
       <c r="C12" s="99" t="s">
         <v>188</v>
       </c>
+      <c r="D12" s="12" t="s">
+        <v>932</v>
+      </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
@@ -11969,14 +12193,20 @@
       <c r="J12" s="16" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
       <c r="C13" s="99" t="s">
         <v>189</v>
       </c>
+      <c r="D13" s="12" t="s">
+        <v>933</v>
+      </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
@@ -11992,8 +12222,11 @@
       <c r="J13" s="16" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="16" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
@@ -12002,6 +12235,9 @@
       </c>
       <c r="C14" s="100" t="s">
         <v>190</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>934</v>
       </c>
       <c r="F14" s="89">
         <v>3</v>
@@ -12010,14 +12246,20 @@
       <c r="J14" s="16" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="16" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
       <c r="C15" s="101" t="s">
         <v>191</v>
       </c>
+      <c r="D15" s="12" t="s">
+        <v>935</v>
+      </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
@@ -12027,14 +12269,20 @@
       <c r="J15" s="16" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="16" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
       <c r="C16" s="102" t="s">
         <v>192</v>
       </c>
+      <c r="D16" s="12" t="s">
+        <v>936</v>
+      </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
@@ -12044,14 +12292,20 @@
       <c r="J16" s="16" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
       <c r="C17" s="102" t="s">
         <v>193</v>
       </c>
+      <c r="D17" s="12" t="s">
+        <v>937</v>
+      </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
@@ -12061,14 +12315,20 @@
       <c r="J17" s="16" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="16" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
       <c r="C18" s="102" t="s">
         <v>194</v>
       </c>
+      <c r="D18" s="12" t="s">
+        <v>938</v>
+      </c>
       <c r="E18" t="s">
         <v>6</v>
       </c>
@@ -12078,14 +12338,20 @@
       <c r="J18" s="16" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="16" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
       <c r="C19" s="112" t="s">
         <v>545</v>
       </c>
+      <c r="D19" s="12" t="s">
+        <v>939</v>
+      </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
@@ -12098,14 +12364,20 @@
       <c r="J19" s="16" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="16" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
       <c r="C20" s="111" t="s">
         <v>195</v>
       </c>
+      <c r="D20" s="12" t="s">
+        <v>940</v>
+      </c>
       <c r="E20" t="s">
         <v>6</v>
       </c>
@@ -12118,14 +12390,20 @@
       <c r="J20" s="16" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="16" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
       <c r="C21" s="111" t="s">
         <v>196</v>
       </c>
+      <c r="D21" s="12" t="s">
+        <v>941</v>
+      </c>
       <c r="E21" t="s">
         <v>6</v>
       </c>
@@ -12138,14 +12416,20 @@
       <c r="J21" s="16" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="16" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
       <c r="C22" s="113" t="s">
         <v>197</v>
       </c>
+      <c r="D22" s="12" t="s">
+        <v>942</v>
+      </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
@@ -12161,14 +12445,20 @@
       <c r="J22" s="16" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K22" s="16" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
       <c r="C23" s="102" t="s">
         <v>198</v>
       </c>
+      <c r="D23" s="12" t="s">
+        <v>943</v>
+      </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
@@ -12184,14 +12474,20 @@
       <c r="J23" s="16" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="16" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
       <c r="C24" s="102" t="s">
         <v>199</v>
       </c>
+      <c r="D24" s="12" t="s">
+        <v>944</v>
+      </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
@@ -12204,14 +12500,20 @@
       <c r="J24" s="16" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="16" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
       <c r="C25" s="103" t="s">
         <v>200</v>
       </c>
+      <c r="D25" s="12" t="s">
+        <v>945</v>
+      </c>
       <c r="E25" t="s">
         <v>6</v>
       </c>
@@ -12224,14 +12526,20 @@
       <c r="J25" s="16" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="16" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
       <c r="C26" s="104" t="s">
         <v>201</v>
       </c>
+      <c r="D26" s="12" t="s">
+        <v>946</v>
+      </c>
       <c r="E26" t="s">
         <v>606</v>
       </c>
@@ -12247,14 +12555,20 @@
       <c r="J26" s="16" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K26" s="16" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>202</v>
       </c>
+      <c r="D27" s="12" t="s">
+        <v>947</v>
+      </c>
       <c r="E27" t="s">
         <v>6</v>
       </c>
@@ -12270,14 +12584,20 @@
       <c r="J27" s="16" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K27" s="16" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
       <c r="C28" s="104" t="s">
         <v>203</v>
       </c>
+      <c r="D28" s="12" t="s">
+        <v>948</v>
+      </c>
       <c r="E28" t="s">
         <v>6</v>
       </c>
@@ -12290,14 +12610,20 @@
       <c r="J28" s="16" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="16" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>204</v>
       </c>
+      <c r="D29" s="12" t="s">
+        <v>949</v>
+      </c>
       <c r="E29" t="s">
         <v>6</v>
       </c>
@@ -12310,14 +12636,20 @@
       <c r="J29" s="16" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K29" s="16" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
       <c r="C30" s="104" t="s">
         <v>205</v>
       </c>
+      <c r="D30" s="12" t="s">
+        <v>950</v>
+      </c>
       <c r="E30" t="s">
         <v>6</v>
       </c>
@@ -12330,14 +12662,20 @@
       <c r="J30" s="16" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K30" s="16" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
       <c r="C31" s="104" t="s">
         <v>206</v>
       </c>
+      <c r="D31" s="12" t="s">
+        <v>951</v>
+      </c>
       <c r="E31" s="18" t="s">
         <v>604</v>
       </c>
@@ -12353,14 +12691,20 @@
       <c r="J31" s="16" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K31" s="16" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
       <c r="C32" s="104" t="s">
         <v>207</v>
       </c>
+      <c r="D32" s="12" t="s">
+        <v>952</v>
+      </c>
       <c r="E32" t="s">
         <v>605</v>
       </c>
@@ -12376,8 +12720,11 @@
       <c r="J32" s="16" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="16" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>30</v>
       </c>
@@ -12387,19 +12734,28 @@
       <c r="C33" s="110" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="D33" s="12" t="s">
+        <v>953</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>954</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A45" s="107"/>
       <c r="C45" s="109" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
         <v>560</v>
       </c>
@@ -12449,8 +12805,69 @@
     <hyperlink ref="J17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java" xr:uid="{00000000-0004-0000-0800-00001E000000}"/>
     <hyperlink ref="J18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java" xr:uid="{00000000-0004-0000-0800-00001F000000}"/>
     <hyperlink ref="J14" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java" xr:uid="{00000000-0004-0000-0800-000020000000}"/>
+    <hyperlink ref="D4" r:id="rId34" xr:uid="{D4ABD334-FF44-43AE-90F3-A426BA291205}"/>
+    <hyperlink ref="D5" r:id="rId35" xr:uid="{5E05733A-284E-4FDA-98A6-85F18DB3705E}"/>
+    <hyperlink ref="D6" r:id="rId36" xr:uid="{468ABA04-F935-4AF5-8BCD-7EEBF72EEBB2}"/>
+    <hyperlink ref="D7" r:id="rId37" xr:uid="{8EEAF7B6-A66F-46E1-82F0-3A193972E421}"/>
+    <hyperlink ref="D8" r:id="rId38" xr:uid="{9EF3EDBF-E848-486B-BEF0-1DED9E79C138}"/>
+    <hyperlink ref="D9" r:id="rId39" xr:uid="{87CC0FE9-8085-48E8-BFA0-0108B61B1E64}"/>
+    <hyperlink ref="D10" r:id="rId40" xr:uid="{8238F27C-6864-42AE-99F5-191EA7F98785}"/>
+    <hyperlink ref="D11" r:id="rId41" xr:uid="{D66F9AE9-99D4-4337-9DCE-CD042AB181FB}"/>
+    <hyperlink ref="D12" r:id="rId42" xr:uid="{A6BAA88D-959B-442B-9A77-E357B9163DEE}"/>
+    <hyperlink ref="D13" r:id="rId43" xr:uid="{85B8EBF8-E2BC-4699-8950-08598C8DD897}"/>
+    <hyperlink ref="D14" r:id="rId44" xr:uid="{4386827D-EF8C-4314-91AB-429D5B11EA7A}"/>
+    <hyperlink ref="D15" r:id="rId45" xr:uid="{D17649FE-74BE-4682-8066-F4BADB6FECC7}"/>
+    <hyperlink ref="D16" r:id="rId46" xr:uid="{40E39304-329B-4AAD-AA74-CD5F23A18F30}"/>
+    <hyperlink ref="D17" r:id="rId47" xr:uid="{12FCA221-FE48-46B0-A5B5-F236B28A6AC3}"/>
+    <hyperlink ref="D18" r:id="rId48" xr:uid="{30DB6669-37DC-426C-BA24-9EAA0084525D}"/>
+    <hyperlink ref="D19" r:id="rId49" xr:uid="{0000924C-55ED-4019-8BAB-712AA7D690B6}"/>
+    <hyperlink ref="D20" r:id="rId50" xr:uid="{37B578C7-8440-4612-AD91-D834287F18EF}"/>
+    <hyperlink ref="D21" r:id="rId51" xr:uid="{168790AF-0DF3-4D99-8D25-EA78E31C13D8}"/>
+    <hyperlink ref="D22" r:id="rId52" xr:uid="{7CD8F4D9-E5CD-4422-A128-26E85F6FBAA2}"/>
+    <hyperlink ref="D23" r:id="rId53" xr:uid="{5D6583E3-BD7E-4011-A782-741E9260C6EE}"/>
+    <hyperlink ref="D24" r:id="rId54" xr:uid="{03F0A843-1947-46F7-AF21-6AA99AD3A577}"/>
+    <hyperlink ref="D25" r:id="rId55" xr:uid="{B46E31AD-6A76-4E46-84AE-28CB4F069CF6}"/>
+    <hyperlink ref="D26" r:id="rId56" xr:uid="{D167A444-2E44-4A5A-BCE1-B93FE395F20C}"/>
+    <hyperlink ref="D27" r:id="rId57" xr:uid="{ACF2F197-FF05-45EC-B243-1926AF8CE472}"/>
+    <hyperlink ref="D28" r:id="rId58" xr:uid="{165B6DA4-ED97-43F7-92A8-97FD1241D078}"/>
+    <hyperlink ref="D29" r:id="rId59" xr:uid="{F741CDCD-FE7B-4D12-8FA1-1012971C3687}"/>
+    <hyperlink ref="D30" r:id="rId60" xr:uid="{D624581A-0098-4D2D-A9B9-D5CBDF18CCE2}"/>
+    <hyperlink ref="D31" r:id="rId61" xr:uid="{E1487140-06EF-44E8-BF9C-73CDEEA4F204}"/>
+    <hyperlink ref="D32" r:id="rId62" xr:uid="{4EFAD390-F4A8-4647-B5D9-07D1DFAA4DFF}"/>
+    <hyperlink ref="D33" r:id="rId63" xr:uid="{E76A0AF1-3819-4519-9BB7-1AED780D60D7}"/>
+    <hyperlink ref="J33" r:id="rId64" display="https://www.youtube.com/watch?v=t4IKNhNBTdo&amp;list=TLGGXv0lFdWAQ5EyMzA5MjAyMQ" xr:uid="{1C7C3B98-13B3-446C-8B2E-13A29D257446}"/>
+    <hyperlink ref="K4" r:id="rId65" xr:uid="{92709CB9-600F-41C0-BE33-08359F454B90}"/>
+    <hyperlink ref="K5" r:id="rId66" xr:uid="{66B0282D-E9D0-4A9B-A0FC-BC95E8BAA791}"/>
+    <hyperlink ref="K6" r:id="rId67" xr:uid="{71263F6E-F902-4874-92D7-8B8812F556DF}"/>
+    <hyperlink ref="K9" r:id="rId68" xr:uid="{1A6CAD56-C301-4CFA-B61E-28A3F0EBD1D4}"/>
+    <hyperlink ref="K7" r:id="rId69" xr:uid="{CA8B87A3-4918-4440-85F8-FF5068C1BDA3}"/>
+    <hyperlink ref="K8" r:id="rId70" xr:uid="{54C23A46-529E-41CA-B114-8E5C0E203980}"/>
+    <hyperlink ref="K10" r:id="rId71" xr:uid="{D8CEFDF9-4546-4DCA-AB22-4BBB7AE43D93}"/>
+    <hyperlink ref="K11" r:id="rId72" xr:uid="{E527A956-95AD-4E37-B688-4F9321FEAEEA}"/>
+    <hyperlink ref="K12" r:id="rId73" xr:uid="{D544F7DE-F2D8-45D5-875C-188680A4E9D8}"/>
+    <hyperlink ref="K13" r:id="rId74" xr:uid="{132DC6BD-1013-4468-A5B8-465D79EA341D}"/>
+    <hyperlink ref="K15" r:id="rId75" xr:uid="{D16601BC-93A0-47D1-BEAC-96B4E9EBB9D1}"/>
+    <hyperlink ref="K27" r:id="rId76" xr:uid="{5A7AF07C-59AA-40E2-8732-6960D1A59502}"/>
+    <hyperlink ref="K28" r:id="rId77" xr:uid="{6CC363D5-D2D6-449E-9DC2-9AF2CE0965E4}"/>
+    <hyperlink ref="K29" r:id="rId78" xr:uid="{075EB51A-D2E1-473C-BECC-27A4E1584F44}"/>
+    <hyperlink ref="K31" r:id="rId79" xr:uid="{E4F2405F-D9ED-4D9D-A072-14BBE29E9E4F}"/>
+    <hyperlink ref="K26" r:id="rId80" xr:uid="{3873C75A-9F21-4498-B884-5E1354FB1AA1}"/>
+    <hyperlink ref="K30" r:id="rId81" xr:uid="{6C087AD4-6469-4134-9690-3E6272CD0C57}"/>
+    <hyperlink ref="K32" r:id="rId82" xr:uid="{3DA6060A-E7EC-43CB-8C07-B4C5D4FCC5CB}"/>
+    <hyperlink ref="K25" r:id="rId83" xr:uid="{3A3F0012-47E0-44A0-AFFB-8B93E76029BD}"/>
+    <hyperlink ref="K24" r:id="rId84" xr:uid="{F8289C7C-DF8B-4308-9723-40E80424C2CE}"/>
+    <hyperlink ref="K23" r:id="rId85" xr:uid="{58E4C586-43BB-49F9-A45A-15AA028AC0EB}"/>
+    <hyperlink ref="K22" r:id="rId86" xr:uid="{0B2CD971-8ADC-456F-957B-2CFF9A92D1BF}"/>
+    <hyperlink ref="K21" r:id="rId87" xr:uid="{2EBB3680-132B-4A81-A959-7FEAA2C34CD5}"/>
+    <hyperlink ref="K20" r:id="rId88" xr:uid="{21D7929E-FED5-4EA3-A550-AACC7F8EBC87}"/>
+    <hyperlink ref="K19" r:id="rId89" xr:uid="{0D20CBF1-8637-4535-8F71-761001073FDF}"/>
+    <hyperlink ref="K16" r:id="rId90" xr:uid="{F064AF4C-9D2A-412A-852B-3B599ECF7EA9}"/>
+    <hyperlink ref="K17" r:id="rId91" xr:uid="{482BAA88-1AF3-4B0F-A2CE-45337797AA52}"/>
+    <hyperlink ref="K18" r:id="rId92" xr:uid="{F8FAE9A7-1282-44EC-8010-818A8A788402}"/>
+    <hyperlink ref="K14" r:id="rId93" xr:uid="{E80E5B15-DCE7-4E26-A247-680BDA5F0B44}"/>
+    <hyperlink ref="K33" r:id="rId94" xr:uid="{185294D4-5470-4E3F-B257-CC00169630E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId95"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   31-10-2021 - 22:54:49.24
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7B9329-5908-435B-9943-627CB0E6A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16843174-673E-433E-9773-C6FFBCB2E93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -4037,7 +4037,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4420,22 +4420,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="14" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="15" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4446,18 +4430,76 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="14" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="17" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="15" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -4870,10 +4912,10 @@
       <c r="C2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="161" t="s">
+      <c r="F2" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="161"/>
+      <c r="G2" s="151"/>
       <c r="J2" s="90" t="s">
         <v>294</v>
       </c>
@@ -6735,8 +6777,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6745,7 +6787,7 @@
     <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="4" style="8" customWidth="1"/>
     <col min="4" max="4" width="40.85546875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="174" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
@@ -6761,7 +6803,7 @@
       <c r="D1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="154"/>
       <c r="F1" s="16" t="s">
         <v>86</v>
       </c>
@@ -6774,7 +6816,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="154"/>
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6790,7 +6832,7 @@
       <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="166"/>
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6809,10 +6851,10 @@
       <c r="K3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="152" t="s">
+      <c r="L3" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="153" t="s">
+      <c r="M3" s="147" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6826,7 +6868,7 @@
       <c r="D4" s="145" t="s">
         <v>801</v>
       </c>
-      <c r="E4" s="146" t="s">
+      <c r="E4" s="167" t="s">
         <v>800</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -6847,7 +6889,7 @@
       <c r="L4" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="154" t="s">
+      <c r="M4" s="148" t="s">
         <v>745</v>
       </c>
       <c r="N4" t="str">
@@ -6865,7 +6907,7 @@
       <c r="D5" s="140" t="s">
         <v>738</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="168" t="s">
         <v>802</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -6886,7 +6928,7 @@
       <c r="L5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="155" t="s">
+      <c r="M5" s="149" t="s">
         <v>746</v>
       </c>
       <c r="N5" t="str">
@@ -6904,7 +6946,7 @@
       <c r="D6" s="140" t="s">
         <v>739</v>
       </c>
-      <c r="E6" s="147" t="s">
+      <c r="E6" s="168" t="s">
         <v>803</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -6925,7 +6967,7 @@
       <c r="L6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="155" t="s">
+      <c r="M6" s="149" t="s">
         <v>747</v>
       </c>
       <c r="N6" t="str">
@@ -6943,7 +6985,7 @@
       <c r="D7" s="140" t="s">
         <v>740</v>
       </c>
-      <c r="E7" s="147" t="s">
+      <c r="E7" s="168" t="s">
         <v>804</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -6964,7 +7006,7 @@
       <c r="L7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="155" t="s">
+      <c r="M7" s="149" t="s">
         <v>748</v>
       </c>
       <c r="N7" t="str">
@@ -6982,7 +7024,7 @@
       <c r="D8" s="140" t="s">
         <v>741</v>
       </c>
-      <c r="E8" s="147" t="s">
+      <c r="E8" s="168" t="s">
         <v>805</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -7003,7 +7045,7 @@
       <c r="L8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="155" t="s">
+      <c r="M8" s="149" t="s">
         <v>749</v>
       </c>
       <c r="N8" t="str">
@@ -7018,7 +7060,7 @@
       <c r="D9" s="140" t="s">
         <v>742</v>
       </c>
-      <c r="E9" s="147" t="s">
+      <c r="E9" s="168" t="s">
         <v>806</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -7036,7 +7078,7 @@
       <c r="L9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="155" t="s">
+      <c r="M9" s="149" t="s">
         <v>750</v>
       </c>
       <c r="N9" t="str">
@@ -7054,7 +7096,7 @@
       <c r="D10" s="140" t="s">
         <v>743</v>
       </c>
-      <c r="E10" s="147" t="s">
+      <c r="E10" s="168" t="s">
         <v>807</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -7078,7 +7120,7 @@
       <c r="L10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="155" t="s">
+      <c r="M10" s="149" t="s">
         <v>751</v>
       </c>
       <c r="N10" t="str">
@@ -7096,7 +7138,7 @@
       <c r="D11" s="140" t="s">
         <v>744</v>
       </c>
-      <c r="E11" s="147" t="s">
+      <c r="E11" s="168" t="s">
         <v>808</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -7120,7 +7162,7 @@
       <c r="L11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="155" t="s">
+      <c r="M11" s="149" t="s">
         <v>752</v>
       </c>
       <c r="N11" t="str">
@@ -7138,7 +7180,7 @@
       <c r="D12" s="141" t="s">
         <v>776</v>
       </c>
-      <c r="E12" s="148" t="s">
+      <c r="E12" s="169" t="s">
         <v>809</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -7156,7 +7198,7 @@
       <c r="L12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="155" t="s">
+      <c r="M12" s="149" t="s">
         <v>753</v>
       </c>
       <c r="N12" t="str">
@@ -7174,7 +7216,7 @@
       <c r="D13" s="141" t="s">
         <v>777</v>
       </c>
-      <c r="E13" s="148" t="s">
+      <c r="E13" s="169" t="s">
         <v>810</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -7195,7 +7237,7 @@
       <c r="L13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="155" t="s">
+      <c r="M13" s="149" t="s">
         <v>754</v>
       </c>
       <c r="N13" t="str">
@@ -7213,7 +7255,7 @@
       <c r="D14" s="141" t="s">
         <v>778</v>
       </c>
-      <c r="E14" s="148" t="s">
+      <c r="E14" s="169" t="s">
         <v>811</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -7234,7 +7276,7 @@
       <c r="L14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="155" t="s">
+      <c r="M14" s="149" t="s">
         <v>755</v>
       </c>
       <c r="N14" t="str">
@@ -7252,7 +7294,7 @@
       <c r="D15" s="141" t="s">
         <v>779</v>
       </c>
-      <c r="E15" s="148" t="s">
+      <c r="E15" s="169" t="s">
         <v>812</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -7267,7 +7309,7 @@
       <c r="L15" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="M15" s="155" t="s">
+      <c r="M15" s="149" t="s">
         <v>756</v>
       </c>
       <c r="N15" t="str">
@@ -7285,7 +7327,7 @@
       <c r="D16" s="141" t="s">
         <v>780</v>
       </c>
-      <c r="E16" s="148" t="s">
+      <c r="E16" s="169" t="s">
         <v>813</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -7300,7 +7342,7 @@
       <c r="L16" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="M16" s="155" t="s">
+      <c r="M16" s="149" t="s">
         <v>757</v>
       </c>
       <c r="N16" t="str">
@@ -7318,7 +7360,7 @@
       <c r="D17" s="141" t="s">
         <v>781</v>
       </c>
-      <c r="E17" s="148" t="s">
+      <c r="E17" s="169" t="s">
         <v>814</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -7336,7 +7378,7 @@
       <c r="L17" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="M17" s="155" t="s">
+      <c r="M17" s="149" t="s">
         <v>758</v>
       </c>
       <c r="N17" t="str">
@@ -7354,7 +7396,7 @@
       <c r="D18" s="143" t="s">
         <v>782</v>
       </c>
-      <c r="E18" s="149" t="s">
+      <c r="E18" s="170" t="s">
         <v>815</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -7372,7 +7414,7 @@
       <c r="L18" s="16" t="s">
         <v>641</v>
       </c>
-      <c r="M18" s="155" t="s">
+      <c r="M18" s="149" t="s">
         <v>759</v>
       </c>
       <c r="N18" t="str">
@@ -7390,7 +7432,7 @@
       <c r="D19" s="143" t="s">
         <v>783</v>
       </c>
-      <c r="E19" s="149" t="s">
+      <c r="E19" s="170" t="s">
         <v>816</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -7405,7 +7447,7 @@
       <c r="L19" s="16" t="s">
         <v>642</v>
       </c>
-      <c r="M19" s="155" t="s">
+      <c r="M19" s="149" t="s">
         <v>760</v>
       </c>
       <c r="N19" t="str">
@@ -7423,7 +7465,7 @@
       <c r="D20" s="143" t="s">
         <v>784</v>
       </c>
-      <c r="E20" s="149" t="s">
+      <c r="E20" s="170" t="s">
         <v>817</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -7438,7 +7480,7 @@
       <c r="L20" s="16" t="s">
         <v>640</v>
       </c>
-      <c r="M20" s="155" t="s">
+      <c r="M20" s="149" t="s">
         <v>761</v>
       </c>
       <c r="N20" t="str">
@@ -7456,7 +7498,7 @@
       <c r="D21" s="143" t="s">
         <v>785</v>
       </c>
-      <c r="E21" s="149" t="s">
+      <c r="E21" s="170" t="s">
         <v>818</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -7471,7 +7513,7 @@
       <c r="L21" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="M21" s="155" t="s">
+      <c r="M21" s="149" t="s">
         <v>762</v>
       </c>
       <c r="N21" t="str">
@@ -7489,7 +7531,7 @@
       <c r="D22" s="143" t="s">
         <v>786</v>
       </c>
-      <c r="E22" s="149" t="s">
+      <c r="E22" s="170" t="s">
         <v>819</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -7504,7 +7546,7 @@
       <c r="L22" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="M22" s="155" t="s">
+      <c r="M22" s="149" t="s">
         <v>763</v>
       </c>
       <c r="N22" t="str">
@@ -7522,7 +7564,7 @@
       <c r="D23" s="142" t="s">
         <v>787</v>
       </c>
-      <c r="E23" s="150" t="s">
+      <c r="E23" s="171" t="s">
         <v>820</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -7543,7 +7585,7 @@
       <c r="L23" s="16" t="s">
         <v>637</v>
       </c>
-      <c r="M23" s="155" t="s">
+      <c r="M23" s="149" t="s">
         <v>764</v>
       </c>
       <c r="N23" t="str">
@@ -7561,7 +7603,7 @@
       <c r="D24" s="142" t="s">
         <v>788</v>
       </c>
-      <c r="E24" s="150" t="s">
+      <c r="E24" s="171" t="s">
         <v>821</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -7582,7 +7624,7 @@
       <c r="L24" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="M24" s="155" t="s">
+      <c r="M24" s="149" t="s">
         <v>765</v>
       </c>
       <c r="N24" t="str">
@@ -7600,7 +7642,7 @@
       <c r="D25" s="142" t="s">
         <v>789</v>
       </c>
-      <c r="E25" s="150" t="s">
+      <c r="E25" s="171" t="s">
         <v>822</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -7618,7 +7660,7 @@
       <c r="L25" s="16" t="s">
         <v>633</v>
       </c>
-      <c r="M25" s="155" t="s">
+      <c r="M25" s="149" t="s">
         <v>766</v>
       </c>
       <c r="N25" t="str">
@@ -7636,7 +7678,7 @@
       <c r="D26" s="142" t="s">
         <v>790</v>
       </c>
-      <c r="E26" s="150" t="s">
+      <c r="E26" s="171" t="s">
         <v>823</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -7654,7 +7696,7 @@
       <c r="L26" s="16" t="s">
         <v>634</v>
       </c>
-      <c r="M26" s="155" t="s">
+      <c r="M26" s="149" t="s">
         <v>767</v>
       </c>
       <c r="N26" t="str">
@@ -7672,7 +7714,7 @@
       <c r="D27" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="E27" s="150" t="s">
+      <c r="E27" s="171" t="s">
         <v>824</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -7693,7 +7735,7 @@
       <c r="L27" s="16" t="s">
         <v>635</v>
       </c>
-      <c r="M27" s="155" t="s">
+      <c r="M27" s="149" t="s">
         <v>768</v>
       </c>
       <c r="N27" t="str">
@@ -7711,7 +7753,7 @@
       <c r="D28" s="142" t="s">
         <v>792</v>
       </c>
-      <c r="E28" s="150" t="s">
+      <c r="E28" s="171" t="s">
         <v>825</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -7729,7 +7771,7 @@
       <c r="L28" s="16" t="s">
         <v>636</v>
       </c>
-      <c r="M28" s="155" t="s">
+      <c r="M28" s="149" t="s">
         <v>769</v>
       </c>
       <c r="N28" t="str">
@@ -7747,7 +7789,7 @@
       <c r="D29" s="142" t="s">
         <v>793</v>
       </c>
-      <c r="E29" s="150" t="s">
+      <c r="E29" s="171" t="s">
         <v>826</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -7768,7 +7810,7 @@
       <c r="L29" s="16" t="s">
         <v>631</v>
       </c>
-      <c r="M29" s="155" t="s">
+      <c r="M29" s="149" t="s">
         <v>770</v>
       </c>
       <c r="N29" t="str">
@@ -7786,7 +7828,7 @@
       <c r="D30" s="144" t="s">
         <v>794</v>
       </c>
-      <c r="E30" s="151" t="s">
+      <c r="E30" s="172" t="s">
         <v>827</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7807,7 +7849,7 @@
       <c r="L30" s="16" t="s">
         <v>626</v>
       </c>
-      <c r="M30" s="155" t="s">
+      <c r="M30" s="149" t="s">
         <v>771</v>
       </c>
       <c r="N30" t="str">
@@ -7825,7 +7867,7 @@
       <c r="D31" s="144" t="s">
         <v>795</v>
       </c>
-      <c r="E31" s="151" t="s">
+      <c r="E31" s="172" t="s">
         <v>828</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -7846,7 +7888,7 @@
       <c r="L31" s="16" t="s">
         <v>630</v>
       </c>
-      <c r="M31" s="155" t="s">
+      <c r="M31" s="149" t="s">
         <v>772</v>
       </c>
       <c r="N31" t="str">
@@ -7864,7 +7906,7 @@
       <c r="D32" s="144" t="s">
         <v>796</v>
       </c>
-      <c r="E32" s="151" t="s">
+      <c r="E32" s="172" t="s">
         <v>829</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -7885,7 +7927,7 @@
       <c r="L32" s="16" t="s">
         <v>629</v>
       </c>
-      <c r="M32" s="155" t="s">
+      <c r="M32" s="149" t="s">
         <v>773</v>
       </c>
       <c r="N32" t="str">
@@ -7897,7 +7939,7 @@
       <c r="D33" s="144" t="s">
         <v>797</v>
       </c>
-      <c r="E33" s="151" t="s">
+      <c r="E33" s="172" t="s">
         <v>829</v>
       </c>
       <c r="H33" s="2">
@@ -7909,7 +7951,7 @@
       <c r="L33" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="M33" s="155" t="s">
+      <c r="M33" s="149" t="s">
         <v>774</v>
       </c>
       <c r="N33" t="str">
@@ -7927,7 +7969,7 @@
       <c r="D34" s="144" t="s">
         <v>799</v>
       </c>
-      <c r="E34" s="151" t="s">
+      <c r="E34" s="172" t="s">
         <v>798</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -7948,7 +7990,7 @@
       <c r="L34" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="M34" s="156" t="s">
+      <c r="M34" s="150" t="s">
         <v>775</v>
       </c>
       <c r="N34" t="str">
@@ -7958,22 +8000,22 @@
     </row>
     <row r="35" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
+      <c r="E35" s="163"/>
       <c r="L35" s="16"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="163"/>
       <c r="L36" s="16"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
+      <c r="E37" s="173"/>
       <c r="L37" s="16"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
+      <c r="E38" s="163"/>
       <c r="L38" s="16"/>
     </row>
   </sheetData>
@@ -8645,14 +8687,14 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="52.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="154" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
@@ -8667,7 +8709,6 @@
       <c r="B1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="5"/>
       <c r="D1" s="16" t="s">
         <v>310</v>
       </c>
@@ -8681,7 +8722,7 @@
       <c r="B2" s="106" t="s">
         <v>542</v>
       </c>
-      <c r="C2" s="157"/>
+      <c r="C2" s="164"/>
       <c r="D2" s="16"/>
       <c r="H2" s="16"/>
       <c r="J2"/>
@@ -8691,7 +8732,7 @@
       <c r="B3" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="158"/>
+      <c r="C3" s="165"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="34"/>
@@ -8707,7 +8748,7 @@
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="166"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -8737,7 +8778,7 @@
       <c r="B5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="153" t="s">
         <v>847</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -8770,7 +8811,7 @@
       <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="153" t="s">
         <v>848</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -8803,7 +8844,7 @@
       <c r="B7" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="153" t="s">
         <v>849</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -8836,7 +8877,7 @@
       <c r="B8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="153" t="s">
         <v>850</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -8869,7 +8910,7 @@
       <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="153" t="s">
         <v>851</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -8899,7 +8940,7 @@
       <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="153" t="s">
         <v>852</v>
       </c>
       <c r="D10" s="56" t="s">
@@ -8930,7 +8971,7 @@
       <c r="B11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="153" t="s">
         <v>853</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -8966,7 +9007,7 @@
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="153" t="s">
         <v>854</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -8999,7 +9040,7 @@
       <c r="B13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="153" t="s">
         <v>855</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -9032,7 +9073,7 @@
       <c r="B14" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="153" t="s">
         <v>856</v>
       </c>
       <c r="D14" s="56" t="s">
@@ -9066,7 +9107,7 @@
       <c r="B15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="153" t="s">
         <v>857</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -9099,7 +9140,7 @@
       <c r="B16" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="153" t="s">
         <v>858</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -9129,7 +9170,7 @@
       <c r="B17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="153" t="s">
         <v>859</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -9159,7 +9200,7 @@
       <c r="B18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="153" t="s">
         <v>860</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -9189,7 +9230,7 @@
       <c r="B19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="153" t="s">
         <v>861</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -9216,7 +9257,7 @@
       <c r="B20" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="153" t="s">
         <v>862</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -9252,7 +9293,7 @@
       <c r="B21" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="153" t="s">
         <v>863</v>
       </c>
       <c r="D21" s="53" t="s">
@@ -9277,44 +9318,44 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="31"/>
+      <c r="C22" s="153"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="31"/>
+      <c r="C23" s="153"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="31"/>
+      <c r="C24" s="153"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="31"/>
+      <c r="C25" s="153"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="31"/>
+      <c r="C26" s="153"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="31"/>
+      <c r="C27" s="153"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="31"/>
+      <c r="C28" s="153"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
-      <c r="C30" s="159"/>
+      <c r="C30" s="160"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
-      <c r="C31" s="159"/>
+      <c r="C31" s="160"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
-      <c r="C32" s="159"/>
+      <c r="C32" s="160"/>
     </row>
     <row r="33" spans="1:10" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C33" s="158"/>
+      <c r="C33" s="165"/>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="34"/>
@@ -9330,7 +9371,7 @@
       <c r="B34" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="C34" s="31"/>
+      <c r="C34" s="153"/>
       <c r="D34" s="5" t="s">
         <v>177</v>
       </c>
@@ -9352,7 +9393,7 @@
       <c r="B35" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="153"/>
       <c r="D35" s="5" t="s">
         <v>177</v>
       </c>
@@ -9377,7 +9418,7 @@
       <c r="B36" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="C36" s="31"/>
+      <c r="C36" s="153"/>
       <c r="D36" s="5" t="s">
         <v>5</v>
       </c>
@@ -9399,7 +9440,7 @@
       <c r="B37" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="153"/>
       <c r="D37" s="5" t="s">
         <v>322</v>
       </c>
@@ -9425,7 +9466,7 @@
       <c r="B38" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="31"/>
+      <c r="C38" s="153"/>
       <c r="D38" s="5" t="s">
         <v>322</v>
       </c>
@@ -9448,7 +9489,7 @@
       <c r="B39" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="C39" s="31"/>
+      <c r="C39" s="153"/>
       <c r="D39" s="5" t="s">
         <v>322</v>
       </c>
@@ -9473,7 +9514,7 @@
       <c r="B40" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="C40" s="21"/>
+      <c r="C40" s="153"/>
       <c r="D40" s="5" t="s">
         <v>177</v>
       </c>
@@ -9495,7 +9536,7 @@
       <c r="B41" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="21"/>
+      <c r="C41" s="153"/>
       <c r="D41" s="5" t="s">
         <v>322</v>
       </c>
@@ -9520,7 +9561,7 @@
       <c r="B42" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="C42" s="21"/>
+      <c r="C42" s="153"/>
       <c r="D42" s="5" t="s">
         <v>322</v>
       </c>
@@ -9545,7 +9586,7 @@
       <c r="B43" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="C43" s="21"/>
+      <c r="C43" s="153"/>
       <c r="D43" s="5" t="s">
         <v>177</v>
       </c>
@@ -9570,7 +9611,7 @@
       <c r="B44" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="C44" s="21"/>
+      <c r="C44" s="153"/>
       <c r="D44" s="5" t="s">
         <v>177</v>
       </c>
@@ -9598,7 +9639,7 @@
       <c r="B45" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="C45" s="21"/>
+      <c r="C45" s="153"/>
       <c r="D45" s="5" t="s">
         <v>177</v>
       </c>
@@ -9626,7 +9667,7 @@
       <c r="B46" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="C46" s="160"/>
+      <c r="C46" s="163"/>
       <c r="D46" s="5" t="s">
         <v>5</v>
       </c>
@@ -9651,7 +9692,7 @@
       <c r="B47" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="C47" s="160"/>
+      <c r="C47" s="163"/>
       <c r="I47" s="10" t="s">
         <v>363</v>
       </c>
@@ -9660,25 +9701,25 @@
       <c r="B48" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="C48" s="160"/>
+      <c r="C48" s="163"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="C49" s="160"/>
+      <c r="C49" s="163"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="C50" s="160"/>
+      <c r="C50" s="163"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="C51" s="160"/>
+      <c r="C51" s="163"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9765,13 +9806,14 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="46.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="154" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
     <col min="8" max="8" width="49.42578125" customWidth="1"/>
@@ -9783,23 +9825,22 @@
       <c r="B1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="5"/>
       <c r="D1" s="16" t="s">
         <v>310</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:12" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="152" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
       <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:12" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9809,7 +9850,7 @@
       <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="159"/>
       <c r="D3" s="28" t="s">
         <v>1</v>
       </c>
@@ -9839,7 +9880,7 @@
       <c r="B4" s="64" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="161" t="s">
         <v>864</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -9872,7 +9913,7 @@
       <c r="B5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="161" t="s">
         <v>865</v>
       </c>
       <c r="D5" s="5"/>
@@ -9899,7 +9940,7 @@
       <c r="B6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="161" t="s">
         <v>866</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -9930,7 +9971,7 @@
       <c r="B7" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="161" t="s">
         <v>867</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -9954,14 +9995,14 @@
         <v>|[Queue to Stack Adapter- pop efficient ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/queue-to-stack-adapter-pop-efficient/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java)|</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="161" t="s">
         <v>868</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -9985,14 +10026,14 @@
         <v>|[Stack to Queue Adapter-Add efficient](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-add-efficient-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java)|</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="161" t="s">
         <v>869</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -10016,14 +10057,14 @@
         <v>|[Stack to Queue Adapter-Remove efficient](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/stack-to-queue-adapter-remove-efficient-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java)|</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="161" t="s">
         <v>870</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -10056,7 +10097,7 @@
       <c r="B11" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="153"/>
       <c r="D11" s="5" t="s">
         <v>374</v>
       </c>
@@ -10086,13 +10127,13 @@
       <c r="B14" s="16" t="s">
         <v>413</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="163"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10749,8 +10790,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M34"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10758,7 +10799,7 @@
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="160" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="56" customWidth="1"/>
@@ -10772,7 +10813,7 @@
       <c r="C1" s="87" t="s">
         <v>511</v>
       </c>
-      <c r="D1" s="87"/>
+      <c r="D1" s="157"/>
       <c r="E1" s="5">
         <v>0</v>
       </c>
@@ -10783,7 +10824,7 @@
       <c r="C2" s="88" t="s">
         <v>512</v>
       </c>
-      <c r="D2" s="88"/>
+      <c r="D2" s="158"/>
       <c r="E2" s="88" t="s">
         <v>513</v>
       </c>
@@ -10792,25 +10833,25 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="D3" s="157"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
+      <c r="D4" s="157"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
+      <c r="D5" s="157"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
+      <c r="D6" s="157"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10823,7 +10864,7 @@
       <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="159"/>
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
@@ -10851,14 +10892,14 @@
         <v>416</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="C9" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="161" t="s">
         <v>879</v>
       </c>
       <c r="E9" t="s">
@@ -10878,14 +10919,14 @@
         <v>|[ Add Last In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-last-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>2</v>
       </c>
       <c r="C10" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="161" t="s">
         <v>880</v>
       </c>
       <c r="E10" t="s">
@@ -10905,14 +10946,14 @@
         <v>|[ Display A Linkedlist ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>3</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="161" t="s">
         <v>881</v>
       </c>
       <c r="E11" t="s">
@@ -10932,14 +10973,14 @@
         <v>|[ Remove First In Linkedlist ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-first-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>4</v>
       </c>
       <c r="C12" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="161" t="s">
         <v>882</v>
       </c>
       <c r="E12" t="s">
@@ -10959,14 +11000,14 @@
         <v>|[ Get Value In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/get-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>5</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="161" t="s">
         <v>883</v>
       </c>
       <c r="E13" t="s">
@@ -10986,14 +11027,14 @@
         <v>|[ Add First In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-first-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>6</v>
       </c>
       <c r="C14" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="161" t="s">
         <v>884</v>
       </c>
       <c r="E14" t="s">
@@ -11013,14 +11054,14 @@
         <v>|[ Add At Index In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/add-at-index-in-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>7</v>
       </c>
       <c r="C15" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="161" t="s">
         <v>885</v>
       </c>
       <c r="E15" t="s">
@@ -11040,14 +11081,14 @@
         <v>|[ Remove Last In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-last-in-linked-list/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java)|</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>8</v>
       </c>
       <c r="C16" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="161" t="s">
         <v>886</v>
       </c>
       <c r="E16" t="s">
@@ -11074,7 +11115,7 @@
       <c r="C17" s="82" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="161" t="s">
         <v>887</v>
       </c>
       <c r="E17" t="s">
@@ -11107,7 +11148,7 @@
       <c r="C18" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="161" t="s">
         <v>888</v>
       </c>
       <c r="E18" t="s">
@@ -11130,14 +11171,14 @@
         <v>|[ Reverse Linked List (pointer Iterative) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-pi-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java)|</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>11</v>
       </c>
       <c r="C19" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="161" t="s">
         <v>889</v>
       </c>
       <c r="E19" t="s">
@@ -11160,14 +11201,14 @@
         <v>|[ Linked List To Stack Adapter ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linkedlist-to-stack-adapter-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java)|</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>12</v>
       </c>
       <c r="C20" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="161" t="s">
         <v>890</v>
       </c>
       <c r="E20" t="s">
@@ -11190,14 +11231,14 @@
         <v>|[ Linked List To Queue Adapter ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/linked-list-to-queue-adapter-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java)|</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>13</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="161" t="s">
         <v>891</v>
       </c>
       <c r="E21" t="s">
@@ -11220,14 +11261,14 @@
         <v>|[ Kth Node From End Of Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kth-from-last-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java)|</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>14</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="161" t="s">
         <v>892</v>
       </c>
       <c r="E22" t="s">
@@ -11250,14 +11291,14 @@
         <v>|[ Mid Of Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mid-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java)|</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>15</v>
       </c>
       <c r="C23" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="161" t="s">
         <v>893</v>
       </c>
       <c r="E23" t="s">
@@ -11286,14 +11327,14 @@
         <v>|[ Merge Two Sorted Linked Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/merge-two-sorted-linked-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java)|</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>16</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="161" t="s">
         <v>894</v>
       </c>
       <c r="E24" t="s">
@@ -11313,14 +11354,14 @@
         <v>|[ Merge Sort A Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/mergesort-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java)|</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>17</v>
       </c>
       <c r="C25" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="161" t="s">
         <v>895</v>
       </c>
       <c r="E25" t="s">
@@ -11343,14 +11384,14 @@
         <v>|[ Remove Duplicates In A Sorted Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/remove-duplicates-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java)|</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>18</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="161" t="s">
         <v>896</v>
       </c>
       <c r="E26" t="s">
@@ -11370,14 +11411,14 @@
         <v>|[ Odd Even Linked List Medium](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/odd-even-linked-list-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java)|</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>19</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="161" t="s">
         <v>897</v>
       </c>
       <c r="E27" t="s">
@@ -11397,14 +11438,14 @@
         <v>|[ K Reverse In Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/kreverse-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java)|</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>20</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="161" t="s">
         <v>898</v>
       </c>
       <c r="E28" t="s">
@@ -11424,14 +11465,14 @@
         <v>|[ Display Reverse (recursive) - Linked List ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/display-reverse-linkedlist-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java)|</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>21</v>
       </c>
       <c r="C29" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="161" t="s">
         <v>899</v>
       </c>
       <c r="E29" t="s">
@@ -11451,14 +11492,14 @@
         <v>|[ Reverse Linked List (pointer - Recursive) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/linkedlist/reverse-linkedlist-pr-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java)|</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>22</v>
       </c>
       <c r="C30" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="161" t="s">
         <v>900</v>
       </c>
       <c r="E30" t="s">
@@ -11488,7 +11529,7 @@
       <c r="C31" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="161" t="s">
         <v>901</v>
       </c>
       <c r="E31" t="s">
@@ -11524,7 +11565,7 @@
       <c r="C32" s="91" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="161" t="s">
         <v>902</v>
       </c>
       <c r="E32" t="s">
@@ -11557,7 +11598,7 @@
       <c r="C33" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="161" t="s">
         <v>903</v>
       </c>
       <c r="E33" t="s">
@@ -11590,7 +11631,7 @@
       <c r="C34" s="86" t="s">
         <v>505</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="161" t="s">
         <v>904</v>
       </c>
       <c r="E34" t="s">
@@ -11621,14 +11662,14 @@
       <c r="C36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="D36" s="77"/>
+      <c r="D36" s="162"/>
       <c r="G36" s="78"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C38" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="163"/>
       <c r="F38" t="s">
         <v>6</v>
       </c>
@@ -11640,13 +11681,13 @@
       <c r="C39" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="D39" s="16"/>
+      <c r="D39" s="163"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C40" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="163"/>
       <c r="F40" t="s">
         <v>6</v>
       </c>
@@ -11658,7 +11699,7 @@
       <c r="C41" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="163"/>
       <c r="F41" t="s">
         <v>6</v>
       </c>
@@ -11670,7 +11711,7 @@
       <c r="C42" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="163"/>
       <c r="F42" t="s">
         <v>6</v>
       </c>
@@ -11682,7 +11723,7 @@
       <c r="C43" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D43" s="163"/>
       <c r="F43" t="s">
         <v>6</v>
       </c>
@@ -11698,7 +11739,7 @@
       <c r="C44" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D44" s="163"/>
       <c r="F44" t="s">
         <v>6</v>
       </c>
@@ -11710,7 +11751,7 @@
       <c r="C45" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="D45" s="16"/>
+      <c r="D45" s="163"/>
       <c r="F45" t="s">
         <v>6</v>
       </c>
@@ -11722,7 +11763,7 @@
       <c r="C46" s="16" t="s">
         <v>470</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="163"/>
       <c r="F46" t="s">
         <v>6</v>
       </c>
@@ -11737,7 +11778,7 @@
       <c r="C47" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="D47" s="16"/>
+      <c r="D47" s="163"/>
       <c r="G47" s="5">
         <v>0</v>
       </c>
@@ -11746,7 +11787,7 @@
       <c r="C48" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="D48" s="16"/>
+      <c r="D48" s="163"/>
       <c r="F48" t="s">
         <v>6</v>
       </c>
@@ -11758,7 +11799,7 @@
       <c r="C49" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="D49" s="16"/>
+      <c r="D49" s="163"/>
       <c r="F49" t="s">
         <v>6</v>
       </c>
@@ -11874,15 +11915,15 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="3" max="3" width="45.140625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="154" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="42.28515625" customWidth="1"/>
     <col min="8" max="8" width="46.7109375" customWidth="1"/>
@@ -11915,7 +11956,7 @@
       <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="155" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -11937,7 +11978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>1</v>
       </c>
@@ -11947,7 +11988,7 @@
       <c r="C4" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="153" t="s">
         <v>924</v>
       </c>
       <c r="F4" s="89"/>
@@ -11958,7 +11999,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -11968,7 +12009,7 @@
       <c r="C5" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="153" t="s">
         <v>925</v>
       </c>
       <c r="F5" s="89"/>
@@ -11986,7 +12027,7 @@
       <c r="C6" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="153" t="s">
         <v>926</v>
       </c>
       <c r="E6" t="s">
@@ -12018,7 +12059,7 @@
       <c r="C7" s="99" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="153" t="s">
         <v>927</v>
       </c>
       <c r="E7" t="s">
@@ -12040,14 +12081,14 @@
         <v>956</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
       <c r="C8" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="153" t="s">
         <v>928</v>
       </c>
       <c r="E8" t="s">
@@ -12069,14 +12110,14 @@
         <v>957</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
       <c r="C9" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="153" t="s">
         <v>929</v>
       </c>
       <c r="E9" t="s">
@@ -12098,14 +12139,14 @@
         <v>958</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>7</v>
       </c>
       <c r="C10" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="153" t="s">
         <v>930</v>
       </c>
       <c r="E10" t="s">
@@ -12130,14 +12171,14 @@
         <v>959</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
       <c r="C11" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="153" t="s">
         <v>931</v>
       </c>
       <c r="E11" t="s">
@@ -12162,7 +12203,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -12172,7 +12213,7 @@
       <c r="C12" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="153" t="s">
         <v>932</v>
       </c>
       <c r="E12" t="s">
@@ -12197,14 +12238,14 @@
         <v>961</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
       <c r="C13" s="99" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="153" t="s">
         <v>933</v>
       </c>
       <c r="E13" t="s">
@@ -12226,7 +12267,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
@@ -12236,7 +12277,7 @@
       <c r="C14" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="153" t="s">
         <v>934</v>
       </c>
       <c r="F14" s="89">
@@ -12250,14 +12291,14 @@
         <v>961</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
       <c r="C15" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="153" t="s">
         <v>935</v>
       </c>
       <c r="E15" t="s">
@@ -12273,14 +12314,14 @@
         <v>963</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
       <c r="C16" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="153" t="s">
         <v>936</v>
       </c>
       <c r="E16" t="s">
@@ -12296,14 +12337,14 @@
         <v>964</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
       <c r="C17" s="102" t="s">
         <v>193</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="153" t="s">
         <v>937</v>
       </c>
       <c r="E17" t="s">
@@ -12319,14 +12360,14 @@
         <v>965</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
       <c r="C18" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="153" t="s">
         <v>938</v>
       </c>
       <c r="E18" t="s">
@@ -12342,14 +12383,14 @@
         <v>965</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
       <c r="C19" s="112" t="s">
         <v>545</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="153" t="s">
         <v>939</v>
       </c>
       <c r="E19" t="s">
@@ -12368,14 +12409,14 @@
         <v>966</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
       <c r="C20" s="111" t="s">
         <v>195</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="153" t="s">
         <v>940</v>
       </c>
       <c r="E20" t="s">
@@ -12394,14 +12435,14 @@
         <v>967</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
       <c r="C21" s="111" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="153" t="s">
         <v>941</v>
       </c>
       <c r="E21" t="s">
@@ -12420,14 +12461,14 @@
         <v>968</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
       <c r="C22" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="153" t="s">
         <v>942</v>
       </c>
       <c r="E22" t="s">
@@ -12449,14 +12490,14 @@
         <v>969</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
       <c r="C23" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="153" t="s">
         <v>943</v>
       </c>
       <c r="E23" t="s">
@@ -12478,14 +12519,14 @@
         <v>970</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
       <c r="C24" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="153" t="s">
         <v>944</v>
       </c>
       <c r="E24" t="s">
@@ -12504,14 +12545,14 @@
         <v>971</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
       <c r="C25" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="153" t="s">
         <v>945</v>
       </c>
       <c r="E25" t="s">
@@ -12530,14 +12571,14 @@
         <v>972</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
       <c r="C26" s="104" t="s">
         <v>201</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="153" t="s">
         <v>946</v>
       </c>
       <c r="E26" t="s">
@@ -12559,14 +12600,14 @@
         <v>973</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="153" t="s">
         <v>947</v>
       </c>
       <c r="E27" t="s">
@@ -12588,14 +12629,14 @@
         <v>974</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
       <c r="C28" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="153" t="s">
         <v>948</v>
       </c>
       <c r="E28" t="s">
@@ -12614,14 +12655,14 @@
         <v>975</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="153" t="s">
         <v>949</v>
       </c>
       <c r="E29" t="s">
@@ -12640,14 +12681,14 @@
         <v>976</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
       <c r="C30" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="153" t="s">
         <v>950</v>
       </c>
       <c r="E30" t="s">
@@ -12666,14 +12707,14 @@
         <v>977</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
       <c r="C31" s="104" t="s">
         <v>206</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="153" t="s">
         <v>951</v>
       </c>
       <c r="E31" s="18" t="s">
@@ -12695,14 +12736,14 @@
         <v>978</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
       <c r="C32" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="153" t="s">
         <v>952</v>
       </c>
       <c r="E32" t="s">
@@ -12724,7 +12765,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>30</v>
       </c>
@@ -12734,7 +12775,7 @@
       <c r="C33" s="110" t="s">
         <v>208</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="153" t="s">
         <v>953</v>
       </c>
       <c r="J33" s="16" t="s">
@@ -12749,6 +12790,7 @@
       <c r="C45" s="109" t="s">
         <v>544</v>
       </c>
+      <c r="D45" s="156"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   01-11-2021 - 11:09:29.15
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16843174-673E-433E-9773-C6FFBCB2E93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BDCBAF-216A-404F-A7AF-C97C91B6B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="981">
   <si>
     <t>TOPIC</t>
   </si>
@@ -6777,7 +6777,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -8686,8 +8686,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8784,9 +8784,6 @@
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
-        <v>5</v>
-      </c>
       <c r="G5" s="10" t="s">
         <v>296</v>
       </c>
@@ -8817,9 +8814,6 @@
       <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
       <c r="G6" s="10" t="s">
         <v>299</v>
       </c>
@@ -8850,9 +8844,6 @@
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
       <c r="G7" s="10" t="s">
         <v>303</v>
       </c>
@@ -8883,9 +8874,6 @@
       <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
       <c r="H8" s="10" t="s">
         <v>305</v>
       </c>
@@ -8916,9 +8904,6 @@
       <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
       <c r="H9" s="10" t="s">
         <v>307</v>
       </c>
@@ -8947,9 +8932,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="57"/>
-      <c r="F10" s="58">
-        <v>5</v>
-      </c>
+      <c r="F10" s="58"/>
       <c r="H10" s="10" t="s">
         <v>316</v>
       </c>
@@ -8977,9 +8960,6 @@
       <c r="D11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="2">
-        <v>3</v>
-      </c>
       <c r="G11" s="10" t="s">
         <v>333</v>
       </c>
@@ -9013,9 +8993,6 @@
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
       <c r="G12" s="10" t="s">
         <v>331</v>
       </c>
@@ -9046,9 +9023,6 @@
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
       <c r="G13" s="10" t="s">
         <v>332</v>
       </c>
@@ -9080,9 +9054,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="57"/>
-      <c r="F14" s="58">
-        <v>3</v>
-      </c>
+      <c r="F14" s="58"/>
       <c r="G14" s="10" t="s">
         <v>334</v>
       </c>
@@ -9113,9 +9085,6 @@
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="2">
-        <v>3</v>
-      </c>
       <c r="H15" s="10" t="s">
         <v>366</v>
       </c>
@@ -9146,9 +9115,6 @@
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="2">
-        <v>3</v>
-      </c>
       <c r="G16" s="10" t="s">
         <v>368</v>
       </c>
@@ -9176,9 +9142,6 @@
       <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="2">
-        <v>3</v>
-      </c>
       <c r="H17" s="10" t="s">
         <v>369</v>
       </c>
@@ -9206,9 +9169,6 @@
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="2">
-        <v>3</v>
-      </c>
       <c r="G18" s="10" t="s">
         <v>370</v>
       </c>
@@ -9236,9 +9196,6 @@
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="2">
-        <v>3</v>
-      </c>
       <c r="J19" s="16" t="s">
         <v>396</v>
       </c>
@@ -9263,9 +9220,6 @@
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2">
-        <v>3</v>
-      </c>
       <c r="G20" s="10" t="s">
         <v>399</v>
       </c>
@@ -9300,9 +9254,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="54"/>
-      <c r="F21" s="55">
-        <v>3</v>
-      </c>
+      <c r="F21" s="55"/>
       <c r="H21" s="10" t="s">
         <v>372</v>
       </c>
@@ -9807,7 +9759,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F4" sqref="F4:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9887,9 +9839,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="10" t="s">
         <v>411</v>
       </c>
@@ -9947,9 +9897,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
@@ -9978,9 +9926,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
@@ -10009,9 +9955,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="11"/>
@@ -10040,9 +9984,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="11"/>
@@ -10071,9 +10013,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="10"/>
       <c r="H10" s="65" t="s">
         <v>412</v>
@@ -10791,7 +10731,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10871,9 +10811,7 @@
       <c r="F7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="30" t="s">
-        <v>455</v>
-      </c>
+      <c r="G7" s="30"/>
       <c r="H7" s="27" t="s">
         <v>10</v>
       </c>
@@ -10905,9 +10843,6 @@
       <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="5">
-        <v>3</v>
-      </c>
       <c r="K9" s="16" t="s">
         <v>416</v>
       </c>
@@ -10932,9 +10867,6 @@
       <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="5">
-        <v>3</v>
-      </c>
       <c r="K10" s="16" t="s">
         <v>416</v>
       </c>
@@ -10959,9 +10891,6 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="5">
-        <v>3</v>
-      </c>
       <c r="K11" s="16" t="s">
         <v>416</v>
       </c>
@@ -10986,9 +10915,6 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="5">
-        <v>3</v>
-      </c>
       <c r="K12" s="16" t="s">
         <v>416</v>
       </c>
@@ -11013,9 +10939,6 @@
       <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="5">
-        <v>3</v>
-      </c>
       <c r="K13" s="16" t="s">
         <v>416</v>
       </c>
@@ -11040,9 +10963,6 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="5">
-        <v>3</v>
-      </c>
       <c r="K14" s="16" t="s">
         <v>416</v>
       </c>
@@ -11067,9 +10987,6 @@
       <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="5">
-        <v>3</v>
-      </c>
       <c r="K15" s="16" t="s">
         <v>416</v>
       </c>
@@ -11094,9 +11011,6 @@
       <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="5">
-        <v>3</v>
-      </c>
       <c r="K16" s="16" t="s">
         <v>416</v>
       </c>
@@ -11121,9 +11035,6 @@
       <c r="E17" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="5">
-        <v>3</v>
-      </c>
       <c r="H17" s="18" t="s">
         <v>433</v>
       </c>
@@ -11154,9 +11065,6 @@
       <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="5">
-        <v>3</v>
-      </c>
       <c r="H18" s="18" t="s">
         <v>436</v>
       </c>
@@ -11184,9 +11092,6 @@
       <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="5">
-        <v>3</v>
-      </c>
       <c r="H19" s="18" t="s">
         <v>434</v>
       </c>
@@ -11214,9 +11119,6 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="5">
-        <v>3</v>
-      </c>
       <c r="H20" s="18" t="s">
         <v>435</v>
       </c>
@@ -11244,9 +11146,6 @@
       <c r="E21" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="5">
-        <v>3</v>
-      </c>
       <c r="H21" s="18" t="s">
         <v>438</v>
       </c>
@@ -11274,9 +11173,6 @@
       <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="5">
-        <v>3</v>
-      </c>
       <c r="H22" s="18" t="s">
         <v>437</v>
       </c>
@@ -11304,9 +11200,6 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="5">
-        <v>3</v>
-      </c>
       <c r="H23" s="16" t="s">
         <v>465</v>
       </c>
@@ -11340,9 +11233,6 @@
       <c r="E24" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="5">
-        <v>3</v>
-      </c>
       <c r="K24" s="16" t="s">
         <v>468</v>
       </c>
@@ -11367,9 +11257,6 @@
       <c r="E25" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="5">
-        <v>3</v>
-      </c>
       <c r="H25" s="16" t="s">
         <v>469</v>
       </c>
@@ -11397,9 +11284,6 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="5">
-        <v>3</v>
-      </c>
       <c r="K26" s="16" t="s">
         <v>481</v>
       </c>
@@ -11424,9 +11308,6 @@
       <c r="E27" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="5">
-        <v>3</v>
-      </c>
       <c r="K27" s="16" t="s">
         <v>489</v>
       </c>
@@ -11451,9 +11332,6 @@
       <c r="E28" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="5">
-        <v>3</v>
-      </c>
       <c r="K28" s="16" t="s">
         <v>499</v>
       </c>
@@ -11478,9 +11356,6 @@
       <c r="E29" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="5">
-        <v>3</v>
-      </c>
       <c r="K29" s="16" t="s">
         <v>500</v>
       </c>
@@ -11505,9 +11380,6 @@
       <c r="E30" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="5">
-        <v>3</v>
-      </c>
       <c r="H30" s="18" t="s">
         <v>490</v>
       </c>
@@ -11535,9 +11407,6 @@
       <c r="E31" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="5">
-        <v>3</v>
-      </c>
       <c r="H31" s="18" t="s">
         <v>502</v>
       </c>
@@ -11571,9 +11440,6 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="5">
-        <v>3</v>
-      </c>
       <c r="H32" s="18" t="s">
         <v>509</v>
       </c>
@@ -11604,9 +11470,6 @@
       <c r="E33" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="5">
-        <v>3</v>
-      </c>
       <c r="H33" s="10" t="s">
         <v>516</v>
       </c>
@@ -11636,9 +11499,6 @@
       </c>
       <c r="E34" t="s">
         <v>5</v>
-      </c>
-      <c r="G34" s="5">
-        <v>3</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>517</v>
@@ -11673,9 +11533,6 @@
       <c r="F38" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C39" s="16" t="s">
@@ -11691,9 +11548,6 @@
       <c r="F40" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C41" s="16" t="s">
@@ -11703,9 +11557,6 @@
       <c r="F41" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C42" s="16" t="s">
@@ -11715,9 +11566,6 @@
       <c r="F42" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C43" s="16" t="s">
@@ -11727,9 +11575,6 @@
       <c r="F43" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
       <c r="H43" s="16" t="s">
         <v>480</v>
       </c>
@@ -11743,9 +11588,6 @@
       <c r="F44" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C45" s="16" t="s">
@@ -11755,9 +11597,6 @@
       <c r="F45" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C46" s="16" t="s">
@@ -11767,9 +11606,6 @@
       <c r="F46" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
@@ -11779,9 +11615,6 @@
         <v>471</v>
       </c>
       <c r="D47" s="163"/>
-      <c r="G47" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
@@ -11791,20 +11624,14 @@
       <c r="F48" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="16" t="s">
         <v>506</v>
       </c>
       <c r="D49" s="163"/>
       <c r="F49" t="s">
         <v>6</v>
-      </c>
-      <c r="G49" s="5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11916,7 +11743,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11962,9 +11789,7 @@
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>455</v>
-      </c>
+      <c r="F3" s="30"/>
       <c r="G3" s="27" t="s">
         <v>10</v>
       </c>
@@ -12033,9 +11858,7 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="89">
-        <v>3</v>
-      </c>
+      <c r="F6" s="89"/>
       <c r="G6" s="94" t="s">
         <v>527</v>
       </c>
@@ -12065,9 +11888,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="89">
-        <v>3</v>
-      </c>
+      <c r="F7" s="89"/>
       <c r="G7" t="s">
         <v>463</v>
       </c>
@@ -12094,9 +11915,7 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="89">
-        <v>3</v>
-      </c>
+      <c r="F8" s="89"/>
       <c r="G8" t="s">
         <v>463</v>
       </c>
@@ -12123,9 +11942,7 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="89">
-        <v>3</v>
-      </c>
+      <c r="F9" s="89"/>
       <c r="G9" t="s">
         <v>463</v>
       </c>
@@ -12152,9 +11969,7 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="89">
-        <v>3</v>
-      </c>
+      <c r="F10" s="89"/>
       <c r="G10" s="96" t="s">
         <v>463</v>
       </c>
@@ -12184,9 +11999,7 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="89">
-        <v>3</v>
-      </c>
+      <c r="F11" s="89"/>
       <c r="G11" s="95" t="s">
         <v>534</v>
       </c>
@@ -12219,9 +12032,7 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="89">
-        <v>3</v>
-      </c>
+      <c r="F12" s="89"/>
       <c r="G12" t="s">
         <v>535</v>
       </c>
@@ -12251,9 +12062,7 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="89">
-        <v>3</v>
-      </c>
+      <c r="F13" s="89"/>
       <c r="G13" t="s">
         <v>543</v>
       </c>
@@ -12280,9 +12089,7 @@
       <c r="D14" s="153" t="s">
         <v>934</v>
       </c>
-      <c r="F14" s="89">
-        <v>3</v>
-      </c>
+      <c r="F14" s="89"/>
       <c r="G14" s="18"/>
       <c r="J14" s="16" t="s">
         <v>531</v>
@@ -12304,9 +12111,7 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="89">
-        <v>3</v>
-      </c>
+      <c r="F15" s="89"/>
       <c r="J15" s="16" t="s">
         <v>587</v>
       </c>
@@ -12327,9 +12132,7 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="89">
-        <v>3</v>
-      </c>
+      <c r="F16" s="89"/>
       <c r="J16" s="16" t="s">
         <v>602</v>
       </c>
@@ -12350,9 +12153,7 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="89">
-        <v>3</v>
-      </c>
+      <c r="F17" s="89"/>
       <c r="J17" s="16" t="s">
         <v>603</v>
       </c>
@@ -12373,9 +12174,7 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="89">
-        <v>3</v>
-      </c>
+      <c r="F18" s="89"/>
       <c r="J18" s="16" t="s">
         <v>603</v>
       </c>
@@ -12396,9 +12195,7 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="89">
-        <v>3</v>
-      </c>
+      <c r="F19" s="89"/>
       <c r="G19" t="s">
         <v>565</v>
       </c>
@@ -12422,9 +12219,7 @@
       <c r="E20" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="89">
-        <v>3</v>
-      </c>
+      <c r="F20" s="89"/>
       <c r="G20" t="s">
         <v>566</v>
       </c>
@@ -12448,9 +12243,7 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="89">
-        <v>3</v>
-      </c>
+      <c r="F21" s="89"/>
       <c r="G21" t="s">
         <v>567</v>
       </c>
@@ -12474,9 +12267,7 @@
       <c r="E22" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="89">
-        <v>3</v>
-      </c>
+      <c r="F22" s="89"/>
       <c r="G22" t="s">
         <v>568</v>
       </c>
@@ -12503,9 +12294,7 @@
       <c r="E23" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="89">
-        <v>3</v>
-      </c>
+      <c r="F23" s="89"/>
       <c r="G23" t="s">
         <v>546</v>
       </c>
@@ -12532,9 +12321,7 @@
       <c r="E24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="89">
-        <v>3</v>
-      </c>
+      <c r="F24" s="89"/>
       <c r="G24" t="s">
         <v>547</v>
       </c>
@@ -12558,9 +12345,7 @@
       <c r="E25" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="89">
-        <v>3</v>
-      </c>
+      <c r="F25" s="89"/>
       <c r="G25" t="s">
         <v>548</v>
       </c>
@@ -12584,9 +12369,7 @@
       <c r="E26" t="s">
         <v>606</v>
       </c>
-      <c r="F26" s="89">
-        <v>3</v>
-      </c>
+      <c r="F26" s="89"/>
       <c r="G26" t="s">
         <v>549</v>
       </c>
@@ -12613,9 +12396,7 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="89">
-        <v>3</v>
-      </c>
+      <c r="F27" s="89"/>
       <c r="G27" s="18" t="s">
         <v>550</v>
       </c>
@@ -12642,9 +12423,7 @@
       <c r="E28" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="89">
-        <v>3</v>
-      </c>
+      <c r="F28" s="89"/>
       <c r="G28" s="18" t="s">
         <v>552</v>
       </c>
@@ -12668,9 +12447,7 @@
       <c r="E29" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="89">
-        <v>3</v>
-      </c>
+      <c r="F29" s="89"/>
       <c r="G29" t="s">
         <v>553</v>
       </c>
@@ -12694,9 +12471,7 @@
       <c r="E30" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="89">
-        <v>3</v>
-      </c>
+      <c r="F30" s="89"/>
       <c r="G30" s="18" t="s">
         <v>554</v>
       </c>
@@ -12720,9 +12495,7 @@
       <c r="E31" s="18" t="s">
         <v>604</v>
       </c>
-      <c r="F31" s="89">
-        <v>3</v>
-      </c>
+      <c r="F31" s="89"/>
       <c r="G31" s="18" t="s">
         <v>555</v>
       </c>
@@ -12749,9 +12522,7 @@
       <c r="E32" t="s">
         <v>605</v>
       </c>
-      <c r="F32" s="89">
-        <v>3</v>
-      </c>
+      <c r="F32" s="89"/>
       <c r="G32" s="18" t="s">
         <v>556</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   02-11-2021 - 11:40:03.94
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BDCBAF-216A-404F-A7AF-C97C91B6B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D9244-587C-4EBC-BFEF-87C82CE1C43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -3192,12 +3192,6 @@
     <t>https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/two-stacks-official/ojquestion</t>
   </si>
   <si>
-    <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java</t>
-  </si>
-  <si>
-    <t>https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java</t>
-  </si>
-  <si>
     <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java</t>
   </si>
   <si>
@@ -3520,6 +3514,12 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=t4IKNhNBTdo&amp;list=TLGGXv0lFdWAQ5EyMzA5MjAyMQ</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java</t>
+  </si>
+  <si>
+    <t>https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java</t>
   </si>
 </sst>
 </file>
@@ -4429,77 +4429,77 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="16" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="14" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="17" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="15" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="14" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="17" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="15" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="fill" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -4912,10 +4912,10 @@
       <c r="C2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="151"/>
+      <c r="G2" s="173"/>
       <c r="J2" s="90" t="s">
         <v>294</v>
       </c>
@@ -6787,7 +6787,7 @@
     <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="4" style="8" customWidth="1"/>
     <col min="4" max="4" width="40.85546875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="174" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="172" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
@@ -6803,7 +6803,7 @@
       <c r="D1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="154"/>
+      <c r="E1" s="152"/>
       <c r="F1" s="16" t="s">
         <v>86</v>
       </c>
@@ -6816,7 +6816,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" s="8"/>
-      <c r="E2" s="154"/>
+      <c r="E2" s="152"/>
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6832,7 +6832,7 @@
       <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="166"/>
+      <c r="E3" s="164"/>
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6868,7 +6868,7 @@
       <c r="D4" s="145" t="s">
         <v>801</v>
       </c>
-      <c r="E4" s="167" t="s">
+      <c r="E4" s="165" t="s">
         <v>800</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -6907,7 +6907,7 @@
       <c r="D5" s="140" t="s">
         <v>738</v>
       </c>
-      <c r="E5" s="168" t="s">
+      <c r="E5" s="166" t="s">
         <v>802</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -6946,7 +6946,7 @@
       <c r="D6" s="140" t="s">
         <v>739</v>
       </c>
-      <c r="E6" s="168" t="s">
+      <c r="E6" s="166" t="s">
         <v>803</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -6985,7 +6985,7 @@
       <c r="D7" s="140" t="s">
         <v>740</v>
       </c>
-      <c r="E7" s="168" t="s">
+      <c r="E7" s="166" t="s">
         <v>804</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -7024,7 +7024,7 @@
       <c r="D8" s="140" t="s">
         <v>741</v>
       </c>
-      <c r="E8" s="168" t="s">
+      <c r="E8" s="166" t="s">
         <v>805</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -7060,7 +7060,7 @@
       <c r="D9" s="140" t="s">
         <v>742</v>
       </c>
-      <c r="E9" s="168" t="s">
+      <c r="E9" s="166" t="s">
         <v>806</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -7096,7 +7096,7 @@
       <c r="D10" s="140" t="s">
         <v>743</v>
       </c>
-      <c r="E10" s="168" t="s">
+      <c r="E10" s="166" t="s">
         <v>807</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -7138,7 +7138,7 @@
       <c r="D11" s="140" t="s">
         <v>744</v>
       </c>
-      <c r="E11" s="168" t="s">
+      <c r="E11" s="166" t="s">
         <v>808</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -7180,7 +7180,7 @@
       <c r="D12" s="141" t="s">
         <v>776</v>
       </c>
-      <c r="E12" s="169" t="s">
+      <c r="E12" s="167" t="s">
         <v>809</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -7216,7 +7216,7 @@
       <c r="D13" s="141" t="s">
         <v>777</v>
       </c>
-      <c r="E13" s="169" t="s">
+      <c r="E13" s="167" t="s">
         <v>810</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -7255,7 +7255,7 @@
       <c r="D14" s="141" t="s">
         <v>778</v>
       </c>
-      <c r="E14" s="169" t="s">
+      <c r="E14" s="167" t="s">
         <v>811</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -7294,7 +7294,7 @@
       <c r="D15" s="141" t="s">
         <v>779</v>
       </c>
-      <c r="E15" s="169" t="s">
+      <c r="E15" s="167" t="s">
         <v>812</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -7327,7 +7327,7 @@
       <c r="D16" s="141" t="s">
         <v>780</v>
       </c>
-      <c r="E16" s="169" t="s">
+      <c r="E16" s="167" t="s">
         <v>813</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -7360,7 +7360,7 @@
       <c r="D17" s="141" t="s">
         <v>781</v>
       </c>
-      <c r="E17" s="169" t="s">
+      <c r="E17" s="167" t="s">
         <v>814</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -7396,7 +7396,7 @@
       <c r="D18" s="143" t="s">
         <v>782</v>
       </c>
-      <c r="E18" s="170" t="s">
+      <c r="E18" s="168" t="s">
         <v>815</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -7432,7 +7432,7 @@
       <c r="D19" s="143" t="s">
         <v>783</v>
       </c>
-      <c r="E19" s="170" t="s">
+      <c r="E19" s="168" t="s">
         <v>816</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -7465,7 +7465,7 @@
       <c r="D20" s="143" t="s">
         <v>784</v>
       </c>
-      <c r="E20" s="170" t="s">
+      <c r="E20" s="168" t="s">
         <v>817</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -7498,7 +7498,7 @@
       <c r="D21" s="143" t="s">
         <v>785</v>
       </c>
-      <c r="E21" s="170" t="s">
+      <c r="E21" s="168" t="s">
         <v>818</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -7531,7 +7531,7 @@
       <c r="D22" s="143" t="s">
         <v>786</v>
       </c>
-      <c r="E22" s="170" t="s">
+      <c r="E22" s="168" t="s">
         <v>819</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -7564,7 +7564,7 @@
       <c r="D23" s="142" t="s">
         <v>787</v>
       </c>
-      <c r="E23" s="171" t="s">
+      <c r="E23" s="169" t="s">
         <v>820</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -7603,7 +7603,7 @@
       <c r="D24" s="142" t="s">
         <v>788</v>
       </c>
-      <c r="E24" s="171" t="s">
+      <c r="E24" s="169" t="s">
         <v>821</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -7642,7 +7642,7 @@
       <c r="D25" s="142" t="s">
         <v>789</v>
       </c>
-      <c r="E25" s="171" t="s">
+      <c r="E25" s="169" t="s">
         <v>822</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -7678,7 +7678,7 @@
       <c r="D26" s="142" t="s">
         <v>790</v>
       </c>
-      <c r="E26" s="171" t="s">
+      <c r="E26" s="169" t="s">
         <v>823</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -7714,7 +7714,7 @@
       <c r="D27" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="E27" s="171" t="s">
+      <c r="E27" s="169" t="s">
         <v>824</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -7753,7 +7753,7 @@
       <c r="D28" s="142" t="s">
         <v>792</v>
       </c>
-      <c r="E28" s="171" t="s">
+      <c r="E28" s="169" t="s">
         <v>825</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -7789,7 +7789,7 @@
       <c r="D29" s="142" t="s">
         <v>793</v>
       </c>
-      <c r="E29" s="171" t="s">
+      <c r="E29" s="169" t="s">
         <v>826</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -7828,7 +7828,7 @@
       <c r="D30" s="144" t="s">
         <v>794</v>
       </c>
-      <c r="E30" s="172" t="s">
+      <c r="E30" s="170" t="s">
         <v>827</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7867,7 +7867,7 @@
       <c r="D31" s="144" t="s">
         <v>795</v>
       </c>
-      <c r="E31" s="172" t="s">
+      <c r="E31" s="170" t="s">
         <v>828</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -7906,7 +7906,7 @@
       <c r="D32" s="144" t="s">
         <v>796</v>
       </c>
-      <c r="E32" s="172" t="s">
+      <c r="E32" s="170" t="s">
         <v>829</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -7939,7 +7939,7 @@
       <c r="D33" s="144" t="s">
         <v>797</v>
       </c>
-      <c r="E33" s="172" t="s">
+      <c r="E33" s="170" t="s">
         <v>829</v>
       </c>
       <c r="H33" s="2">
@@ -7969,7 +7969,7 @@
       <c r="D34" s="144" t="s">
         <v>799</v>
       </c>
-      <c r="E34" s="172" t="s">
+      <c r="E34" s="170" t="s">
         <v>798</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -8000,22 +8000,22 @@
     </row>
     <row r="35" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D35" s="16"/>
-      <c r="E35" s="163"/>
+      <c r="E35" s="161"/>
       <c r="L35" s="16"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D36" s="16"/>
-      <c r="E36" s="163"/>
+      <c r="E36" s="161"/>
       <c r="L36" s="16"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D37" s="67"/>
-      <c r="E37" s="173"/>
+      <c r="E37" s="171"/>
       <c r="L37" s="16"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D38" s="16"/>
-      <c r="E38" s="163"/>
+      <c r="E38" s="161"/>
       <c r="L38" s="16"/>
     </row>
   </sheetData>
@@ -8686,7 +8686,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F5" sqref="F5:F21"/>
     </sheetView>
   </sheetViews>
@@ -8694,7 +8694,7 @@
   <cols>
     <col min="1" max="1" width="6.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="52.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="154" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="152" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
@@ -8722,7 +8722,7 @@
       <c r="B2" s="106" t="s">
         <v>542</v>
       </c>
-      <c r="C2" s="164"/>
+      <c r="C2" s="162"/>
       <c r="D2" s="16"/>
       <c r="H2" s="16"/>
       <c r="J2"/>
@@ -8732,7 +8732,7 @@
       <c r="B3" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="165"/>
+      <c r="C3" s="163"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="34"/>
@@ -8748,7 +8748,7 @@
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="166"/>
+      <c r="C4" s="164"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -8778,7 +8778,7 @@
       <c r="B5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="151" t="s">
         <v>847</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -8808,7 +8808,7 @@
       <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="151" t="s">
         <v>848</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -8838,7 +8838,7 @@
       <c r="B7" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="151" t="s">
         <v>849</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -8868,7 +8868,7 @@
       <c r="B8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="153" t="s">
+      <c r="C8" s="151" t="s">
         <v>850</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -8898,7 +8898,7 @@
       <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="151" t="s">
         <v>851</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -8925,7 +8925,7 @@
       <c r="B10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="153" t="s">
+      <c r="C10" s="151" t="s">
         <v>852</v>
       </c>
       <c r="D10" s="56" t="s">
@@ -8954,7 +8954,7 @@
       <c r="B11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="153" t="s">
+      <c r="C11" s="151" t="s">
         <v>853</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -8987,7 +8987,7 @@
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="153" t="s">
+      <c r="C12" s="151" t="s">
         <v>854</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -9017,7 +9017,7 @@
       <c r="B13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="153" t="s">
+      <c r="C13" s="151" t="s">
         <v>855</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -9047,7 +9047,7 @@
       <c r="B14" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="153" t="s">
+      <c r="C14" s="151" t="s">
         <v>856</v>
       </c>
       <c r="D14" s="56" t="s">
@@ -9079,7 +9079,7 @@
       <c r="B15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="153" t="s">
+      <c r="C15" s="151" t="s">
         <v>857</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -9109,7 +9109,7 @@
       <c r="B16" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="153" t="s">
+      <c r="C16" s="151" t="s">
         <v>858</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -9136,7 +9136,7 @@
       <c r="B17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="153" t="s">
+      <c r="C17" s="151" t="s">
         <v>859</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -9163,7 +9163,7 @@
       <c r="B18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="153" t="s">
+      <c r="C18" s="151" t="s">
         <v>860</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -9190,7 +9190,7 @@
       <c r="B19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="153" t="s">
+      <c r="C19" s="151" t="s">
         <v>861</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -9214,7 +9214,7 @@
       <c r="B20" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="153" t="s">
+      <c r="C20" s="151" t="s">
         <v>862</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -9247,7 +9247,7 @@
       <c r="B21" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="153" t="s">
+      <c r="C21" s="151" t="s">
         <v>863</v>
       </c>
       <c r="D21" s="53" t="s">
@@ -9270,44 +9270,44 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="153"/>
+      <c r="C22" s="151"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="153"/>
+      <c r="C23" s="151"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="153"/>
+      <c r="C24" s="151"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="153"/>
+      <c r="C25" s="151"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="153"/>
+      <c r="C26" s="151"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="153"/>
+      <c r="C27" s="151"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="153"/>
+      <c r="C28" s="151"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
-      <c r="C30" s="160"/>
+      <c r="C30" s="158"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
-      <c r="C31" s="160"/>
+      <c r="C31" s="158"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
-      <c r="C32" s="160"/>
+      <c r="C32" s="158"/>
     </row>
     <row r="33" spans="1:10" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C33" s="165"/>
+      <c r="C33" s="163"/>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="34"/>
@@ -9323,7 +9323,7 @@
       <c r="B34" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="C34" s="153"/>
+      <c r="C34" s="151"/>
       <c r="D34" s="5" t="s">
         <v>177</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="B35" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="153"/>
+      <c r="C35" s="151"/>
       <c r="D35" s="5" t="s">
         <v>177</v>
       </c>
@@ -9370,7 +9370,7 @@
       <c r="B36" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="C36" s="153"/>
+      <c r="C36" s="151"/>
       <c r="D36" s="5" t="s">
         <v>5</v>
       </c>
@@ -9392,7 +9392,7 @@
       <c r="B37" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C37" s="153"/>
+      <c r="C37" s="151"/>
       <c r="D37" s="5" t="s">
         <v>322</v>
       </c>
@@ -9418,7 +9418,7 @@
       <c r="B38" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="153"/>
+      <c r="C38" s="151"/>
       <c r="D38" s="5" t="s">
         <v>322</v>
       </c>
@@ -9441,7 +9441,7 @@
       <c r="B39" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="C39" s="153"/>
+      <c r="C39" s="151"/>
       <c r="D39" s="5" t="s">
         <v>322</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="B40" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="C40" s="153"/>
+      <c r="C40" s="151"/>
       <c r="D40" s="5" t="s">
         <v>177</v>
       </c>
@@ -9488,7 +9488,7 @@
       <c r="B41" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="153"/>
+      <c r="C41" s="151"/>
       <c r="D41" s="5" t="s">
         <v>322</v>
       </c>
@@ -9513,7 +9513,7 @@
       <c r="B42" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="C42" s="153"/>
+      <c r="C42" s="151"/>
       <c r="D42" s="5" t="s">
         <v>322</v>
       </c>
@@ -9538,7 +9538,7 @@
       <c r="B43" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="C43" s="153"/>
+      <c r="C43" s="151"/>
       <c r="D43" s="5" t="s">
         <v>177</v>
       </c>
@@ -9563,7 +9563,7 @@
       <c r="B44" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="C44" s="153"/>
+      <c r="C44" s="151"/>
       <c r="D44" s="5" t="s">
         <v>177</v>
       </c>
@@ -9591,7 +9591,7 @@
       <c r="B45" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="C45" s="153"/>
+      <c r="C45" s="151"/>
       <c r="D45" s="5" t="s">
         <v>177</v>
       </c>
@@ -9619,7 +9619,7 @@
       <c r="B46" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="C46" s="163"/>
+      <c r="C46" s="161"/>
       <c r="D46" s="5" t="s">
         <v>5</v>
       </c>
@@ -9644,7 +9644,7 @@
       <c r="B47" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="C47" s="163"/>
+      <c r="C47" s="161"/>
       <c r="I47" s="10" t="s">
         <v>363</v>
       </c>
@@ -9653,25 +9653,25 @@
       <c r="B48" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="C48" s="163"/>
+      <c r="C48" s="161"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="C49" s="163"/>
+      <c r="C49" s="161"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="C50" s="163"/>
+      <c r="C50" s="161"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="C51" s="163"/>
+      <c r="C51" s="161"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9758,14 +9758,14 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F10"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.42578125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="154" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="152" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
     <col min="8" max="8" width="49.42578125" customWidth="1"/>
@@ -9783,16 +9783,16 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:12" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="174" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
       <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:12" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9802,7 +9802,7 @@
       <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="159"/>
+      <c r="C3" s="157"/>
       <c r="D3" s="28" t="s">
         <v>1</v>
       </c>
@@ -9832,7 +9832,7 @@
       <c r="B4" s="64" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="C4" s="159" t="s">
         <v>864</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -9849,11 +9849,11 @@
         <v>382</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>871</v>
+        <v>979</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",B4,"](",C4,")|[Solution](",K4,")|")</f>
-        <v>|[Normal queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java)|</v>
+        <v>|[Normal queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/normal-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java)|</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -9863,7 +9863,7 @@
       <c r="B5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="161" t="s">
+      <c r="C5" s="159" t="s">
         <v>865</v>
       </c>
       <c r="D5" s="5"/>
@@ -9876,11 +9876,11 @@
         <v>381</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>872</v>
+        <v>980</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L11" si="0">CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
-        <v>|[Dynamic Queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java)|</v>
+        <v>|[Dynamic Queue](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/stacks-and-queues/dynamic-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java)|</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -9890,7 +9890,7 @@
       <c r="B6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="161" t="s">
+      <c r="C6" s="159" t="s">
         <v>866</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -9905,7 +9905,7 @@
         <v>407</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -9919,7 +9919,7 @@
       <c r="B7" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="161" t="s">
+      <c r="C7" s="159" t="s">
         <v>867</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -9934,7 +9934,7 @@
         <v>406</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -9948,7 +9948,7 @@
       <c r="B8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="161" t="s">
+      <c r="C8" s="159" t="s">
         <v>868</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -9963,7 +9963,7 @@
         <v>410</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -9977,7 +9977,7 @@
       <c r="B9" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="161" t="s">
+      <c r="C9" s="159" t="s">
         <v>869</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -9992,7 +9992,7 @@
         <v>409</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -10006,7 +10006,7 @@
       <c r="B10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="161" t="s">
+      <c r="C10" s="159" t="s">
         <v>870</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -10023,7 +10023,7 @@
         <v>408</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -10037,7 +10037,7 @@
       <c r="B11" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="153"/>
+      <c r="C11" s="151"/>
       <c r="D11" s="5" t="s">
         <v>374</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>377</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -10067,13 +10067,13 @@
       <c r="B14" s="16" t="s">
         <v>413</v>
       </c>
-      <c r="C14" s="163"/>
+      <c r="C14" s="161"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="C15" s="163"/>
+      <c r="C15" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10082,8 +10082,8 @@
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://auth.geeksforgeeks.org/?to=https%3A%2F%2Fpractice.geeksforgeeks.org%2Fproblems%2Fgenerate-binary-numbers-1587115620%2F1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
     <hyperlink ref="D1" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="J5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="J4" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
     <hyperlink ref="J11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
     <hyperlink ref="J7" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
     <hyperlink ref="J6" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
@@ -10739,7 +10739,7 @@
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="160" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="158" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="56" customWidth="1"/>
@@ -10753,7 +10753,7 @@
       <c r="C1" s="87" t="s">
         <v>511</v>
       </c>
-      <c r="D1" s="157"/>
+      <c r="D1" s="155"/>
       <c r="E1" s="5">
         <v>0</v>
       </c>
@@ -10764,7 +10764,7 @@
       <c r="C2" s="88" t="s">
         <v>512</v>
       </c>
-      <c r="D2" s="158"/>
+      <c r="D2" s="156"/>
       <c r="E2" s="88" t="s">
         <v>513</v>
       </c>
@@ -10773,25 +10773,25 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="C3" s="87"/>
-      <c r="D3" s="157"/>
+      <c r="D3" s="155"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="C4" s="87"/>
-      <c r="D4" s="157"/>
+      <c r="D4" s="155"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="C5" s="87"/>
-      <c r="D5" s="157"/>
+      <c r="D5" s="155"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="C6" s="87"/>
-      <c r="D6" s="157"/>
+      <c r="D6" s="155"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10804,7 +10804,7 @@
       <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="159"/>
+      <c r="D7" s="157"/>
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
@@ -10837,8 +10837,8 @@
       <c r="C9" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="D9" s="161" t="s">
-        <v>879</v>
+      <c r="D9" s="159" t="s">
+        <v>877</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -10847,7 +10847,7 @@
         <v>416</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M9" t="str">
         <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",L9,")|")</f>
@@ -10861,8 +10861,8 @@
       <c r="C10" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="161" t="s">
-        <v>880</v>
+      <c r="D10" s="159" t="s">
+        <v>878</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -10871,7 +10871,7 @@
         <v>416</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ref="M10:M34" si="0">CONCATENATE("|[",C10,"](",D10,")|[Solution](",L10,")|")</f>
@@ -10885,8 +10885,8 @@
       <c r="C11" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="D11" s="161" t="s">
-        <v>881</v>
+      <c r="D11" s="159" t="s">
+        <v>879</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -10895,7 +10895,7 @@
         <v>416</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
@@ -10909,8 +10909,8 @@
       <c r="C12" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="161" t="s">
-        <v>882</v>
+      <c r="D12" s="159" t="s">
+        <v>880</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -10919,7 +10919,7 @@
         <v>416</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
@@ -10933,8 +10933,8 @@
       <c r="C13" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="D13" s="161" t="s">
-        <v>883</v>
+      <c r="D13" s="159" t="s">
+        <v>881</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -10943,7 +10943,7 @@
         <v>416</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
@@ -10957,8 +10957,8 @@
       <c r="C14" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="D14" s="161" t="s">
-        <v>884</v>
+      <c r="D14" s="159" t="s">
+        <v>882</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -10967,7 +10967,7 @@
         <v>416</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -10981,8 +10981,8 @@
       <c r="C15" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="161" t="s">
-        <v>885</v>
+      <c r="D15" s="159" t="s">
+        <v>883</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -10991,7 +10991,7 @@
         <v>416</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
@@ -11005,8 +11005,8 @@
       <c r="C16" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="D16" s="161" t="s">
-        <v>886</v>
+      <c r="D16" s="159" t="s">
+        <v>884</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -11015,7 +11015,7 @@
         <v>416</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -11029,8 +11029,8 @@
       <c r="C17" s="82" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="161" t="s">
-        <v>887</v>
+      <c r="D17" s="159" t="s">
+        <v>885</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -11045,7 +11045,7 @@
         <v>487</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -11059,8 +11059,8 @@
       <c r="C18" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="161" t="s">
-        <v>888</v>
+      <c r="D18" s="159" t="s">
+        <v>886</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -11072,7 +11072,7 @@
         <v>488</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -11086,8 +11086,8 @@
       <c r="C19" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="D19" s="161" t="s">
-        <v>889</v>
+      <c r="D19" s="159" t="s">
+        <v>887</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -11099,7 +11099,7 @@
         <v>483</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -11113,8 +11113,8 @@
       <c r="C20" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="161" t="s">
-        <v>890</v>
+      <c r="D20" s="159" t="s">
+        <v>888</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -11126,7 +11126,7 @@
         <v>484</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -11140,8 +11140,8 @@
       <c r="C21" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="161" t="s">
-        <v>891</v>
+      <c r="D21" s="159" t="s">
+        <v>889</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -11153,7 +11153,7 @@
         <v>485</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -11167,8 +11167,8 @@
       <c r="C22" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D22" s="161" t="s">
-        <v>892</v>
+      <c r="D22" s="159" t="s">
+        <v>890</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -11180,7 +11180,7 @@
         <v>486</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
@@ -11194,8 +11194,8 @@
       <c r="C23" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="D23" s="161" t="s">
-        <v>893</v>
+      <c r="D23" s="159" t="s">
+        <v>891</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -11213,7 +11213,7 @@
         <v>466</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -11227,8 +11227,8 @@
       <c r="C24" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="161" t="s">
-        <v>894</v>
+      <c r="D24" s="159" t="s">
+        <v>892</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -11237,7 +11237,7 @@
         <v>468</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
@@ -11251,8 +11251,8 @@
       <c r="C25" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D25" s="161" t="s">
-        <v>895</v>
+      <c r="D25" s="159" t="s">
+        <v>893</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -11264,7 +11264,7 @@
         <v>482</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
@@ -11278,8 +11278,8 @@
       <c r="C26" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="161" t="s">
-        <v>896</v>
+      <c r="D26" s="159" t="s">
+        <v>894</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -11288,7 +11288,7 @@
         <v>481</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
@@ -11302,8 +11302,8 @@
       <c r="C27" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="161" t="s">
-        <v>897</v>
+      <c r="D27" s="159" t="s">
+        <v>895</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -11312,7 +11312,7 @@
         <v>489</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
@@ -11326,8 +11326,8 @@
       <c r="C28" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="161" t="s">
-        <v>898</v>
+      <c r="D28" s="159" t="s">
+        <v>896</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
@@ -11336,7 +11336,7 @@
         <v>499</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
@@ -11350,8 +11350,8 @@
       <c r="C29" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="D29" s="161" t="s">
-        <v>899</v>
+      <c r="D29" s="159" t="s">
+        <v>897</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -11360,7 +11360,7 @@
         <v>500</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
@@ -11374,8 +11374,8 @@
       <c r="C30" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D30" s="161" t="s">
-        <v>900</v>
+      <c r="D30" s="159" t="s">
+        <v>898</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -11387,7 +11387,7 @@
         <v>501</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
@@ -11401,8 +11401,8 @@
       <c r="C31" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="161" t="s">
-        <v>901</v>
+      <c r="D31" s="159" t="s">
+        <v>899</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -11420,7 +11420,7 @@
         <v>503</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
@@ -11434,8 +11434,8 @@
       <c r="C32" s="91" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="161" t="s">
-        <v>902</v>
+      <c r="D32" s="159" t="s">
+        <v>900</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -11450,7 +11450,7 @@
         <v>515</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
@@ -11464,8 +11464,8 @@
       <c r="C33" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="161" t="s">
-        <v>903</v>
+      <c r="D33" s="159" t="s">
+        <v>901</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -11477,7 +11477,7 @@
         <v>519</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
@@ -11494,8 +11494,8 @@
       <c r="C34" s="86" t="s">
         <v>505</v>
       </c>
-      <c r="D34" s="161" t="s">
-        <v>904</v>
+      <c r="D34" s="159" t="s">
+        <v>902</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -11507,7 +11507,7 @@
         <v>520</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="0"/>
@@ -11522,14 +11522,14 @@
       <c r="C36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="D36" s="162"/>
+      <c r="D36" s="160"/>
       <c r="G36" s="78"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C38" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="D38" s="163"/>
+      <c r="D38" s="161"/>
       <c r="F38" t="s">
         <v>6</v>
       </c>
@@ -11538,13 +11538,13 @@
       <c r="C39" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="D39" s="163"/>
+      <c r="D39" s="161"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C40" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D40" s="163"/>
+      <c r="D40" s="161"/>
       <c r="F40" t="s">
         <v>6</v>
       </c>
@@ -11553,7 +11553,7 @@
       <c r="C41" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="D41" s="163"/>
+      <c r="D41" s="161"/>
       <c r="F41" t="s">
         <v>6</v>
       </c>
@@ -11562,7 +11562,7 @@
       <c r="C42" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="D42" s="163"/>
+      <c r="D42" s="161"/>
       <c r="F42" t="s">
         <v>6</v>
       </c>
@@ -11571,7 +11571,7 @@
       <c r="C43" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="D43" s="163"/>
+      <c r="D43" s="161"/>
       <c r="F43" t="s">
         <v>6</v>
       </c>
@@ -11584,7 +11584,7 @@
       <c r="C44" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="D44" s="163"/>
+      <c r="D44" s="161"/>
       <c r="F44" t="s">
         <v>6</v>
       </c>
@@ -11593,7 +11593,7 @@
       <c r="C45" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="D45" s="163"/>
+      <c r="D45" s="161"/>
       <c r="F45" t="s">
         <v>6</v>
       </c>
@@ -11602,7 +11602,7 @@
       <c r="C46" s="16" t="s">
         <v>470</v>
       </c>
-      <c r="D46" s="163"/>
+      <c r="D46" s="161"/>
       <c r="F46" t="s">
         <v>6</v>
       </c>
@@ -11614,13 +11614,13 @@
       <c r="C47" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="D47" s="163"/>
+      <c r="D47" s="161"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="D48" s="163"/>
+      <c r="D48" s="161"/>
       <c r="F48" t="s">
         <v>6</v>
       </c>
@@ -11629,7 +11629,7 @@
       <c r="C49" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="D49" s="163"/>
+      <c r="D49" s="161"/>
       <c r="F49" t="s">
         <v>6</v>
       </c>
@@ -11750,7 +11750,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
     <col min="3" max="3" width="45.140625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="154" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="152" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="42.28515625" customWidth="1"/>
     <col min="8" max="8" width="46.7109375" customWidth="1"/>
@@ -11783,7 +11783,7 @@
       <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="155" t="s">
+      <c r="D3" s="153" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -11813,15 +11813,15 @@
       <c r="C4" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="153" t="s">
-        <v>924</v>
+      <c r="D4" s="151" t="s">
+        <v>922</v>
       </c>
       <c r="F4" s="89"/>
       <c r="J4" s="16" t="s">
         <v>521</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11834,15 +11834,15 @@
       <c r="C5" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="153" t="s">
-        <v>925</v>
+      <c r="D5" s="151" t="s">
+        <v>923</v>
       </c>
       <c r="F5" s="89"/>
       <c r="J5" s="16" t="s">
         <v>521</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11852,8 +11852,8 @@
       <c r="C6" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="153" t="s">
-        <v>926</v>
+      <c r="D6" s="151" t="s">
+        <v>924</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -11872,7 +11872,7 @@
         <v>521</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11882,8 +11882,8 @@
       <c r="C7" s="99" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="153" t="s">
-        <v>927</v>
+      <c r="D7" s="151" t="s">
+        <v>925</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -11899,7 +11899,7 @@
         <v>523</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -11909,8 +11909,8 @@
       <c r="C8" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="153" t="s">
-        <v>928</v>
+      <c r="D8" s="151" t="s">
+        <v>926</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -11926,7 +11926,7 @@
         <v>524</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11936,8 +11936,8 @@
       <c r="C9" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="153" t="s">
-        <v>929</v>
+      <c r="D9" s="151" t="s">
+        <v>927</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -11953,7 +11953,7 @@
         <v>522</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11963,8 +11963,8 @@
       <c r="C10" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="153" t="s">
-        <v>930</v>
+      <c r="D10" s="151" t="s">
+        <v>928</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -11983,7 +11983,7 @@
         <v>529</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11993,8 +11993,8 @@
       <c r="C11" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="D11" s="153" t="s">
-        <v>931</v>
+      <c r="D11" s="151" t="s">
+        <v>929</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -12013,7 +12013,7 @@
         <v>530</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -12026,8 +12026,8 @@
       <c r="C12" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="153" t="s">
-        <v>932</v>
+      <c r="D12" s="151" t="s">
+        <v>930</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -12046,7 +12046,7 @@
         <v>531</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -12056,8 +12056,8 @@
       <c r="C13" s="99" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="153" t="s">
-        <v>933</v>
+      <c r="D13" s="151" t="s">
+        <v>931</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -12073,7 +12073,7 @@
         <v>532</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12086,8 +12086,8 @@
       <c r="C14" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="153" t="s">
-        <v>934</v>
+      <c r="D14" s="151" t="s">
+        <v>932</v>
       </c>
       <c r="F14" s="89"/>
       <c r="G14" s="18"/>
@@ -12095,7 +12095,7 @@
         <v>531</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -12105,8 +12105,8 @@
       <c r="C15" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="153" t="s">
-        <v>935</v>
+      <c r="D15" s="151" t="s">
+        <v>933</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -12116,7 +12116,7 @@
         <v>587</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -12126,8 +12126,8 @@
       <c r="C16" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="D16" s="153" t="s">
-        <v>936</v>
+      <c r="D16" s="151" t="s">
+        <v>934</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -12137,7 +12137,7 @@
         <v>602</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -12147,8 +12147,8 @@
       <c r="C17" s="102" t="s">
         <v>193</v>
       </c>
-      <c r="D17" s="153" t="s">
-        <v>937</v>
+      <c r="D17" s="151" t="s">
+        <v>935</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -12158,7 +12158,7 @@
         <v>603</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12168,8 +12168,8 @@
       <c r="C18" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="D18" s="153" t="s">
-        <v>938</v>
+      <c r="D18" s="151" t="s">
+        <v>936</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -12179,7 +12179,7 @@
         <v>603</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -12189,8 +12189,8 @@
       <c r="C19" s="112" t="s">
         <v>545</v>
       </c>
-      <c r="D19" s="153" t="s">
-        <v>939</v>
+      <c r="D19" s="151" t="s">
+        <v>937</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -12203,7 +12203,7 @@
         <v>601</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -12213,8 +12213,8 @@
       <c r="C20" s="111" t="s">
         <v>195</v>
       </c>
-      <c r="D20" s="153" t="s">
-        <v>940</v>
+      <c r="D20" s="151" t="s">
+        <v>938</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -12227,7 +12227,7 @@
         <v>600</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -12237,8 +12237,8 @@
       <c r="C21" s="111" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="153" t="s">
-        <v>941</v>
+      <c r="D21" s="151" t="s">
+        <v>939</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -12251,7 +12251,7 @@
         <v>599</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12261,8 +12261,8 @@
       <c r="C22" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="D22" s="153" t="s">
-        <v>942</v>
+      <c r="D22" s="151" t="s">
+        <v>940</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -12278,7 +12278,7 @@
         <v>598</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -12288,8 +12288,8 @@
       <c r="C23" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="D23" s="153" t="s">
-        <v>943</v>
+      <c r="D23" s="151" t="s">
+        <v>941</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -12305,7 +12305,7 @@
         <v>597</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -12315,8 +12315,8 @@
       <c r="C24" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="D24" s="153" t="s">
-        <v>944</v>
+      <c r="D24" s="151" t="s">
+        <v>942</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -12329,7 +12329,7 @@
         <v>596</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12339,8 +12339,8 @@
       <c r="C25" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="D25" s="153" t="s">
-        <v>945</v>
+      <c r="D25" s="151" t="s">
+        <v>943</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -12353,7 +12353,7 @@
         <v>595</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -12363,8 +12363,8 @@
       <c r="C26" s="104" t="s">
         <v>201</v>
       </c>
-      <c r="D26" s="153" t="s">
-        <v>946</v>
+      <c r="D26" s="151" t="s">
+        <v>944</v>
       </c>
       <c r="E26" t="s">
         <v>606</v>
@@ -12380,7 +12380,7 @@
         <v>592</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -12390,8 +12390,8 @@
       <c r="C27" s="104" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="153" t="s">
-        <v>947</v>
+      <c r="D27" s="151" t="s">
+        <v>945</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -12407,7 +12407,7 @@
         <v>588</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -12417,8 +12417,8 @@
       <c r="C28" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="153" t="s">
-        <v>948</v>
+      <c r="D28" s="151" t="s">
+        <v>946</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -12431,7 +12431,7 @@
         <v>589</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -12441,8 +12441,8 @@
       <c r="C29" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="153" t="s">
-        <v>949</v>
+      <c r="D29" s="151" t="s">
+        <v>947</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -12455,7 +12455,7 @@
         <v>590</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -12465,8 +12465,8 @@
       <c r="C30" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="153" t="s">
-        <v>950</v>
+      <c r="D30" s="151" t="s">
+        <v>948</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -12479,7 +12479,7 @@
         <v>593</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -12489,8 +12489,8 @@
       <c r="C31" s="104" t="s">
         <v>206</v>
       </c>
-      <c r="D31" s="153" t="s">
-        <v>951</v>
+      <c r="D31" s="151" t="s">
+        <v>949</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>604</v>
@@ -12506,7 +12506,7 @@
         <v>591</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -12516,8 +12516,8 @@
       <c r="C32" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="D32" s="153" t="s">
-        <v>952</v>
+      <c r="D32" s="151" t="s">
+        <v>950</v>
       </c>
       <c r="E32" t="s">
         <v>605</v>
@@ -12533,7 +12533,7 @@
         <v>594</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12546,14 +12546,14 @@
       <c r="C33" s="110" t="s">
         <v>208</v>
       </c>
-      <c r="D33" s="153" t="s">
-        <v>953</v>
+      <c r="D33" s="151" t="s">
+        <v>951</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
@@ -12561,7 +12561,7 @@
       <c r="C45" s="109" t="s">
         <v>544</v>
       </c>
-      <c r="D45" s="156"/>
+      <c r="D45" s="154"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   03-11-2021 - 13:06:13.14
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4066B65E-4C45-488D-AACB-19BDC32FF83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808077-E4F8-444C-8513-2A0E6B67FF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2727,9 +2727,6 @@
     <t>circular trver in maze</t>
   </si>
   <si>
-    <t>Detect cycle in a directed graph | Practice | GeeksforGeeks</t>
-  </si>
-  <si>
     <t>use bfs and replace queue with stack</t>
   </si>
   <si>
@@ -3874,6 +3871,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>Detect cycle in a directed graph Practice  GeeksforGeeks</t>
   </si>
 </sst>
 </file>
@@ -5530,7 +5530,7 @@
         <v>232</v>
       </c>
       <c r="D4" s="151" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E4" s="12"/>
       <c r="G4" s="5">
@@ -5543,7 +5543,7 @@
         <v>607</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",L4,")|")</f>
@@ -5561,7 +5561,7 @@
         <v>233</v>
       </c>
       <c r="D5" s="151" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="5">
@@ -5574,7 +5574,7 @@
         <v>607</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M23" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",L5,")|")</f>
@@ -5592,7 +5592,7 @@
         <v>234</v>
       </c>
       <c r="D6" s="151" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E6" s="12"/>
       <c r="G6" s="5">
@@ -5605,7 +5605,7 @@
         <v>607</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -5620,7 +5620,7 @@
         <v>235</v>
       </c>
       <c r="D7" s="175" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" t="s">
@@ -5636,7 +5636,7 @@
         <v>608</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
@@ -5654,7 +5654,7 @@
         <v>236</v>
       </c>
       <c r="D8" s="175" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" t="s">
@@ -5670,7 +5670,7 @@
         <v>609</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
@@ -5685,7 +5685,7 @@
         <v>237</v>
       </c>
       <c r="D9" s="175" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" t="s">
@@ -5701,7 +5701,7 @@
         <v>530</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
@@ -5716,7 +5716,7 @@
         <v>238</v>
       </c>
       <c r="D10" s="175" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" t="s">
@@ -5732,7 +5732,7 @@
         <v>610</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
@@ -5747,7 +5747,7 @@
         <v>239</v>
       </c>
       <c r="D11" s="175" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" t="s">
@@ -5763,7 +5763,7 @@
         <v>600</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
@@ -5778,7 +5778,7 @@
         <v>240</v>
       </c>
       <c r="D12" s="175" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" t="s">
@@ -5794,7 +5794,7 @@
         <v>611</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
@@ -5809,7 +5809,7 @@
         <v>241</v>
       </c>
       <c r="D13" s="175" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" t="s">
@@ -5825,7 +5825,7 @@
         <v>647</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
@@ -5840,7 +5840,7 @@
         <v>242</v>
       </c>
       <c r="D14" s="175" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" t="s">
@@ -5856,7 +5856,7 @@
         <v>613</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -5871,7 +5871,7 @@
         <v>243</v>
       </c>
       <c r="D15" s="175" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" t="s">
@@ -5887,7 +5887,7 @@
         <v>619</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
@@ -5902,7 +5902,7 @@
         <v>244</v>
       </c>
       <c r="D16" s="175" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" t="s">
@@ -5915,7 +5915,7 @@
         <v>621</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -5930,7 +5930,7 @@
         <v>245</v>
       </c>
       <c r="D17" s="175" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" t="s">
@@ -5949,7 +5949,7 @@
         <v>616</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -5964,7 +5964,7 @@
         <v>246</v>
       </c>
       <c r="D18" s="175" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" t="s">
@@ -5977,7 +5977,7 @@
         <v>624</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -5992,7 +5992,7 @@
         <v>248</v>
       </c>
       <c r="D19" s="175" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" t="s">
@@ -6008,7 +6008,7 @@
         <v>625</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -6023,7 +6023,7 @@
         <v>249</v>
       </c>
       <c r="D20" s="175" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" t="s">
@@ -6036,7 +6036,7 @@
         <v>643</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -6051,7 +6051,7 @@
         <v>250</v>
       </c>
       <c r="D21" s="175" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" t="s">
@@ -6064,7 +6064,7 @@
         <v>644</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -6079,7 +6079,7 @@
         <v>251</v>
       </c>
       <c r="D22" s="175" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" t="s">
@@ -6092,7 +6092,7 @@
         <v>645</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
@@ -6107,7 +6107,7 @@
         <v>247</v>
       </c>
       <c r="D23" s="175" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" t="s">
@@ -6120,7 +6120,7 @@
         <v>622</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -6216,8 +6216,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6282,10 +6282,14 @@
         <v>252</v>
       </c>
       <c r="D4" s="151" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
+      </c>
+      <c r="L4" t="str">
+        <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",K4,")|")</f>
+        <v>|[ Binary Search Tree - Introduction](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-search-tree/bst-official/video)|[Solution]()|</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6299,10 +6303,14 @@
         <v>253</v>
       </c>
       <c r="D5" s="151" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
+      </c>
+      <c r="L5" t="str">
+        <f>CONCATENATE("|[",C5,"](",D5,")|[Solution](",K5,")|")</f>
+        <v>|[ Binary Search Tree - Constructor](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-search-tree/bst-constructor/video)|[Solution]()|</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6313,7 +6321,7 @@
         <v>254</v>
       </c>
       <c r="D6" s="151" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -6322,7 +6330,7 @@
         <v>664</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="L6" t="str">
         <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|")</f>
@@ -6337,7 +6345,7 @@
         <v>255</v>
       </c>
       <c r="D7" s="151" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -6346,7 +6354,7 @@
         <v>661</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L13" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
@@ -6361,7 +6369,7 @@
         <v>257</v>
       </c>
       <c r="D8" s="151" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -6376,7 +6384,7 @@
         <v>258</v>
       </c>
       <c r="D9" s="151" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -6385,7 +6393,7 @@
         <v>663</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -6400,7 +6408,7 @@
         <v>259</v>
       </c>
       <c r="D10" s="151" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -6409,7 +6417,7 @@
         <v>662</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -6424,7 +6432,7 @@
         <v>260</v>
       </c>
       <c r="D11" s="151" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -6433,7 +6441,7 @@
         <v>665</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -6451,7 +6459,7 @@
         <v>261</v>
       </c>
       <c r="D12" s="151" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -6460,7 +6468,7 @@
         <v>446</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -6475,7 +6483,7 @@
         <v>256</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -6484,7 +6492,7 @@
         <v>666</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -6595,7 +6603,7 @@
         <v>267</v>
       </c>
       <c r="D6" s="151" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -6609,7 +6617,7 @@
         <v>268</v>
       </c>
       <c r="D7" s="151" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -6618,7 +6626,7 @@
         <v>657</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="L7" t="str">
         <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|")</f>
@@ -6633,7 +6641,7 @@
         <v>269</v>
       </c>
       <c r="D8" s="151" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -6642,7 +6650,7 @@
         <v>658</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ref="L8:L17" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
@@ -6657,7 +6665,7 @@
         <v>270</v>
       </c>
       <c r="D9" s="151" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -6666,7 +6674,7 @@
         <v>659</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -6681,7 +6689,7 @@
         <v>271</v>
       </c>
       <c r="D10" s="151" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -6690,7 +6698,7 @@
         <v>668</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -6708,7 +6716,7 @@
         <v>262</v>
       </c>
       <c r="D11" s="151" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -6717,7 +6725,7 @@
         <v>654</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -6732,7 +6740,7 @@
         <v>263</v>
       </c>
       <c r="D12" s="151" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -6741,7 +6749,7 @@
         <v>655</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -6756,7 +6764,7 @@
         <v>264</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -6765,7 +6773,7 @@
         <v>652</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -6780,7 +6788,7 @@
         <v>265</v>
       </c>
       <c r="D14" s="151" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -6792,7 +6800,7 @@
         <v>653</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -6807,7 +6815,7 @@
         <v>266</v>
       </c>
       <c r="D15" s="151" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -6819,7 +6827,7 @@
         <v>656</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -6834,7 +6842,7 @@
         <v>272</v>
       </c>
       <c r="D16" s="151" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -6843,7 +6851,7 @@
         <v>667</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -6858,7 +6866,7 @@
         <v>273</v>
       </c>
       <c r="D17" s="151" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -6867,7 +6875,7 @@
         <v>660</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -6885,7 +6893,7 @@
         <v>274</v>
       </c>
       <c r="D18" s="151" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6899,7 +6907,7 @@
         <v>275</v>
       </c>
       <c r="D19" s="151" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G19" t="s">
         <v>681</v>
@@ -6953,8 +6961,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D25"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7020,7 +7028,7 @@
         <v>276</v>
       </c>
       <c r="D4" s="151" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",K4,")|")</f>
@@ -7038,7 +7046,7 @@
         <v>278</v>
       </c>
       <c r="D5" s="151" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="G5" t="s">
         <v>669</v>
@@ -7050,7 +7058,7 @@
         <v>674</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L25" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",K5,")|")</f>
@@ -7068,7 +7076,7 @@
         <v>279</v>
       </c>
       <c r="D6" s="151" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>671</v>
@@ -7080,7 +7088,7 @@
         <v>675</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -7098,13 +7106,13 @@
         <v>280</v>
       </c>
       <c r="D7" s="151" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>699</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -7122,13 +7130,13 @@
         <v>281</v>
       </c>
       <c r="D8" s="151" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>700</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -7146,13 +7154,13 @@
         <v>282</v>
       </c>
       <c r="D9" s="151" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>701</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -7170,13 +7178,13 @@
         <v>283</v>
       </c>
       <c r="D10" s="151" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>702</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -7194,13 +7202,13 @@
         <v>284</v>
       </c>
       <c r="D11" s="151" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>703</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -7218,13 +7226,13 @@
         <v>285</v>
       </c>
       <c r="D12" s="151" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>704</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -7242,13 +7250,13 @@
         <v>286</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="J13" s="16" t="s">
         <v>705</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -7266,13 +7274,13 @@
         <v>287</v>
       </c>
       <c r="D14" s="151" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="J14" s="16" t="s">
         <v>706</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -7290,7 +7298,7 @@
         <v>288</v>
       </c>
       <c r="D15" s="151" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="G15" t="s">
         <v>698</v>
@@ -7299,7 +7307,7 @@
         <v>707</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -7317,7 +7325,7 @@
         <v>289</v>
       </c>
       <c r="D16" s="151" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G16" t="s">
         <v>697</v>
@@ -7326,7 +7334,7 @@
         <v>708</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -7344,7 +7352,7 @@
         <v>290</v>
       </c>
       <c r="D17" s="151" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G17" t="s">
         <v>687</v>
@@ -7353,7 +7361,7 @@
         <v>709</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -7371,7 +7379,7 @@
         <v>692</v>
       </c>
       <c r="D18" s="151" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="G18" t="s">
         <v>688</v>
@@ -7386,7 +7394,7 @@
         <v>710</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -7404,7 +7412,7 @@
         <v>691</v>
       </c>
       <c r="D19" s="151" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="G19" t="s">
         <v>689</v>
@@ -7416,7 +7424,7 @@
         <v>711</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -7434,19 +7442,19 @@
         <v>291</v>
       </c>
       <c r="D20" s="151" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G20" t="s">
         <v>695</v>
       </c>
       <c r="H20" t="s">
+        <v>717</v>
+      </c>
+      <c r="J20" s="16" t="s">
         <v>718</v>
       </c>
-      <c r="J20" s="16" t="s">
-        <v>719</v>
-      </c>
       <c r="K20" s="16" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -7464,19 +7472,19 @@
         <v>277</v>
       </c>
       <c r="D21" s="151" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G21" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H21" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -7485,22 +7493,22 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C22" s="16" t="s">
-        <v>716</v>
+        <v>1098</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
-        <v>|[Detect cycle in a directed graph | Practice | GeeksforGeeks](https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1)|[Solution]()|</v>
+        <v>|[Detect cycle in a directed graph Practice  GeeksforGeeks](https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1)|[Solution]()|</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C23" s="16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
@@ -7509,10 +7517,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" s="16" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
@@ -7521,10 +7529,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C25" s="16" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
@@ -7956,10 +7964,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="145" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E4" s="165" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>5</v>
@@ -7980,7 +7988,7 @@
         <v>47</v>
       </c>
       <c r="M4" s="148" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="N4" t="str">
         <f>CONCATENATE("|[",D4,"](",E4,")|[Solution](",M4,")|")</f>
@@ -7995,10 +8003,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="140" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E5" s="166" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>5</v>
@@ -8019,7 +8027,7 @@
         <v>48</v>
       </c>
       <c r="M5" s="149" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N34" si="0">CONCATENATE("|[",D5,"](",E5,")|[Solution](",M5,")|")</f>
@@ -8034,10 +8042,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="140" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E6" s="166" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>5</v>
@@ -8058,7 +8066,7 @@
         <v>53</v>
       </c>
       <c r="M6" s="149" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
@@ -8073,10 +8081,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="140" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E7" s="166" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>5</v>
@@ -8097,7 +8105,7 @@
         <v>54</v>
       </c>
       <c r="M7" s="149" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
@@ -8112,10 +8120,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="140" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E8" s="166" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>5</v>
@@ -8136,7 +8144,7 @@
         <v>55</v>
       </c>
       <c r="M8" s="149" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
@@ -8148,10 +8156,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="140" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E9" s="166" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>6</v>
@@ -8169,7 +8177,7 @@
         <v>62</v>
       </c>
       <c r="M9" s="149" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
@@ -8184,10 +8192,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="140" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E10" s="166" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>5</v>
@@ -8211,7 +8219,7 @@
         <v>58</v>
       </c>
       <c r="M10" s="149" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
@@ -8226,10 +8234,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="140" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E11" s="166" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>5</v>
@@ -8253,7 +8261,7 @@
         <v>61</v>
       </c>
       <c r="M11" s="149" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
@@ -8268,10 +8276,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="141" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E12" s="167" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>5</v>
@@ -8289,7 +8297,7 @@
         <v>65</v>
       </c>
       <c r="M12" s="149" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
@@ -8304,10 +8312,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="141" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E13" s="167" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>5</v>
@@ -8328,7 +8336,7 @@
         <v>67</v>
       </c>
       <c r="M13" s="149" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
@@ -8343,10 +8351,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="141" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E14" s="167" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>5</v>
@@ -8367,7 +8375,7 @@
         <v>69</v>
       </c>
       <c r="M14" s="149" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
@@ -8382,10 +8390,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="141" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E15" s="167" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>5</v>
@@ -8400,7 +8408,7 @@
         <v>402</v>
       </c>
       <c r="M15" s="149" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
@@ -8415,10 +8423,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="141" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E16" s="167" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>5</v>
@@ -8433,7 +8441,7 @@
         <v>403</v>
       </c>
       <c r="M16" s="149" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
@@ -8448,10 +8456,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="141" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E17" s="167" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>5</v>
@@ -8469,7 +8477,7 @@
         <v>404</v>
       </c>
       <c r="M17" s="149" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
@@ -8484,10 +8492,10 @@
         <v>4</v>
       </c>
       <c r="D18" s="143" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E18" s="168" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>5</v>
@@ -8505,7 +8513,7 @@
         <v>641</v>
       </c>
       <c r="M18" s="149" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
@@ -8520,10 +8528,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="143" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E19" s="168" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>5</v>
@@ -8538,7 +8546,7 @@
         <v>642</v>
       </c>
       <c r="M19" s="149" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="0"/>
@@ -8553,10 +8561,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="143" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E20" s="168" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
@@ -8571,7 +8579,7 @@
         <v>640</v>
       </c>
       <c r="M20" s="149" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="0"/>
@@ -8586,10 +8594,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="143" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E21" s="168" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
@@ -8604,7 +8612,7 @@
         <v>638</v>
       </c>
       <c r="M21" s="149" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="0"/>
@@ -8619,10 +8627,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="143" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E22" s="168" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
@@ -8637,7 +8645,7 @@
         <v>639</v>
       </c>
       <c r="M22" s="149" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="0"/>
@@ -8652,10 +8660,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="142" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E23" s="169" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -8676,7 +8684,7 @@
         <v>637</v>
       </c>
       <c r="M23" s="149" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="0"/>
@@ -8691,10 +8699,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="142" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E24" s="169" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -8715,7 +8723,7 @@
         <v>632</v>
       </c>
       <c r="M24" s="149" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="0"/>
@@ -8730,10 +8738,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="142" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E25" s="169" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>5</v>
@@ -8751,7 +8759,7 @@
         <v>633</v>
       </c>
       <c r="M25" s="149" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="0"/>
@@ -8766,10 +8774,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="142" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E26" s="169" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>5</v>
@@ -8787,7 +8795,7 @@
         <v>634</v>
       </c>
       <c r="M26" s="149" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="0"/>
@@ -8802,10 +8810,10 @@
         <v>4</v>
       </c>
       <c r="D27" s="142" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E27" s="169" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>5</v>
@@ -8826,7 +8834,7 @@
         <v>635</v>
       </c>
       <c r="M27" s="149" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="0"/>
@@ -8841,10 +8849,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="142" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E28" s="169" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>5</v>
@@ -8862,7 +8870,7 @@
         <v>636</v>
       </c>
       <c r="M28" s="149" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="0"/>
@@ -8877,10 +8885,10 @@
         <v>4</v>
       </c>
       <c r="D29" s="142" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E29" s="169" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>5</v>
@@ -8901,7 +8909,7 @@
         <v>631</v>
       </c>
       <c r="M29" s="149" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="0"/>
@@ -8916,10 +8924,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="144" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E30" s="170" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>5</v>
@@ -8940,7 +8948,7 @@
         <v>626</v>
       </c>
       <c r="M30" s="149" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="0"/>
@@ -8955,10 +8963,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="144" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E31" s="170" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>5</v>
@@ -8979,7 +8987,7 @@
         <v>630</v>
       </c>
       <c r="M31" s="149" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="0"/>
@@ -8994,10 +9002,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="144" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E32" s="170" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>5</v>
@@ -9018,7 +9026,7 @@
         <v>629</v>
       </c>
       <c r="M32" s="149" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="0"/>
@@ -9027,10 +9035,10 @@
     </row>
     <row r="33" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="144" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E33" s="170" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H33" s="2">
         <v>2</v>
@@ -9042,7 +9050,7 @@
         <v>628</v>
       </c>
       <c r="M33" s="149" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="0"/>
@@ -9057,10 +9065,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="144" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E34" s="170" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>5</v>
@@ -9081,7 +9089,7 @@
         <v>627</v>
       </c>
       <c r="M34" s="150" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="0"/>
@@ -9869,7 +9877,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="151" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
@@ -9884,7 +9892,7 @@
         <v>298</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="L5" t="str">
         <f>CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
@@ -9899,7 +9907,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="151" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -9914,7 +9922,7 @@
         <v>297</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ref="L6:L21" si="0">CONCATENATE("|[",B6,"](",C6,")|[Solution](",K6,")|")</f>
@@ -9929,7 +9937,7 @@
         <v>302</v>
       </c>
       <c r="C7" s="151" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -9944,7 +9952,7 @@
         <v>504</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -9959,7 +9967,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="151" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -9974,7 +9982,7 @@
         <v>306</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -9989,7 +9997,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="151" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -10001,7 +10009,7 @@
         <v>308</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -10016,7 +10024,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="151" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>5</v>
@@ -10030,7 +10038,7 @@
         <v>317</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -10045,7 +10053,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="151" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
@@ -10063,7 +10071,7 @@
         <v>392</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -10078,7 +10086,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="151" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -10093,7 +10101,7 @@
         <v>393</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -10108,7 +10116,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="151" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -10123,7 +10131,7 @@
         <v>390</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -10138,7 +10146,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="151" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>5</v>
@@ -10155,7 +10163,7 @@
         <v>391</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -10170,7 +10178,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="151" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -10185,7 +10193,7 @@
         <v>388</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -10200,7 +10208,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="151" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -10212,7 +10220,7 @@
         <v>389</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -10227,7 +10235,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
@@ -10239,7 +10247,7 @@
         <v>394</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -10254,7 +10262,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="151" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -10266,7 +10274,7 @@
         <v>395</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -10281,7 +10289,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="151" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
@@ -10290,7 +10298,7 @@
         <v>396</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -10305,7 +10313,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="151" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
@@ -10323,7 +10331,7 @@
         <v>397</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -10338,7 +10346,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="151" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D21" s="53" t="s">
         <v>5</v>
@@ -10352,7 +10360,7 @@
         <v>398</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -10923,7 +10931,7 @@
         <v>379</v>
       </c>
       <c r="C4" s="159" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -10939,7 +10947,7 @@
         <v>382</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",B4,"](",C4,")|[Solution](",K4,")|")</f>
@@ -10954,7 +10962,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="159" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -10966,7 +10974,7 @@
         <v>381</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L11" si="0">CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
@@ -10981,7 +10989,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="159" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -10995,7 +11003,7 @@
         <v>407</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -11010,7 +11018,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="159" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -11024,7 +11032,7 @@
         <v>406</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -11039,7 +11047,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="159" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -11053,7 +11061,7 @@
         <v>410</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -11068,7 +11076,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="159" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -11082,7 +11090,7 @@
         <v>409</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -11097,7 +11105,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="159" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
@@ -11113,7 +11121,7 @@
         <v>408</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -11146,7 +11154,7 @@
         <v>377</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -11247,7 +11255,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>455</v>
@@ -11270,7 +11278,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D4" s="70" t="s">
         <v>147</v>
@@ -11290,7 +11298,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D5" s="70" t="s">
         <v>148</v>
@@ -11310,7 +11318,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D6" s="70" t="s">
         <v>149</v>
@@ -11330,7 +11338,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D7" s="70" t="s">
         <v>150</v>
@@ -11350,7 +11358,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D8" s="70" t="s">
         <v>151</v>
@@ -11370,7 +11378,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D9" s="70" t="s">
         <v>152</v>
@@ -11390,7 +11398,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D10" s="136" t="s">
         <v>153</v>
@@ -11407,10 +11415,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>154</v>
@@ -11427,10 +11435,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C12" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D12" s="137" t="s">
         <v>155</v>
@@ -11447,10 +11455,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="135" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C13" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D13" s="137" t="s">
         <v>156</v>
@@ -11470,10 +11478,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C14" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D14" s="137" t="s">
         <v>157</v>
@@ -11493,10 +11501,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="135" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D15" s="138" t="s">
         <v>158</v>
@@ -11516,7 +11524,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D16" s="84" t="s">
         <v>159</v>
@@ -11533,7 +11541,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="90" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D17" s="84" t="s">
         <v>160</v>
@@ -11550,7 +11558,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="90" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D18" s="84" t="s">
         <v>161</v>
@@ -11567,7 +11575,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D19" s="84" t="s">
         <v>162</v>
@@ -11584,7 +11592,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D20" s="84" t="s">
         <v>163</v>
@@ -11601,7 +11609,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D21" s="72" t="s">
         <v>164</v>
@@ -11618,7 +11626,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="90" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D22" s="72" t="s">
         <v>165</v>
@@ -11635,7 +11643,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="135" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D23" s="72" t="s">
         <v>166</v>
@@ -11652,7 +11660,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="135" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D24" s="73" t="s">
         <v>167</v>
@@ -11669,7 +11677,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="135" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D25" s="73" t="s">
         <v>168</v>
@@ -11686,7 +11694,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="135" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D26" s="73" t="s">
         <v>169</v>
@@ -11703,7 +11711,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="135" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D27" s="73" t="s">
         <v>170</v>
@@ -11720,7 +11728,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="135" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D28" s="71" t="s">
         <v>171</v>
@@ -11737,7 +11745,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="135" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D29" s="71" t="s">
         <v>172</v>
@@ -11754,7 +11762,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="135" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D30" s="71" t="s">
         <v>173</v>
@@ -11928,7 +11936,7 @@
         <v>209</v>
       </c>
       <c r="D9" s="159" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -11937,7 +11945,7 @@
         <v>416</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M9" t="str">
         <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",L9,")|")</f>
@@ -11952,7 +11960,7 @@
         <v>210</v>
       </c>
       <c r="D10" s="159" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -11961,7 +11969,7 @@
         <v>416</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ref="M10:M34" si="0">CONCATENATE("|[",C10,"](",D10,")|[Solution](",L10,")|")</f>
@@ -11976,7 +11984,7 @@
         <v>211</v>
       </c>
       <c r="D11" s="159" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -11985,7 +11993,7 @@
         <v>416</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
@@ -12000,7 +12008,7 @@
         <v>212</v>
       </c>
       <c r="D12" s="159" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -12009,7 +12017,7 @@
         <v>416</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
@@ -12024,7 +12032,7 @@
         <v>213</v>
       </c>
       <c r="D13" s="159" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -12033,7 +12041,7 @@
         <v>416</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
@@ -12048,7 +12056,7 @@
         <v>214</v>
       </c>
       <c r="D14" s="159" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -12057,7 +12065,7 @@
         <v>416</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -12072,7 +12080,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="159" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -12081,7 +12089,7 @@
         <v>416</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
@@ -12096,7 +12104,7 @@
         <v>216</v>
       </c>
       <c r="D16" s="159" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -12105,7 +12113,7 @@
         <v>416</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -12120,7 +12128,7 @@
         <v>217</v>
       </c>
       <c r="D17" s="159" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -12135,7 +12143,7 @@
         <v>487</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -12150,7 +12158,7 @@
         <v>218</v>
       </c>
       <c r="D18" s="159" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -12162,7 +12170,7 @@
         <v>488</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -12177,7 +12185,7 @@
         <v>219</v>
       </c>
       <c r="D19" s="159" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -12189,7 +12197,7 @@
         <v>483</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -12204,7 +12212,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="159" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -12216,7 +12224,7 @@
         <v>484</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -12231,7 +12239,7 @@
         <v>221</v>
       </c>
       <c r="D21" s="159" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -12243,7 +12251,7 @@
         <v>485</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -12258,7 +12266,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="159" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -12270,7 +12278,7 @@
         <v>486</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
@@ -12285,7 +12293,7 @@
         <v>223</v>
       </c>
       <c r="D23" s="159" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -12303,7 +12311,7 @@
         <v>466</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -12318,7 +12326,7 @@
         <v>224</v>
       </c>
       <c r="D24" s="159" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -12327,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
@@ -12342,7 +12350,7 @@
         <v>225</v>
       </c>
       <c r="D25" s="159" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -12354,7 +12362,7 @@
         <v>482</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
@@ -12369,7 +12377,7 @@
         <v>178</v>
       </c>
       <c r="D26" s="159" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -12378,7 +12386,7 @@
         <v>481</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
@@ -12393,7 +12401,7 @@
         <v>226</v>
       </c>
       <c r="D27" s="159" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -12402,7 +12410,7 @@
         <v>489</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
@@ -12417,7 +12425,7 @@
         <v>227</v>
       </c>
       <c r="D28" s="159" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
@@ -12426,7 +12434,7 @@
         <v>499</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
@@ -12441,7 +12449,7 @@
         <v>228</v>
       </c>
       <c r="D29" s="159" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -12450,7 +12458,7 @@
         <v>500</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
@@ -12465,7 +12473,7 @@
         <v>229</v>
       </c>
       <c r="D30" s="159" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -12477,7 +12485,7 @@
         <v>501</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
@@ -12492,7 +12500,7 @@
         <v>230</v>
       </c>
       <c r="D31" s="159" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -12510,7 +12518,7 @@
         <v>503</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
@@ -12525,7 +12533,7 @@
         <v>231</v>
       </c>
       <c r="D32" s="159" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -12540,7 +12548,7 @@
         <v>515</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
@@ -12555,7 +12563,7 @@
         <v>179</v>
       </c>
       <c r="D33" s="159" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -12567,7 +12575,7 @@
         <v>519</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
@@ -12585,7 +12593,7 @@
         <v>505</v>
       </c>
       <c r="D34" s="159" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -12597,7 +12605,7 @@
         <v>520</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="0"/>
@@ -12904,7 +12912,7 @@
         <v>180</v>
       </c>
       <c r="D4" s="151" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F4" s="89"/>
       <c r="I4">
@@ -12914,7 +12922,7 @@
         <v>521</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12928,14 +12936,14 @@
         <v>181</v>
       </c>
       <c r="D5" s="151" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F5" s="89"/>
       <c r="J5" s="16" t="s">
         <v>521</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12946,7 +12954,7 @@
         <v>182</v>
       </c>
       <c r="D6" s="151" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -12965,7 +12973,7 @@
         <v>521</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12976,7 +12984,7 @@
         <v>183</v>
       </c>
       <c r="D7" s="151" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -12992,7 +13000,7 @@
         <v>523</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -13003,7 +13011,7 @@
         <v>184</v>
       </c>
       <c r="D8" s="151" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -13019,7 +13027,7 @@
         <v>524</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13030,7 +13038,7 @@
         <v>185</v>
       </c>
       <c r="D9" s="151" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -13046,7 +13054,7 @@
         <v>522</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13057,7 +13065,7 @@
         <v>186</v>
       </c>
       <c r="D10" s="151" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -13076,7 +13084,7 @@
         <v>529</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13087,7 +13095,7 @@
         <v>187</v>
       </c>
       <c r="D11" s="151" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -13106,7 +13114,7 @@
         <v>530</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -13120,7 +13128,7 @@
         <v>188</v>
       </c>
       <c r="D12" s="151" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -13139,7 +13147,7 @@
         <v>531</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -13150,7 +13158,7 @@
         <v>189</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -13166,7 +13174,7 @@
         <v>532</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13180,7 +13188,7 @@
         <v>190</v>
       </c>
       <c r="D14" s="151" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F14" s="89"/>
       <c r="G14" s="18"/>
@@ -13188,7 +13196,7 @@
         <v>531</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -13199,7 +13207,7 @@
         <v>191</v>
       </c>
       <c r="D15" s="151" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -13209,7 +13217,7 @@
         <v>587</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -13220,7 +13228,7 @@
         <v>192</v>
       </c>
       <c r="D16" s="151" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -13230,7 +13238,7 @@
         <v>602</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -13241,7 +13249,7 @@
         <v>193</v>
       </c>
       <c r="D17" s="151" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -13251,7 +13259,7 @@
         <v>603</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13262,7 +13270,7 @@
         <v>194</v>
       </c>
       <c r="D18" s="151" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -13272,7 +13280,7 @@
         <v>603</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -13283,7 +13291,7 @@
         <v>545</v>
       </c>
       <c r="D19" s="151" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -13296,7 +13304,7 @@
         <v>601</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -13307,7 +13315,7 @@
         <v>195</v>
       </c>
       <c r="D20" s="151" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -13320,7 +13328,7 @@
         <v>600</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -13331,7 +13339,7 @@
         <v>196</v>
       </c>
       <c r="D21" s="151" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -13344,7 +13352,7 @@
         <v>599</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13355,7 +13363,7 @@
         <v>197</v>
       </c>
       <c r="D22" s="151" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -13371,7 +13379,7 @@
         <v>598</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -13382,7 +13390,7 @@
         <v>198</v>
       </c>
       <c r="D23" s="151" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -13398,7 +13406,7 @@
         <v>597</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -13409,7 +13417,7 @@
         <v>199</v>
       </c>
       <c r="D24" s="151" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -13422,7 +13430,7 @@
         <v>596</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13433,7 +13441,7 @@
         <v>200</v>
       </c>
       <c r="D25" s="151" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -13446,7 +13454,7 @@
         <v>595</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -13457,7 +13465,7 @@
         <v>201</v>
       </c>
       <c r="D26" s="151" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="E26" t="s">
         <v>606</v>
@@ -13473,7 +13481,7 @@
         <v>592</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -13484,7 +13492,7 @@
         <v>202</v>
       </c>
       <c r="D27" s="151" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -13500,7 +13508,7 @@
         <v>588</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -13511,7 +13519,7 @@
         <v>203</v>
       </c>
       <c r="D28" s="151" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -13524,7 +13532,7 @@
         <v>589</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -13535,7 +13543,7 @@
         <v>204</v>
       </c>
       <c r="D29" s="151" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -13548,7 +13556,7 @@
         <v>590</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -13559,7 +13567,7 @@
         <v>205</v>
       </c>
       <c r="D30" s="151" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -13572,7 +13580,7 @@
         <v>593</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -13583,7 +13591,7 @@
         <v>206</v>
       </c>
       <c r="D31" s="151" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>604</v>
@@ -13599,7 +13607,7 @@
         <v>591</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -13610,7 +13618,7 @@
         <v>207</v>
       </c>
       <c r="D32" s="151" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E32" t="s">
         <v>605</v>
@@ -13626,7 +13634,7 @@
         <v>594</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13640,13 +13648,13 @@
         <v>208</v>
       </c>
       <c r="D33" s="151" t="s">
+        <v>949</v>
+      </c>
+      <c r="J33" s="16" t="s">
         <v>950</v>
       </c>
-      <c r="J33" s="16" t="s">
-        <v>951</v>
-      </c>
       <c r="K33" s="16" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated code on timestamp:   03-11-2021 - 13:10:30.05
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808077-E4F8-444C-8513-2A0E6B67FF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C00F9F2-79F5-4C60-AE07-FA0ADAC74180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -6216,7 +6216,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4:L13"/>
     </sheetView>
   </sheetViews>
@@ -6535,8 +6535,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6653,7 +6653,7 @@
         <v>1067</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" ref="L8:L17" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
+        <f t="shared" ref="L8:L19" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
         <v>|[ K Largest Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/k-largest-elements-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java)|</v>
       </c>
     </row>
@@ -6895,6 +6895,10 @@
       <c r="D18" s="151" t="s">
         <v>1064</v>
       </c>
+      <c r="L18" t="str">
+        <f>CONCATENATE("|[",C17,"](",D17,")|[Solution](",K17,")|")</f>
+        <v>|[ Write Hashmap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java)|</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
@@ -6911,6 +6915,10 @@
       </c>
       <c r="G19" t="s">
         <v>681</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Efficient Heap Constructor](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/heap-eff-constructor/video)|[Solution]()|</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-11-2021 - 13:17:46.06
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C00F9F2-79F5-4C60-AE07-FA0ADAC74180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D7B3FD-4D58-48F8-8319-FF707E2B9E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="1114">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3874,6 +3874,51 @@
   </si>
   <si>
     <t>Detect cycle in a directed graph Practice  GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/introduction_to_heaps/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/k_largest_elements/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/sort_a_k_sorted_array/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/median_priority_queue/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/merge_k_sorted_lists/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/introduction_to_hashmaps/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/highest_frequency_character/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/get_common_elements_1/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/get_common_elements_2/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/longest_consecutive_sequence/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/priority_queue_using_heap/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/write_hashmap/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/efficient_heap_construction/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/heap_comparable_vs_comparator/topic</t>
   </si>
 </sst>
 </file>
@@ -4849,14 +4894,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -5269,10 +5314,10 @@
       <c r="C2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="173" t="s">
+      <c r="F2" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="173"/>
+      <c r="G2" s="174"/>
       <c r="J2" s="90" t="s">
         <v>294</v>
       </c>
@@ -5619,7 +5664,7 @@
       <c r="C7" s="111" t="s">
         <v>235</v>
       </c>
-      <c r="D7" s="175" t="s">
+      <c r="D7" s="173" t="s">
         <v>982</v>
       </c>
       <c r="E7" s="12"/>
@@ -5653,7 +5698,7 @@
       <c r="C8" s="111" t="s">
         <v>236</v>
       </c>
-      <c r="D8" s="175" t="s">
+      <c r="D8" s="173" t="s">
         <v>983</v>
       </c>
       <c r="E8" s="12"/>
@@ -5684,7 +5729,7 @@
       <c r="C9" s="111" t="s">
         <v>237</v>
       </c>
-      <c r="D9" s="175" t="s">
+      <c r="D9" s="173" t="s">
         <v>984</v>
       </c>
       <c r="E9" s="12"/>
@@ -5715,7 +5760,7 @@
       <c r="C10" s="113" t="s">
         <v>238</v>
       </c>
-      <c r="D10" s="175" t="s">
+      <c r="D10" s="173" t="s">
         <v>985</v>
       </c>
       <c r="E10" s="12"/>
@@ -5746,7 +5791,7 @@
       <c r="C11" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="D11" s="175" t="s">
+      <c r="D11" s="173" t="s">
         <v>986</v>
       </c>
       <c r="E11" s="12"/>
@@ -5777,7 +5822,7 @@
       <c r="C12" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="175" t="s">
+      <c r="D12" s="173" t="s">
         <v>987</v>
       </c>
       <c r="E12" s="12"/>
@@ -5808,7 +5853,7 @@
       <c r="C13" s="121" t="s">
         <v>241</v>
       </c>
-      <c r="D13" s="175" t="s">
+      <c r="D13" s="173" t="s">
         <v>988</v>
       </c>
       <c r="E13" s="12"/>
@@ -5839,7 +5884,7 @@
       <c r="C14" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="D14" s="175" t="s">
+      <c r="D14" s="173" t="s">
         <v>989</v>
       </c>
       <c r="E14" s="12"/>
@@ -5870,7 +5915,7 @@
       <c r="C15" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="D15" s="175" t="s">
+      <c r="D15" s="173" t="s">
         <v>990</v>
       </c>
       <c r="E15" s="12"/>
@@ -5901,7 +5946,7 @@
       <c r="C16" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="D16" s="175" t="s">
+      <c r="D16" s="173" t="s">
         <v>991</v>
       </c>
       <c r="E16" s="12"/>
@@ -5929,7 +5974,7 @@
       <c r="C17" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="175" t="s">
+      <c r="D17" s="173" t="s">
         <v>992</v>
       </c>
       <c r="E17" s="12"/>
@@ -5963,7 +6008,7 @@
       <c r="C18" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="D18" s="175" t="s">
+      <c r="D18" s="173" t="s">
         <v>993</v>
       </c>
       <c r="E18" s="12"/>
@@ -5991,7 +6036,7 @@
       <c r="C19" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="D19" s="175" t="s">
+      <c r="D19" s="173" t="s">
         <v>994</v>
       </c>
       <c r="E19" s="12"/>
@@ -6022,7 +6067,7 @@
       <c r="C20" s="99" t="s">
         <v>249</v>
       </c>
-      <c r="D20" s="175" t="s">
+      <c r="D20" s="173" t="s">
         <v>995</v>
       </c>
       <c r="E20" s="12"/>
@@ -6050,7 +6095,7 @@
       <c r="C21" s="99" t="s">
         <v>250</v>
       </c>
-      <c r="D21" s="175" t="s">
+      <c r="D21" s="173" t="s">
         <v>996</v>
       </c>
       <c r="E21" s="12"/>
@@ -6078,7 +6123,7 @@
       <c r="C22" s="126" t="s">
         <v>251</v>
       </c>
-      <c r="D22" s="175" t="s">
+      <c r="D22" s="173" t="s">
         <v>997</v>
       </c>
       <c r="E22" s="12"/>
@@ -6106,7 +6151,7 @@
       <c r="C23" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="D23" s="175" t="s">
+      <c r="D23" s="173" t="s">
         <v>998</v>
       </c>
       <c r="E23" s="12"/>
@@ -6535,8 +6580,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,7 +6589,7 @@
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="3" max="3" width="41.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.140625" customWidth="1"/>
     <col min="8" max="8" width="57.140625" customWidth="1"/>
     <col min="9" max="9" width="37.140625" customWidth="1"/>
@@ -6576,7 +6621,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>455</v>
+        <v>1099</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>10</v>
@@ -6608,6 +6653,9 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
+      <c r="F6" s="151" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -6622,6 +6670,9 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
+      <c r="F7" s="151" t="s">
+        <v>1101</v>
+      </c>
       <c r="J7" s="16" t="s">
         <v>657</v>
       </c>
@@ -6629,8 +6680,8 @@
         <v>1066</v>
       </c>
       <c r="L7" t="str">
-        <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|")</f>
-        <v>|[ Heaps - Introduction And Usage](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/heaps-intro/video)|[Solution]()|</v>
+        <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|[Articles](",F6,")")</f>
+        <v>|[ Heaps - Introduction And Usage](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/heaps-intro/video)|[Solution]()|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/introduction_to_heaps/topic)</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6646,6 +6697,9 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
+      <c r="F8" s="151" t="s">
+        <v>1102</v>
+      </c>
       <c r="J8" s="16" t="s">
         <v>658</v>
       </c>
@@ -6653,7 +6707,7 @@
         <v>1067</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" ref="L8:L19" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
+        <f>CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
         <v>|[ K Largest Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/k-largest-elements-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java)|</v>
       </c>
     </row>
@@ -6670,6 +6724,9 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
+      <c r="F9" s="151" t="s">
+        <v>1103</v>
+      </c>
       <c r="J9" s="16" t="s">
         <v>659</v>
       </c>
@@ -6677,7 +6734,7 @@
         <v>1068</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C8,"](",D8,")|[Solution](",K8,")|")</f>
         <v>|[ Sort K-sorted Array ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/sort-ksorted-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java)|</v>
       </c>
     </row>
@@ -6694,6 +6751,9 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
+      <c r="F10" s="151" t="s">
+        <v>1104</v>
+      </c>
       <c r="J10" s="21" t="s">
         <v>668</v>
       </c>
@@ -6701,7 +6761,7 @@
         <v>1069</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",K9,")|")</f>
         <v>|[ Median Priority Queue ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/median-priority-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java)|</v>
       </c>
     </row>
@@ -6721,6 +6781,9 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
+      <c r="F11" s="151" t="s">
+        <v>1105</v>
+      </c>
       <c r="J11" s="16" t="s">
         <v>654</v>
       </c>
@@ -6728,7 +6791,7 @@
         <v>1070</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C10,"](",D10,")|[Solution](",K10,")|")</f>
         <v>|[ Merge K Sorted Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/merge-k-sorted-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java)|</v>
       </c>
     </row>
@@ -6745,6 +6808,9 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
+      <c r="F12" s="151" t="s">
+        <v>1106</v>
+      </c>
       <c r="J12" s="16" t="s">
         <v>655</v>
       </c>
@@ -6752,7 +6818,7 @@
         <v>1071</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C11,"](",D11,")|[Solution](",K11,")|")</f>
         <v>|[ Hashmap - Introduction](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-intro/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java)|</v>
       </c>
     </row>
@@ -6769,6 +6835,9 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
+      <c r="F13" s="151" t="s">
+        <v>1107</v>
+      </c>
       <c r="J13" s="16" t="s">
         <v>652</v>
       </c>
@@ -6776,7 +6845,7 @@
         <v>1072</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C12,"](",D12,")|[Solution](",K12,")|")</f>
         <v>|[ Highest Frequency Character ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hfc-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java)|</v>
       </c>
     </row>
@@ -6793,6 +6862,9 @@
       <c r="E14" t="s">
         <v>6</v>
       </c>
+      <c r="F14" s="151" t="s">
+        <v>1108</v>
+      </c>
       <c r="G14" t="s">
         <v>648</v>
       </c>
@@ -6803,7 +6875,7 @@
         <v>1073</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C13,"](",D13,")|[Solution](",K13,")|")</f>
         <v>|[ Get Common Elements - 1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce1-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java)|</v>
       </c>
     </row>
@@ -6820,6 +6892,9 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
+      <c r="F15" s="151" t="s">
+        <v>1109</v>
+      </c>
       <c r="G15" s="18" t="s">
         <v>651</v>
       </c>
@@ -6830,7 +6905,7 @@
         <v>1074</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C14,"](",D14,")|[Solution](",K14,")|")</f>
         <v>|[ Get Common Elements - 2 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce2-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java)|</v>
       </c>
     </row>
@@ -6847,6 +6922,9 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
+      <c r="F16" s="151" t="s">
+        <v>1110</v>
+      </c>
       <c r="J16" s="16" t="s">
         <v>667</v>
       </c>
@@ -6854,7 +6932,7 @@
         <v>1075</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C15,"](",D15,")|[Solution](",K15,")|")</f>
         <v>|[ Longest Consecutive Sequence Of Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/lcqs-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java)|</v>
       </c>
     </row>
@@ -6871,6 +6949,9 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
+      <c r="F17" s="151" t="s">
+        <v>1111</v>
+      </c>
       <c r="J17" s="16" t="s">
         <v>660</v>
       </c>
@@ -6878,7 +6959,7 @@
         <v>1076</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C16,"](",D16,")|[Solution](",K16,")|")</f>
         <v>|[ Write Priority Queue Using Heap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/priority-queue-using-heap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java)|</v>
       </c>
     </row>
@@ -6895,6 +6976,9 @@
       <c r="D18" s="151" t="s">
         <v>1064</v>
       </c>
+      <c r="F18" s="151" t="s">
+        <v>1112</v>
+      </c>
       <c r="L18" t="str">
         <f>CONCATENATE("|[",C17,"](",D17,")|[Solution](",K17,")|")</f>
         <v>|[ Write Hashmap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java)|</v>
@@ -6913,11 +6997,14 @@
       <c r="D19" s="151" t="s">
         <v>1065</v>
       </c>
+      <c r="F19" s="151" t="s">
+        <v>1113</v>
+      </c>
       <c r="G19" t="s">
         <v>681</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("|[",C18,"](",D18,")|[Solution](",K18,")|")</f>
         <v>|[ Efficient Heap Constructor](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/heap-eff-constructor/video)|[Solution]()|</v>
       </c>
     </row>
@@ -6959,8 +7046,23 @@
     <hyperlink ref="K15" r:id="rId34" xr:uid="{21562BBF-2FED-4D5C-ABC9-031D4126D22E}"/>
     <hyperlink ref="K17" r:id="rId35" xr:uid="{9B5BFE9E-6F32-44CB-B742-8F98C383FFC8}"/>
     <hyperlink ref="K16" r:id="rId36" xr:uid="{D2299FD8-19C6-40EC-87D3-47DB1FCF2B48}"/>
+    <hyperlink ref="F6" r:id="rId37" xr:uid="{09ED969F-A53F-4C56-9B59-F957DC09F700}"/>
+    <hyperlink ref="F14" r:id="rId38" xr:uid="{8290D6EB-2C2C-4DA7-9590-AD4C08266B1E}"/>
+    <hyperlink ref="F15" r:id="rId39" xr:uid="{1CD33516-C789-4FAB-B9C6-169CF1B70DC5}"/>
+    <hyperlink ref="F7" r:id="rId40" xr:uid="{229A7479-4527-4968-B6D9-CAE0D41ACDF0}"/>
+    <hyperlink ref="F19" r:id="rId41" xr:uid="{3D28C6EF-42B5-4D37-ACF5-11355AFDCA4E}"/>
+    <hyperlink ref="F8" r:id="rId42" xr:uid="{DD39AB34-6BFB-488C-A697-6CE5CF2CA219}"/>
+    <hyperlink ref="F9" r:id="rId43" xr:uid="{C469AE8F-B8D3-4D25-BD0D-AC443A456FD6}"/>
+    <hyperlink ref="F10" r:id="rId44" xr:uid="{9DFC2970-ED47-4C44-A962-A97141C3E676}"/>
+    <hyperlink ref="F16" r:id="rId45" xr:uid="{6CA5A909-7E02-4900-8649-30A568144641}"/>
+    <hyperlink ref="F17" r:id="rId46" xr:uid="{DA36C068-CAF2-4506-8188-70521542F0B5}"/>
+    <hyperlink ref="F18" r:id="rId47" xr:uid="{0637EABE-8F24-4F29-9CDD-70C796857A8F}"/>
+    <hyperlink ref="F11" r:id="rId48" xr:uid="{ED640E93-DD8E-40C3-823C-4D355EF31FC4}"/>
+    <hyperlink ref="F12" r:id="rId49" xr:uid="{098D3FE9-3E35-4560-B3E1-56E25D5AF291}"/>
+    <hyperlink ref="F13" r:id="rId50" xr:uid="{38391B08-8978-4617-A340-7DFCF9171169}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -10889,16 +10991,16 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:12" s="60" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="175" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
       <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:12" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   03-11-2021 - 13:21:30.14
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D7B3FD-4D58-48F8-8319-FF707E2B9E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629047A4-1019-4CC7-AF6E-2D46212FD910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6581,7 +6581,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F19"/>
+      <selection activeCell="L7" sqref="L7:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6707,8 +6707,8 @@
         <v>1067</v>
       </c>
       <c r="L8" t="str">
-        <f>CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
-        <v>|[ K Largest Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/k-largest-elements-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java)|</v>
+        <f t="shared" ref="L8:L19" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|[Articles](",F7,")")</f>
+        <v>|[ K Largest Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/k-largest-elements-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/k_largest_elements/topic)</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6734,8 +6734,8 @@
         <v>1068</v>
       </c>
       <c r="L9" t="str">
-        <f>CONCATENATE("|[",C8,"](",D8,")|[Solution](",K8,")|")</f>
-        <v>|[ Sort K-sorted Array ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/sort-ksorted-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Sort K-sorted Array ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/sort-ksorted-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/sort_a_k_sorted_array/topic)</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6761,8 +6761,8 @@
         <v>1069</v>
       </c>
       <c r="L10" t="str">
-        <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",K9,")|")</f>
-        <v>|[ Median Priority Queue ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/median-priority-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Median Priority Queue ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/median-priority-queue-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/median_priority_queue/topic)</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6791,8 +6791,8 @@
         <v>1070</v>
       </c>
       <c r="L11" t="str">
-        <f>CONCATENATE("|[",C10,"](",D10,")|[Solution](",K10,")|")</f>
-        <v>|[ Merge K Sorted Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/merge-k-sorted-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Merge K Sorted Lists ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/merge-k-sorted-lists-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/merge_k_sorted_lists/topic)</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6818,8 +6818,8 @@
         <v>1071</v>
       </c>
       <c r="L12" t="str">
-        <f>CONCATENATE("|[",C11,"](",D11,")|[Solution](",K11,")|")</f>
-        <v>|[ Hashmap - Introduction](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-intro/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Hashmap - Introduction](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-intro/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/introduction_to_hashmaps/topic)</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6845,8 +6845,8 @@
         <v>1072</v>
       </c>
       <c r="L13" t="str">
-        <f>CONCATENATE("|[",C12,"](",D12,")|[Solution](",K12,")|")</f>
-        <v>|[ Highest Frequency Character ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hfc-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Highest Frequency Character ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hfc-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/highest_frequency_character/topic)</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6875,8 +6875,8 @@
         <v>1073</v>
       </c>
       <c r="L14" t="str">
-        <f>CONCATENATE("|[",C13,"](",D13,")|[Solution](",K13,")|")</f>
-        <v>|[ Get Common Elements - 1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce1-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Get Common Elements - 1 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce1-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/get_common_elements_1/topic)</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6905,8 +6905,8 @@
         <v>1074</v>
       </c>
       <c r="L15" t="str">
-        <f>CONCATENATE("|[",C14,"](",D14,")|[Solution](",K14,")|")</f>
-        <v>|[ Get Common Elements - 2 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce2-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Get Common Elements - 2 ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/gce2-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/get_common_elements_2/topic)</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6932,8 +6932,8 @@
         <v>1075</v>
       </c>
       <c r="L16" t="str">
-        <f>CONCATENATE("|[",C15,"](",D15,")|[Solution](",K15,")|")</f>
-        <v>|[ Longest Consecutive Sequence Of Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/lcqs-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Longest Consecutive Sequence Of Elements ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/lcqs-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/longest_consecutive_sequence/topic)</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6959,8 +6959,8 @@
         <v>1076</v>
       </c>
       <c r="L17" t="str">
-        <f>CONCATENATE("|[",C16,"](",D16,")|[Solution](",K16,")|")</f>
-        <v>|[ Write Priority Queue Using Heap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/priority-queue-using-heap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Write Priority Queue Using Heap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/priority-queue-using-heap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/priority_queue_using_heap/topic)</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6980,8 +6980,8 @@
         <v>1112</v>
       </c>
       <c r="L18" t="str">
-        <f>CONCATENATE("|[",C17,"](",D17,")|[Solution](",K17,")|")</f>
-        <v>|[ Write Hashmap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java)|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Write Hashmap ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/heap-and-hashmap/hashmap-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/write_hashmap/topic)</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7004,8 +7004,8 @@
         <v>681</v>
       </c>
       <c r="L19" t="str">
-        <f>CONCATENATE("|[",C18,"](",D18,")|[Solution](",K18,")|")</f>
-        <v>|[ Efficient Heap Constructor](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/heap-eff-constructor/video)|[Solution]()|</v>
+        <f t="shared" si="0"/>
+        <v>|[ Efficient Heap Constructor](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/heap-eff-constructor/video)|[Solution]()|[Articles](https://www.pepcoding.com/resources/online-java-foundation/hashmap-and-heap/efficient_heap_construction/topic)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-11-2021 - 15:57:00.19
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F970F-4372-48CF-A89F-8012CC98C85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B89B63-E761-4E25-857C-EF9EECD0AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -6935,8 +6935,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:L19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13963,10 +13963,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13980,7 +13980,7 @@
     <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" t="s">
         <v>673</v>
@@ -13989,14 +13989,14 @@
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="C2"/>
       <c r="G2" s="18" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>1</v>
       </c>
@@ -14053,8 +14053,12 @@
       <c r="K4" s="16" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" t="str">
+        <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",K4,")|[Articles](",F4,")")</f>
+        <v>|[ Generic Trees - Introduction And Data Members](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/generic-trees-intro-official/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/introduction_to_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -14076,8 +14080,12 @@
       <c r="K5" s="16" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" t="str">
+        <f t="shared" ref="L5:L33" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",K5,")|[Articles](",F5,")")</f>
+        <v>|[ Generic Tree - Constructor](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/generic-tree-const-official/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/generic_tree_constructor/topic)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>3</v>
       </c>
@@ -14108,8 +14116,12 @@
       <c r="K6" s="16" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Display A Generic Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/display-generic-tree/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/display_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
@@ -14137,8 +14149,12 @@
       <c r="K7" s="16" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Size Of Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/size-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/size_of_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
@@ -14166,8 +14182,12 @@
       <c r="K8" s="16" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Maximum In A Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/max-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/maximum_in_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
@@ -14195,8 +14215,12 @@
       <c r="K9" s="16" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Height Of A Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/height-of-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/height_of_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>7</v>
       </c>
@@ -14227,8 +14251,12 @@
       <c r="K10" s="16" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Generic Tree - Traversals (pre-order, Post-order) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/traversals-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/traversals_in_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
@@ -14259,8 +14287,12 @@
       <c r="K11" s="16" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Level-order Of Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/level-order-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/level_order_of_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -14294,8 +14326,12 @@
       <c r="K12" s="16" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Levelorder Linewise (generic Tree) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/levelorder-linewise-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/level_order_line_wise/topic)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
@@ -14323,8 +14359,12 @@
       <c r="K13" s="16" t="s">
         <v>958</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Levelorder Linewise Zig Zag ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/levelorder-linewise-zigzag-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/levelorder_linewise_zig_zag/topic)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
@@ -14347,8 +14387,12 @@
       <c r="K14" s="16" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Level Order Traversals - More Approaches](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/level-order-traversal-alternates/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/level_order_traversal_more_approaches/topic)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
@@ -14370,8 +14414,12 @@
       <c r="K15" s="16" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Mirror A Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/mirror-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MirrorAGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/mirror_of_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
@@ -14393,8 +14441,12 @@
       <c r="K16" s="16" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Remove Leaves In Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/remove-leaves-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/RemoveLeavesInGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/remove_leaves_in_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -14416,8 +14468,12 @@
       <c r="K17" s="16" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Linearize A Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/linearize-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/linearize_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
@@ -14439,8 +14495,12 @@
       <c r="K18" s="16" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Linearize A Generic Tree - Efficient Approach](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/linearize-gt-efficient/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/linearize_a_generic_tree_efficient_approach/topic)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -14465,8 +14525,12 @@
       <c r="K19" s="16" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Find element In Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/find-in-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/FindElementInGenericTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/find_in_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -14491,8 +14555,12 @@
       <c r="K20" s="16" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Node To Root Path In Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/node-to-root-path-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/NodeToRootPath.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/node_to_root_path_in_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -14517,8 +14585,12 @@
       <c r="K21" s="16" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Lowest Common Ancestor (generic Tree) ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/lca-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LowestCommonAncestor.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/lowest_common_ancestor_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -14546,8 +14618,12 @@
       <c r="K22" s="16" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Distance Between Two Nodes In A Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/distance-between-nodes-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Distancebetween2Nodes.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/distance_between_two_nodes_in_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -14575,8 +14651,12 @@
       <c r="K23" s="16" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Are Trees Similar In Shape ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-generic-trees-similar-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesSimilarInShape.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/are_trees_similar_in_shape/topic)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
@@ -14598,8 +14678,12 @@
       <c r="K24" s="16" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Are Trees Mirror In Shape ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-trees-mirror-in-shape-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java)|[Articles]()</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
@@ -14624,8 +14708,12 @@
       <c r="K25" s="16" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Is Generic Tree Symmetric ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/is-generic-tree-symmetric-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreeSymmetric.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/is_generic_tree_symmetric/topic)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
@@ -14653,8 +14741,12 @@
       <c r="K26" s="16" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Multisolver For Generic Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/multisolver-gt/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Multisolver.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/generic_tree_multisolver/topic)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
@@ -14682,8 +14774,12 @@
       <c r="K27" s="16" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Predecessor And Successor Of An Element ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/pred-succ-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/PredessorAndSuccessorElement.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/predecessor_and_successor_of_an_element/topic)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
@@ -14708,8 +14804,12 @@
       <c r="K28" s="16" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Ceil And Floor In Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/ceil-and-floor-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/CeilAndFloor.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/ceil_and_floor_in_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
@@ -14734,8 +14834,12 @@
       <c r="K29" s="16" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Kth Largest Element In Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/kth-largest-element-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/KthLargestInGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/kth_largest_element_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
@@ -14760,8 +14864,12 @@
       <c r="K30" s="16" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Node With Maximum Subtree Sum ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/node-with-maximum-subtree-sum-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxSumSubtree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/node_with_maximum_subtree_sum/topic)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
@@ -14789,8 +14897,12 @@
       <c r="K31" s="16" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Diameter Of Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/diameter-of-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/DiameterGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/diameter_in_a_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
@@ -14818,8 +14930,12 @@
       <c r="K32" s="16" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Iterative Preorder And Postorder Of Generic Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/iterative-preorder-postorder-generic-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/IterativePreorderPostorderGT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/iterative_pre_order_and_post_order_of_generic_tree/topic)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>30</v>
       </c>
@@ -14841,20 +14957,24 @@
       <c r="K33" s="16" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" s="107" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="L33" t="str">
+        <f t="shared" si="0"/>
+        <v>|[ Iterable And Iterator](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/iterable-iterator-official/video)|[Solution](https://www.youtube.com/watch?v=t4IKNhNBTdo&amp;list=TLGGXv0lFdWAQ5EyMzA5MjAyMQ)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/iterable_and_iterator/topic)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="107" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A45" s="106"/>
       <c r="C45" s="108" t="s">
         <v>544</v>
       </c>
       <c r="D45" s="153"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   04-11-2021 - 15:49:26.67
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B89B63-E761-4E25-857C-EF9EECD0AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A45E2CB-7CB5-4C48-8E97-AA4594ABDA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="1232">
   <si>
     <t>TOPIC</t>
   </si>
@@ -13965,8 +13965,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14669,6 +14669,9 @@
       <c r="E24" t="s">
         <v>6</v>
       </c>
+      <c r="F24" s="16" t="s">
+        <v>1193</v>
+      </c>
       <c r="G24" t="s">
         <v>547</v>
       </c>
@@ -14680,7 +14683,7 @@
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Are Trees Mirror In Shape ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-trees-mirror-in-shape-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java)|[Articles]()</v>
+        <v>|[ Are Trees Mirror In Shape ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/generic-tree/are-trees-mirror-in-shape-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/generic-tree/mirror_of_generic_tree/topic)</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15114,8 +15117,9 @@
     <hyperlink ref="F31" r:id="rId121" xr:uid="{5D39B7C2-D4EA-47BA-887E-BCFAEEBDFD8B}"/>
     <hyperlink ref="F32" r:id="rId122" xr:uid="{F07C787E-1F88-4953-974C-D03F5CD437FC}"/>
     <hyperlink ref="F33" r:id="rId123" xr:uid="{E7F718FB-4210-4D16-8F00-29CA3C0E411D}"/>
+    <hyperlink ref="F24" r:id="rId124" xr:uid="{97BF9C1C-DF60-45F4-9E77-5990901D159A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId124"/>
+  <pageSetup orientation="portrait" r:id="rId125"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   04-11-2021 - 16:36:54.87
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A45E2CB-7CB5-4C48-8E97-AA4594ABDA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44BDB57-AC19-4724-B119-F5DB87A2CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="Linked List" sheetId="5" r:id="rId8"/>
     <sheet name="Generic Tree" sheetId="6" r:id="rId9"/>
     <sheet name="Binary Tree" sheetId="7" r:id="rId10"/>
-    <sheet name="Binary Search Tree" sheetId="8" r:id="rId11"/>
-    <sheet name="Hashmap and Heaps" sheetId="9" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="14" state="hidden" r:id="rId13"/>
-    <sheet name="Graph" sheetId="10" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId11"/>
+    <sheet name="Binary Search Tree" sheetId="8" r:id="rId12"/>
+    <sheet name="Hashmap and Heaps" sheetId="9" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="14" state="hidden" r:id="rId14"/>
+    <sheet name="Graph" sheetId="10" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Sheet1!$A$1:$B$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Sheet1!$A$1:$B$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Sheet2!$C$4:$D$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="1312">
   <si>
     <t>TOPIC</t>
   </si>
@@ -4277,6 +4279,246 @@
   </si>
   <si>
     <t>def</t>
+  </si>
+  <si>
+    <t> Binary Tree - Introduction And Data Members</t>
+  </si>
+  <si>
+    <t> Binary Tree - Constructor</t>
+  </si>
+  <si>
+    <t> Binary Tree Constructor</t>
+  </si>
+  <si>
+    <t> Display A Binary Tree</t>
+  </si>
+  <si>
+    <t> Size, Sum , Max And Height</t>
+  </si>
+  <si>
+    <t> Size, Sum, Maximum And Height Of A Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Traversals In A Binary Tree</t>
+  </si>
+  <si>
+    <t> Traversal In A Binary Tree</t>
+  </si>
+  <si>
+    <t> Level Order Traversal Of Binary Tree</t>
+  </si>
+  <si>
+    <t> Levelorder Traversal Of Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Iterative Pre, Post And Inorder In Binary Tree</t>
+  </si>
+  <si>
+    <t> Iterative Pre, Post And Inorder Traversals Of Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Find Node To Root Path In Binary tree</t>
+  </si>
+  <si>
+    <t> Find And Nodetorootpath In Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Print K Levels Down</t>
+  </si>
+  <si>
+    <t> Print K Levels Down Easy</t>
+  </si>
+  <si>
+    <t> Print Nodes K Distance Away</t>
+  </si>
+  <si>
+    <t> Print Nodes K Distance Away Easy</t>
+  </si>
+  <si>
+    <t> Path To Leaf From Root In Range</t>
+  </si>
+  <si>
+    <t> Path To Leaf From Root In Range Easy</t>
+  </si>
+  <si>
+    <t> Transform To Left Cloned Tree</t>
+  </si>
+  <si>
+    <t> Transform To Left-cloned Tree Easy</t>
+  </si>
+  <si>
+    <t> Transform To Normal From Left Cloned Tree</t>
+  </si>
+  <si>
+    <t> Transform To Normal From Left-cloned Tree Easy</t>
+  </si>
+  <si>
+    <t> Print Single Child Nodes</t>
+  </si>
+  <si>
+    <t> Print Single Child Nodes Easy</t>
+  </si>
+  <si>
+    <t> Remove Leaves In Binary Tree</t>
+  </si>
+  <si>
+    <t> Remove Leaves In Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Diameter of a Binary tree</t>
+  </si>
+  <si>
+    <t> Diameter Of A Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Tilt of a Binary tree</t>
+  </si>
+  <si>
+    <t> Tilt Of Binary Tree Easy</t>
+  </si>
+  <si>
+    <t> Is A Binary Search Tree</t>
+  </si>
+  <si>
+    <t> Is A Binary Search Tree Easy</t>
+  </si>
+  <si>
+    <t> Is balanced tree</t>
+  </si>
+  <si>
+    <t> Is Balanced Tree Easy</t>
+  </si>
+  <si>
+    <t> Largest Bst Subtree Medium</t>
+  </si>
+  <si>
+    <t> Largest Bst subtree</t>
+  </si>
+  <si>
+    <t> Binary Tree Introduction</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-intro/video</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-constructor/video</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_constructor/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-display/video</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/display_a_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size_sum_max_and_height/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size-sum-max-height-binarytree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-traversals/video</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/traversals_in_a_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/level_order_transversal_in_a_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/levelorder-binarytree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative_pre_post_and_inorder_traversals_in_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find_node_to_root_path_in_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Print_k_levels_down/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-k-levels-down-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_nodes_k_distance_away/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Path to leaf from root in range/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_left_cloned_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-left-cloned-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_normal_from_left_cloned_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_single_child_nodes/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-single-child-nodes-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove_leaves_in_binary_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove-leaves-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter_of_a_binary tree /topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter-of-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt_of_a_binary_tree /topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt-of-binary-tree/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_a_binary_search_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-bst-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_balanced_tree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-balanced-binary-tree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest-bst-subtree-official/ojquestion</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest_bst_subtree/topic</t>
+  </si>
+  <si>
+    <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_introduction /topic</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -5860,7 +6102,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M4" sqref="M4:M23"/>
     </sheetView>
   </sheetViews>
@@ -5904,7 +6146,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>455</v>
+        <v>1099</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>10</v>
@@ -5933,8 +6175,8 @@
         <v>979</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="G4" s="5">
-        <v>1</v>
+      <c r="G4" s="172" t="s">
+        <v>1310</v>
       </c>
       <c r="H4" t="s">
         <v>71</v>
@@ -5946,8 +6188,8 @@
         <v>999</v>
       </c>
       <c r="M4" t="str">
-        <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",L4,")|")</f>
-        <v>|[ Binary Tree - Introduction And Data Members](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-intro/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|</v>
+        <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",L4,")|[Articles](",G4,")")</f>
+        <v>|[ Binary Tree - Introduction And Data Members](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-intro/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_introduction /topic)</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5964,8 +6206,8 @@
         <v>980</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="G5" s="5">
-        <v>1</v>
+      <c r="G5" s="172" t="s">
+        <v>1273</v>
       </c>
       <c r="H5" t="s">
         <v>71</v>
@@ -5977,8 +6219,8 @@
         <v>999</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5:M23" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",L5,")|")</f>
-        <v>|[ Binary Tree - Constructor](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-constructor/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|</v>
+        <f t="shared" ref="M5:M23" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",L5,")|[Articles](",G5,")")</f>
+        <v>|[ Binary Tree - Constructor](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-constructor/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_constructor/topic)</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5995,8 +6237,8 @@
         <v>981</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="G6" s="5">
-        <v>1</v>
+      <c r="G6" s="172" t="s">
+        <v>1275</v>
       </c>
       <c r="H6" t="s">
         <v>71</v>
@@ -6009,7 +6251,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Display A Binary Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-display/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|</v>
+        <v>|[ Display A Binary Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-display/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/display_a_binary_tree/topic)</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6026,8 +6268,8 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5">
-        <v>1</v>
+      <c r="G7" s="172" t="s">
+        <v>1276</v>
       </c>
       <c r="H7" t="s">
         <v>71</v>
@@ -6040,7 +6282,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Size, Sum, Maximum And Height Of A Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/size-sum-max-height-binarytree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java)|</v>
+        <v>|[ Size, Sum, Maximum And Height Of A Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/size-sum-max-height-binarytree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size_sum_max_and_height/topic)</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6060,8 +6302,8 @@
       <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="5">
-        <v>11</v>
+      <c r="G8" s="172" t="s">
+        <v>1279</v>
       </c>
       <c r="H8" t="s">
         <v>71</v>
@@ -6074,7 +6316,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Traversals In A Binary Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-traversals/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java)|</v>
+        <v>|[ Traversals In A Binary Tree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-traversals/video)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/traversals_in_a_binary_tree/topic)</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6091,8 +6333,8 @@
       <c r="F9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="5">
-        <v>1</v>
+      <c r="G9" s="172" t="s">
+        <v>1280</v>
       </c>
       <c r="H9" t="s">
         <v>71</v>
@@ -6105,7 +6347,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Levelorder Traversal Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/levelorder-binarytree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java)|</v>
+        <v>|[ Levelorder Traversal Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/levelorder-binarytree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/level_order_transversal_in_a_binary_tree/topic)</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6122,8 +6364,8 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="5">
-        <v>1</v>
+      <c r="G10" s="172" t="s">
+        <v>1282</v>
       </c>
       <c r="H10" t="s">
         <v>71</v>
@@ -6136,7 +6378,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Iterative Pre, Post And Inorder Traversals Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java)|</v>
+        <v>|[ Iterative Pre, Post And Inorder Traversals Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative_pre_post_and_inorder_traversals_in_binary_tree/topic)</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -6153,8 +6395,8 @@
       <c r="F11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="5">
-        <v>1</v>
+      <c r="G11" s="172" t="s">
+        <v>1284</v>
       </c>
       <c r="H11" t="s">
         <v>71</v>
@@ -6167,7 +6409,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Find And Nodetorootpath In Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java)|</v>
+        <v>|[ Find And Nodetorootpath In Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find_node_to_root_path_in_binary_tree/topic)</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -6184,8 +6426,8 @@
       <c r="F12" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="5">
-        <v>1</v>
+      <c r="G12" s="172" t="s">
+        <v>1286</v>
       </c>
       <c r="H12" t="s">
         <v>71</v>
@@ -6198,7 +6440,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Print K Levels Down ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-k-levels-down-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java)|</v>
+        <v>|[ Print K Levels Down ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-k-levels-down-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Print_k_levels_down/topic)</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6215,8 +6457,8 @@
       <c r="F13" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="5">
-        <v>1</v>
+      <c r="G13" s="172" t="s">
+        <v>1288</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>585</v>
@@ -6229,7 +6471,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Print Nodes K Distance Away ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java)|</v>
+        <v>|[ Print Nodes K Distance Away ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_nodes_k_distance_away/topic)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6246,8 +6488,8 @@
       <c r="F14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="5">
-        <v>1</v>
+      <c r="G14" s="172" t="s">
+        <v>1290</v>
       </c>
       <c r="H14" t="s">
         <v>612</v>
@@ -6260,7 +6502,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Path To Leaf From Root In Range ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java)|</v>
+        <v>|[ Path To Leaf From Root In Range ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Path to leaf from root in range/topic)</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -6277,8 +6519,8 @@
       <c r="F15" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="5">
-        <v>1</v>
+      <c r="G15" s="172" t="s">
+        <v>1292</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>620</v>
@@ -6291,7 +6533,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Transform To Left-cloned Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/transform-to-left-cloned-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java)|</v>
+        <v>|[ Transform To Left-cloned Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/transform-to-left-cloned-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_left_cloned_tree/topic)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6308,8 +6550,8 @@
       <c r="F16" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="5">
-        <v>1</v>
+      <c r="G16" s="172" t="s">
+        <v>1294</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>621</v>
@@ -6319,7 +6561,7 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Transform To Normal From Left-cloned Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java)|</v>
+        <v>|[ Transform To Normal From Left-cloned Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_normal_from_left_cloned_tree/topic)</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6336,8 +6578,8 @@
       <c r="F17" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="5">
-        <v>1</v>
+      <c r="G17" s="172" t="s">
+        <v>1296</v>
       </c>
       <c r="H17" t="s">
         <v>617</v>
@@ -6353,7 +6595,7 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Print Single Child Nodes ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-single-child-nodes-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java)|</v>
+        <v>|[ Print Single Child Nodes ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/print-single-child-nodes-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_single_child_nodes/topic)</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -6370,8 +6612,8 @@
       <c r="F18" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="5">
-        <v>1</v>
+      <c r="G18" s="172" t="s">
+        <v>1298</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>624</v>
@@ -6381,7 +6623,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Remove Leaves In Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/remove-leaves-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java)|</v>
+        <v>|[ Remove Leaves In Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/remove-leaves-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove_leaves_in_binary_tree/topic)</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6398,8 +6640,8 @@
       <c r="F19" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="5">
-        <v>1</v>
+      <c r="G19" s="172" t="s">
+        <v>1302</v>
       </c>
       <c r="H19" t="s">
         <v>623</v>
@@ -6412,7 +6654,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Tilt Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/tilt-of-binary-tree/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java)|</v>
+        <v>|[ Tilt Of Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/tilt-of-binary-tree/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt_of_a_binary_tree /topic)</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6429,8 +6671,8 @@
       <c r="F20" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="5">
-        <v>1</v>
+      <c r="G20" s="172" t="s">
+        <v>1304</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>643</v>
@@ -6440,7 +6682,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Is A Binary Search Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/is-bst-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java)|</v>
+        <v>|[ Is A Binary Search Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/is-bst-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_a_binary_search_tree/topic)</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -6457,8 +6699,8 @@
       <c r="F21" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="5">
-        <v>0</v>
+      <c r="G21" s="172" t="s">
+        <v>1306</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>644</v>
@@ -6468,7 +6710,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Is Balanced Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/is-balanced-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java)|</v>
+        <v>|[ Is Balanced Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/is-balanced-binary-tree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_balanced_tree/topic)</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6485,8 +6727,8 @@
       <c r="F22" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="5">
-        <v>0</v>
+      <c r="G22" s="172" t="s">
+        <v>1309</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>645</v>
@@ -6496,7 +6738,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Largest Bst Subtree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/largest-bst-subtree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java)|</v>
+        <v>|[ Largest Bst Subtree](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/largest-bst-subtree-official/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest_bst_subtree/topic)</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -6513,8 +6755,8 @@
       <c r="F23" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="5">
-        <v>0</v>
+      <c r="G23" s="172" t="s">
+        <v>1300</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>622</v>
@@ -6524,8 +6766,11 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
-        <v>|[ Diameter Of A Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/diameter-of-binary-tree/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java)|</v>
-      </c>
+        <v>|[ Diameter Of A Binary Tree ](https://classroom.pepcoding.com/myClassroom/the-switch-program-2/binary-tree/diameter-of-binary-tree/ojquestion)|[Solution](https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java)|[Articles](https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter_of_a_binary tree /topic)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G25" s="172"/>
     </row>
     <row r="37" spans="1:5" s="118" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="117"/>
@@ -6605,13 +6850,488 @@
     <hyperlink ref="K21" r:id="rId59" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java" xr:uid="{47926E29-86F6-41D0-9A87-38F67B694DC2}"/>
     <hyperlink ref="K22" r:id="rId60" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java" xr:uid="{AE4B91D5-62BB-4E14-96B6-B62E7A9B48B6}"/>
     <hyperlink ref="K13" r:id="rId61" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java" xr:uid="{F4B8A9B3-8B83-438A-B0C3-BBD8BB33DDE2}"/>
+    <hyperlink ref="G5" r:id="rId62" xr:uid="{2956A13B-A5F1-4347-8026-8D26ACFE0D7D}"/>
+    <hyperlink ref="G6" r:id="rId63" xr:uid="{7163D36D-0FF2-4A22-A5F2-191B729B69AB}"/>
+    <hyperlink ref="G7" r:id="rId64" xr:uid="{5215A477-2092-4508-B290-F7B6ECBB02E2}"/>
+    <hyperlink ref="G8" r:id="rId65" xr:uid="{1D18D5FD-A58E-4D63-ACB6-CCCE6EE181E4}"/>
+    <hyperlink ref="G9" r:id="rId66" xr:uid="{0C09A442-06FD-48F6-84BB-D253DEC71B58}"/>
+    <hyperlink ref="G10" r:id="rId67" xr:uid="{AA4C3DEB-C132-42F2-9525-73741EAFD8CA}"/>
+    <hyperlink ref="G11" r:id="rId68" xr:uid="{94931CC9-ADA0-43C0-BFA1-E79E27D495F2}"/>
+    <hyperlink ref="G12" r:id="rId69" xr:uid="{DFC180C2-404F-4543-8B93-C346A001119D}"/>
+    <hyperlink ref="G13" r:id="rId70" xr:uid="{1C141227-A8AF-4529-B0E3-F1A9F892AD5F}"/>
+    <hyperlink ref="G14" r:id="rId71" xr:uid="{7000F627-FEF5-41FB-88FC-9E5C3049B56E}"/>
+    <hyperlink ref="G15" r:id="rId72" xr:uid="{A0324302-EDD6-44BC-9125-D33F3BED67B0}"/>
+    <hyperlink ref="G16" r:id="rId73" xr:uid="{5F534A47-F194-436E-93C9-15C51C237A0B}"/>
+    <hyperlink ref="G17" r:id="rId74" xr:uid="{F1A5B49E-C71E-4F80-A820-603C7DD55E0F}"/>
+    <hyperlink ref="G18" r:id="rId75" xr:uid="{03F4942F-05FE-4BEF-AA4F-BA20E27A4C08}"/>
+    <hyperlink ref="G23" r:id="rId76" xr:uid="{0F7051A9-D98F-44C6-9C8D-A5CFAA49B1C7}"/>
+    <hyperlink ref="G19" r:id="rId77" xr:uid="{EA0F8A00-A11E-4417-A985-587B19B17D38}"/>
+    <hyperlink ref="G20" r:id="rId78" xr:uid="{6770C2A1-981A-4891-B247-20D8D05F3FBD}"/>
+    <hyperlink ref="G21" r:id="rId79" xr:uid="{34BB2218-0402-4D34-AFBE-9FEA2A739288}"/>
+    <hyperlink ref="G22" r:id="rId80" xr:uid="{3CABD9A9-A2D4-49DB-9635-3DEB7EC2B92E}"/>
+    <hyperlink ref="G4" r:id="rId81" xr:uid="{887DBCDB-BF96-4F1E-B399-B589DA939821}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId62"/>
+  <pageSetup orientation="portrait" r:id="rId82"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BE486B-21A7-4490-8F97-D3E03752BE85}">
+  <sheetPr codeName="Sheet15" filterMode="1"/>
+  <dimension ref="C4:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="57.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="172" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D5" s="172" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="172" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D6" s="172" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="172" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D7" s="172" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="172" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D8" s="172" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="172" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D9" s="172" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="172" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D10" s="172" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="172" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D11" s="172" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="172" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D12" s="172" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="172" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D13" s="172" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="172" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D14" s="172" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="172" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D15" s="172" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="172" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D16" s="172" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="172" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D17" s="172" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="172" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D18" s="172" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="172" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D19" s="172" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="172" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D20" s="172" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="172" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D21" s="172" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="172" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D22" s="172" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="172" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D23" s="172" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="172" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D24" s="172" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="172" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D25" s="172" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="172" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D26" s="172" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="172" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D27" s="172" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="172" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D28" s="172" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="172" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D29" s="172" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="172" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D30" s="172" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="172" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D31" s="172" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="172" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D32" s="172" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="172" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D33" s="172" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="172" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D34" s="172" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="172" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D35" s="172" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="172" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D36" s="172" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="172" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D37" s="172" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="172" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D38" s="172" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="172" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D39" s="172" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="172" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D40" s="172" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="172" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D41" s="172" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="172" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D42" s="172" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="172" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D43" s="172" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="172" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D44" s="172" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C4:D44" xr:uid="{D8BE486B-21A7-4490-8F97-D3E03752BE85}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_constructor/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_introduction /topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter_of_a_binary tree /topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/display_a_binary_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find_node_to_root_path_in_binary_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_a_binary_search_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_balanced_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative_pre_post_and_inorder_traversals_in_binary_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest_bst_subtree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/level_order_transversal_in_a_binary_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Path to leaf from root in range/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Print_k_levels_down/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_nodes_k_distance_away/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_single_child_nodes/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove_leaves_in_binary_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size_sum_max_and_height/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt_of_a_binary_tree /topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_left_cloned_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_normal_from_left_cloned_tree/topic"/>
+        <filter val="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/traversals_in_a_binary_tree/topic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{24A3FC07-2B3E-41B9-82E8-5C2F44B9267E}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{73EC62DF-C02A-4782-B471-9F691E74A1EF}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{C1A247F4-2020-4324-9618-8823467FA804}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{7F96361E-BE27-477C-80DE-EF4B9564C15D}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{CF46B446-36CA-4F3A-AAB3-44C778BDAA0E}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{D949C3CA-7C2C-4A83-A650-DFCD242F7D13}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{04B0FD9F-546F-493E-8749-506629DB17B9}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{847FCB18-0DE0-4013-AA68-EE105151EF3A}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{331123FD-4DAC-47AD-A46B-6FE9D7B7A1D0}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{17A8567F-F9DD-42FF-BFF1-ED0BB7DDB568}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{A1F3C67E-EFD3-45DE-BE19-D92C88ABB233}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{1827F064-1C44-4D39-ACCA-C660267114D9}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{4FFF90C3-04A9-4E70-9DD2-7E4E2E8CEE9C}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{7CBA4E0B-4519-454D-A2DB-6A9133CBB177}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{1D783AA9-91C2-4E19-B5F8-00F1525A155F}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{E26898F8-F7DF-43D0-B636-11E8AD628889}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{2A347431-1326-44E6-BBBE-E286B23640BD}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{B01E4515-F885-4724-B68B-DD9BF6E0347F}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{D665D0F0-B751-4D82-89E8-8EBB492300FD}"/>
+    <hyperlink ref="D24" r:id="rId20" xr:uid="{B4F7A3F8-75CB-4F83-9865-9018FF525F29}"/>
+    <hyperlink ref="D25" r:id="rId21" xr:uid="{2FCB0A69-5A0A-43AF-ABBD-5B7D6368C914}"/>
+    <hyperlink ref="D26" r:id="rId22" xr:uid="{1F580B66-558C-40B7-91A8-626F65D3FB8E}"/>
+    <hyperlink ref="D27" r:id="rId23" xr:uid="{C7C56B69-4D15-466E-93BA-4589D78D1529}"/>
+    <hyperlink ref="D28" r:id="rId24" xr:uid="{328A3C27-1F1A-4466-92D7-15372A363936}"/>
+    <hyperlink ref="D29" r:id="rId25" xr:uid="{9B5E1E00-B07A-4CEA-B7B1-0FCCD86DD566}"/>
+    <hyperlink ref="D30" r:id="rId26" xr:uid="{7DBB030B-B824-4C84-AEA7-499E9EFC6A3F}"/>
+    <hyperlink ref="D31" r:id="rId27" xr:uid="{8CDB0753-5087-4B20-9509-F5EFA1348A77}"/>
+    <hyperlink ref="D32" r:id="rId28" xr:uid="{B60A00F3-6C5C-47F8-B0F3-F80735893FB1}"/>
+    <hyperlink ref="D33" r:id="rId29" xr:uid="{3D6239B8-8890-428C-A6A2-4568AEB2C521}"/>
+    <hyperlink ref="D34" r:id="rId30" xr:uid="{46F92808-965A-48C4-A944-F0EA4800B102}"/>
+    <hyperlink ref="D35" r:id="rId31" xr:uid="{36574F29-7C54-494F-9463-668F70AED03D}"/>
+    <hyperlink ref="D36" r:id="rId32" xr:uid="{3ADA1F9E-DB80-46F9-8706-882A8D262DB7}"/>
+    <hyperlink ref="D37" r:id="rId33" xr:uid="{88114F59-3FA6-48BA-BE51-340376FAAD7F}"/>
+    <hyperlink ref="D38" r:id="rId34" xr:uid="{47756E9C-57CB-4896-B246-253C2C1C2017}"/>
+    <hyperlink ref="D39" r:id="rId35" xr:uid="{CF56DD27-12DF-480F-A7F4-71ED5A14745C}"/>
+    <hyperlink ref="D40" r:id="rId36" xr:uid="{5E47345F-7C78-4E29-9C1A-FD081DACC99F}"/>
+    <hyperlink ref="D41" r:id="rId37" xr:uid="{1813BC59-9985-46DF-825C-8338894D171F}"/>
+    <hyperlink ref="D42" r:id="rId38" xr:uid="{7809BBD7-56DD-4BC2-9CC5-DCF099CD88F0}"/>
+    <hyperlink ref="D43" r:id="rId39" xr:uid="{2C40B6B2-CDAB-49BA-9440-808DF0865DFC}"/>
+    <hyperlink ref="D44" r:id="rId40" xr:uid="{16C49EB5-7449-442F-BAA2-3BF8E973DA68}"/>
+    <hyperlink ref="C5" r:id="rId41" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-intro/video" xr:uid="{2257EBB5-FD27-4AC2-89EF-CC04AB9005FE}"/>
+    <hyperlink ref="C6" r:id="rId42" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-constructor/video" xr:uid="{566EBBBE-1A96-41A1-8FA6-29482273D1D5}"/>
+    <hyperlink ref="C7" r:id="rId43" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_constructor/topic" xr:uid="{226496AB-CB3E-4D17-8462-47D2055A2F1F}"/>
+    <hyperlink ref="C8" r:id="rId44" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-display/video" xr:uid="{97F642FD-661A-4EDA-B8D5-5535154E5AD2}"/>
+    <hyperlink ref="C9" r:id="rId45" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/display_a_binary_tree/topic" xr:uid="{A20CC5D9-052A-4E61-9D84-BDB89F1C3CFC}"/>
+    <hyperlink ref="C10" r:id="rId46" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size_sum_max_and_height/topic" xr:uid="{C7A2092C-4E46-46E3-B3DA-30F200C132CD}"/>
+    <hyperlink ref="C11" r:id="rId47" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size-sum-max-height-binarytree-official/ojquestion" xr:uid="{14507403-3885-4955-9E17-D5BDE6DE7728}"/>
+    <hyperlink ref="C12" r:id="rId48" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-traversals/video" xr:uid="{2EE1D873-6F95-48D7-9111-DB8C3B7BC31F}"/>
+    <hyperlink ref="C13" r:id="rId49" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/traversals_in_a_binary_tree/topic" xr:uid="{E853193E-63F6-46A8-B90D-B32E87AD0AB3}"/>
+    <hyperlink ref="C14" r:id="rId50" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/level_order_transversal_in_a_binary_tree/topic" xr:uid="{33BFE810-3BB8-47F3-A434-592B3BC75843}"/>
+    <hyperlink ref="C15" r:id="rId51" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/levelorder-binarytree-official/ojquestion" xr:uid="{F9EE5B4D-EABF-49EC-986F-F0B28A2B6D2C}"/>
+    <hyperlink ref="C16" r:id="rId52" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative_pre_post_and_inorder_traversals_in_binary_tree/topic" xr:uid="{D218A2F7-2F01-443D-BBB8-3DCE9ADD14E8}"/>
+    <hyperlink ref="C17" r:id="rId53" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion" xr:uid="{A4E917DA-DFD4-4EBC-883B-BBCB61D603C0}"/>
+    <hyperlink ref="C18" r:id="rId54" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find_node_to_root_path_in_binary_tree/topic" xr:uid="{3D8BDF83-2F06-48DD-9208-04E723079449}"/>
+    <hyperlink ref="C19" r:id="rId55" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion" xr:uid="{0429E290-46F4-4BB3-845A-01B5C0218F72}"/>
+    <hyperlink ref="C20" r:id="rId56" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Print_k_levels_down/topic" xr:uid="{D59498E8-9A91-408D-92F3-F8D520A2A858}"/>
+    <hyperlink ref="C21" r:id="rId57" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-k-levels-down-official/ojquestion" xr:uid="{2F8E188F-9634-4938-AB7A-2189DF71BE2B}"/>
+    <hyperlink ref="C22" r:id="rId58" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_nodes_k_distance_away/topic" xr:uid="{7AD93CD4-4544-4E4F-8B57-FC3CACBDE174}"/>
+    <hyperlink ref="C23" r:id="rId59" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion" xr:uid="{418A4EB0-BFB3-4AC5-918B-600F7D9F387A}"/>
+    <hyperlink ref="C24" r:id="rId60" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Path to leaf from root in range/topic" xr:uid="{AA557FE0-57AE-4D82-BEB6-1979141A2218}"/>
+    <hyperlink ref="C25" r:id="rId61" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion" xr:uid="{26B5940F-C6CE-4D1F-B20B-FE1A70018BC7}"/>
+    <hyperlink ref="C26" r:id="rId62" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_left_cloned_tree/topic" xr:uid="{B3702F57-4733-4A1B-ACF2-2E8E2B248862}"/>
+    <hyperlink ref="C27" r:id="rId63" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-left-cloned-tree-official/ojquestion" xr:uid="{1DB1B16E-9B3A-4066-AD61-B57CACB832B9}"/>
+    <hyperlink ref="C28" r:id="rId64" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_normal_from_left_cloned_tree/topic" xr:uid="{E6C902FE-1521-4D23-BA28-801399BCD608}"/>
+    <hyperlink ref="C29" r:id="rId65" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion" xr:uid="{E4563485-1F55-40E8-8DE1-BD4D5D6E139F}"/>
+    <hyperlink ref="C30" r:id="rId66" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_single_child_nodes/topic" xr:uid="{D8537BA8-7305-4C91-AD84-E7BE8167DDCD}"/>
+    <hyperlink ref="C31" r:id="rId67" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-single-child-nodes-official/ojquestion" xr:uid="{48368993-C6A2-4CBE-91AA-005123D9E846}"/>
+    <hyperlink ref="C32" r:id="rId68" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove_leaves_in_binary_tree/topic" xr:uid="{D8415E7F-65B8-4AFE-B5F3-E634A8D076E2}"/>
+    <hyperlink ref="C33" r:id="rId69" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove-leaves-binary-tree-official/ojquestion" xr:uid="{3106EDB1-C55C-4544-962F-2BE31D31DBBE}"/>
+    <hyperlink ref="C34" r:id="rId70" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter_of_a_binary tree /topic" xr:uid="{D16C8E4F-4DDE-4F5A-B8D9-0D16974E293E}"/>
+    <hyperlink ref="C35" r:id="rId71" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter-of-binary-tree-official/ojquestion" xr:uid="{F3EAF4E4-5711-4771-A51F-464FF0CAF0B6}"/>
+    <hyperlink ref="C36" r:id="rId72" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt_of_a_binary_tree /topic" xr:uid="{8D1495CA-C805-4101-8450-DEB08C1FBC32}"/>
+    <hyperlink ref="C37" r:id="rId73" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt-of-binary-tree/ojquestion" xr:uid="{7A4647B8-C080-42FD-99ED-6150A16F791E}"/>
+    <hyperlink ref="C38" r:id="rId74" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_a_binary_search_tree/topic" xr:uid="{4A1F1342-24C4-4B75-A985-97B5747FC0F6}"/>
+    <hyperlink ref="C39" r:id="rId75" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-bst-official/ojquestion" xr:uid="{F4964919-BB83-4655-B8BD-5F0CA28BF484}"/>
+    <hyperlink ref="C40" r:id="rId76" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_balanced_tree/topic" xr:uid="{DD4D01D2-AA02-428D-AC56-5C220C46ACD9}"/>
+    <hyperlink ref="C41" r:id="rId77" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-balanced-binary-tree-official/ojquestion" xr:uid="{86121917-7142-45F3-9D8C-C2ED668DA9B9}"/>
+    <hyperlink ref="C42" r:id="rId78" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest-bst-subtree-official/ojquestion" xr:uid="{6371934C-BF33-42F7-96C2-DB685AA0AC6B}"/>
+    <hyperlink ref="C43" r:id="rId79" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest_bst_subtree/topic" xr:uid="{4CC4C2B8-A378-451E-AAEB-11F88E112D9F}"/>
+    <hyperlink ref="C44" r:id="rId80" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_introduction /topic" xr:uid="{CEC37375-5ED6-4102-961E-FE3DAD562DC7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L13"/>
@@ -6930,7 +7650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L19"/>
@@ -7425,7 +8145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA793C4-B268-4627-BA9A-70F3F31131C4}">
   <sheetPr codeName="Sheet14" filterMode="1"/>
   <dimension ref="A1:B60"/>
@@ -8081,7 +8801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:L35"/>
@@ -13965,8 +14685,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   04-11-2021 - 16:40:52.96
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44BDB57-AC19-4724-B119-F5DB87A2CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C79D7B-48C7-43AE-A756-923BABBB54B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="1293">
   <si>
     <t>TOPIC</t>
   </si>
@@ -4287,115 +4287,58 @@
     <t> Binary Tree - Constructor</t>
   </si>
   <si>
-    <t> Binary Tree Constructor</t>
-  </si>
-  <si>
     <t> Display A Binary Tree</t>
   </si>
   <si>
-    <t> Size, Sum , Max And Height</t>
-  </si>
-  <si>
     <t> Size, Sum, Maximum And Height Of A Binary Tree Easy</t>
   </si>
   <si>
     <t> Traversals In A Binary Tree</t>
   </si>
   <si>
-    <t> Traversal In A Binary Tree</t>
-  </si>
-  <si>
-    <t> Level Order Traversal Of Binary Tree</t>
-  </si>
-  <si>
     <t> Levelorder Traversal Of Binary Tree Easy</t>
   </si>
   <si>
-    <t> Iterative Pre, Post And Inorder In Binary Tree</t>
-  </si>
-  <si>
     <t> Iterative Pre, Post And Inorder Traversals Of Binary Tree Easy</t>
   </si>
   <si>
-    <t> Find Node To Root Path In Binary tree</t>
-  </si>
-  <si>
     <t> Find And Nodetorootpath In Binary Tree Easy</t>
   </si>
   <si>
-    <t> Print K Levels Down</t>
-  </si>
-  <si>
     <t> Print K Levels Down Easy</t>
   </si>
   <si>
-    <t> Print Nodes K Distance Away</t>
-  </si>
-  <si>
     <t> Print Nodes K Distance Away Easy</t>
   </si>
   <si>
-    <t> Path To Leaf From Root In Range</t>
-  </si>
-  <si>
     <t> Path To Leaf From Root In Range Easy</t>
   </si>
   <si>
-    <t> Transform To Left Cloned Tree</t>
-  </si>
-  <si>
     <t> Transform To Left-cloned Tree Easy</t>
   </si>
   <si>
-    <t> Transform To Normal From Left Cloned Tree</t>
-  </si>
-  <si>
     <t> Transform To Normal From Left-cloned Tree Easy</t>
   </si>
   <si>
-    <t> Print Single Child Nodes</t>
-  </si>
-  <si>
     <t> Print Single Child Nodes Easy</t>
   </si>
   <si>
-    <t> Remove Leaves In Binary Tree</t>
-  </si>
-  <si>
     <t> Remove Leaves In Binary Tree Easy</t>
   </si>
   <si>
-    <t> Diameter of a Binary tree</t>
-  </si>
-  <si>
     <t> Diameter Of A Binary Tree Easy</t>
   </si>
   <si>
-    <t> Tilt of a Binary tree</t>
-  </si>
-  <si>
     <t> Tilt Of Binary Tree Easy</t>
   </si>
   <si>
-    <t> Is A Binary Search Tree</t>
-  </si>
-  <si>
     <t> Is A Binary Search Tree Easy</t>
   </si>
   <si>
-    <t> Is balanced tree</t>
-  </si>
-  <si>
     <t> Is Balanced Tree Easy</t>
   </si>
   <si>
     <t> Largest Bst Subtree Medium</t>
-  </si>
-  <si>
-    <t> Largest Bst subtree</t>
-  </si>
-  <si>
-    <t> Binary Tree Introduction</t>
   </si>
   <si>
     <t>https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-intro/video</t>
@@ -6102,8 +6045,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6176,7 +6119,7 @@
       </c>
       <c r="E4" s="12"/>
       <c r="G4" s="172" t="s">
-        <v>1310</v>
+        <v>1291</v>
       </c>
       <c r="H4" t="s">
         <v>71</v>
@@ -6207,7 +6150,7 @@
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="172" t="s">
-        <v>1273</v>
+        <v>1254</v>
       </c>
       <c r="H5" t="s">
         <v>71</v>
@@ -6238,7 +6181,7 @@
       </c>
       <c r="E6" s="12"/>
       <c r="G6" s="172" t="s">
-        <v>1275</v>
+        <v>1256</v>
       </c>
       <c r="H6" t="s">
         <v>71</v>
@@ -6269,7 +6212,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="172" t="s">
-        <v>1276</v>
+        <v>1257</v>
       </c>
       <c r="H7" t="s">
         <v>71</v>
@@ -6303,7 +6246,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="172" t="s">
-        <v>1279</v>
+        <v>1260</v>
       </c>
       <c r="H8" t="s">
         <v>71</v>
@@ -6334,7 +6277,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="172" t="s">
-        <v>1280</v>
+        <v>1261</v>
       </c>
       <c r="H9" t="s">
         <v>71</v>
@@ -6365,7 +6308,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="172" t="s">
-        <v>1282</v>
+        <v>1263</v>
       </c>
       <c r="H10" t="s">
         <v>71</v>
@@ -6396,7 +6339,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="172" t="s">
-        <v>1284</v>
+        <v>1265</v>
       </c>
       <c r="H11" t="s">
         <v>71</v>
@@ -6427,7 +6370,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="172" t="s">
-        <v>1286</v>
+        <v>1267</v>
       </c>
       <c r="H12" t="s">
         <v>71</v>
@@ -6458,7 +6401,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="172" t="s">
-        <v>1288</v>
+        <v>1269</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>585</v>
@@ -6489,7 +6432,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="172" t="s">
-        <v>1290</v>
+        <v>1271</v>
       </c>
       <c r="H14" t="s">
         <v>612</v>
@@ -6520,7 +6463,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="172" t="s">
-        <v>1292</v>
+        <v>1273</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>620</v>
@@ -6551,7 +6494,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="172" t="s">
-        <v>1294</v>
+        <v>1275</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>621</v>
@@ -6579,7 +6522,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="172" t="s">
-        <v>1296</v>
+        <v>1277</v>
       </c>
       <c r="H17" t="s">
         <v>617</v>
@@ -6613,7 +6556,7 @@
         <v>6</v>
       </c>
       <c r="G18" s="172" t="s">
-        <v>1298</v>
+        <v>1279</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>624</v>
@@ -6641,7 +6584,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="172" t="s">
-        <v>1302</v>
+        <v>1283</v>
       </c>
       <c r="H19" t="s">
         <v>623</v>
@@ -6672,7 +6615,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="172" t="s">
-        <v>1304</v>
+        <v>1285</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>643</v>
@@ -6700,7 +6643,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="172" t="s">
-        <v>1306</v>
+        <v>1287</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>644</v>
@@ -6728,7 +6671,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="172" t="s">
-        <v>1309</v>
+        <v>1290</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>645</v>
@@ -6756,7 +6699,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="172" t="s">
-        <v>1300</v>
+        <v>1281</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>622</v>
@@ -6881,8 +6824,8 @@
   <sheetPr codeName="Sheet15" filterMode="1"/>
   <dimension ref="C4:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6895,7 +6838,7 @@
         <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>1311</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="5" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6903,7 +6846,7 @@
         <v>1232</v>
       </c>
       <c r="D5" s="172" t="s">
-        <v>1271</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="6" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6911,312 +6854,232 @@
         <v>1233</v>
       </c>
       <c r="D6" s="172" t="s">
-        <v>1272</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="172" t="s">
-        <v>1234</v>
-      </c>
-      <c r="D7" s="172" t="s">
-        <v>1273</v>
-      </c>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
     </row>
     <row r="8" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" s="172" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D8" s="172" t="s">
-        <v>1274</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="172" t="s">
-        <v>1235</v>
-      </c>
-      <c r="D9" s="172" t="s">
-        <v>1275</v>
-      </c>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="172" t="s">
-        <v>1236</v>
-      </c>
-      <c r="D10" s="172" t="s">
-        <v>1276</v>
-      </c>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
     </row>
     <row r="11" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" s="172" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="D11" s="172" t="s">
-        <v>1277</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="12" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="172" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="D12" s="172" t="s">
-        <v>1278</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="172" t="s">
-        <v>1239</v>
-      </c>
-      <c r="D13" s="172" t="s">
-        <v>1279</v>
-      </c>
+      <c r="C13" s="172"/>
+      <c r="D13" s="172"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="172" t="s">
-        <v>1240</v>
-      </c>
-      <c r="D14" s="172" t="s">
-        <v>1280</v>
-      </c>
+      <c r="C14" s="172"/>
+      <c r="D14" s="172"/>
     </row>
     <row r="15" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="172" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="D15" s="172" t="s">
-        <v>1281</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="172" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D16" s="172" t="s">
-        <v>1282</v>
-      </c>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
     </row>
     <row r="17" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C17" s="172" t="s">
-        <v>1243</v>
+        <v>1238</v>
       </c>
       <c r="D17" s="172" t="s">
-        <v>1283</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="172" t="s">
-        <v>1244</v>
-      </c>
-      <c r="D18" s="172" t="s">
-        <v>1284</v>
-      </c>
+      <c r="C18" s="172"/>
+      <c r="D18" s="172"/>
     </row>
     <row r="19" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C19" s="172" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="D19" s="172" t="s">
-        <v>1285</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="172" t="s">
-        <v>1246</v>
-      </c>
-      <c r="D20" s="172" t="s">
-        <v>1286</v>
-      </c>
+      <c r="C20" s="172"/>
+      <c r="D20" s="172"/>
     </row>
     <row r="21" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="172" t="s">
-        <v>1247</v>
+        <v>1240</v>
       </c>
       <c r="D21" s="172" t="s">
-        <v>1287</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="172" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D22" s="172" t="s">
-        <v>1288</v>
-      </c>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
     </row>
     <row r="23" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C23" s="172" t="s">
-        <v>1249</v>
+        <v>1241</v>
       </c>
       <c r="D23" s="172" t="s">
-        <v>1289</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="172" t="s">
-        <v>1250</v>
-      </c>
-      <c r="D24" s="172" t="s">
-        <v>1290</v>
-      </c>
+      <c r="C24" s="172"/>
+      <c r="D24" s="172"/>
     </row>
     <row r="25" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C25" s="172" t="s">
-        <v>1251</v>
+        <v>1242</v>
       </c>
       <c r="D25" s="172" t="s">
-        <v>1291</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="172" t="s">
-        <v>1252</v>
-      </c>
-      <c r="D26" s="172" t="s">
-        <v>1292</v>
-      </c>
+      <c r="C26" s="172"/>
+      <c r="D26" s="172"/>
     </row>
     <row r="27" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C27" s="172" t="s">
-        <v>1253</v>
+        <v>1243</v>
       </c>
       <c r="D27" s="172" t="s">
-        <v>1293</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="172" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D28" s="172" t="s">
-        <v>1294</v>
-      </c>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
     </row>
     <row r="29" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C29" s="172" t="s">
-        <v>1255</v>
+        <v>1244</v>
       </c>
       <c r="D29" s="172" t="s">
-        <v>1295</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="172" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D30" s="172" t="s">
-        <v>1296</v>
-      </c>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
     </row>
     <row r="31" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C31" s="172" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
       <c r="D31" s="172" t="s">
-        <v>1297</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="172" t="s">
-        <v>1258</v>
-      </c>
-      <c r="D32" s="172" t="s">
-        <v>1298</v>
-      </c>
+      <c r="C32" s="172"/>
+      <c r="D32" s="172"/>
     </row>
     <row r="33" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C33" s="172" t="s">
-        <v>1259</v>
+        <v>1246</v>
       </c>
       <c r="D33" s="172" t="s">
-        <v>1299</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="172" t="s">
-        <v>1260</v>
-      </c>
-      <c r="D34" s="172" t="s">
-        <v>1300</v>
-      </c>
+      <c r="C34" s="172"/>
+      <c r="D34" s="172"/>
     </row>
     <row r="35" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35" s="172" t="s">
-        <v>1261</v>
+        <v>1247</v>
       </c>
       <c r="D35" s="172" t="s">
-        <v>1301</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="172" t="s">
-        <v>1262</v>
-      </c>
-      <c r="D36" s="172" t="s">
-        <v>1302</v>
-      </c>
+      <c r="C36" s="172"/>
+      <c r="D36" s="172"/>
     </row>
     <row r="37" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C37" s="172" t="s">
-        <v>1263</v>
+        <v>1248</v>
       </c>
       <c r="D37" s="172" t="s">
-        <v>1303</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="172" t="s">
-        <v>1264</v>
-      </c>
-      <c r="D38" s="172" t="s">
-        <v>1304</v>
-      </c>
+      <c r="C38" s="172"/>
+      <c r="D38" s="172"/>
     </row>
     <row r="39" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C39" s="172" t="s">
-        <v>1265</v>
+        <v>1249</v>
       </c>
       <c r="D39" s="172" t="s">
-        <v>1305</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="172" t="s">
-        <v>1266</v>
-      </c>
-      <c r="D40" s="172" t="s">
-        <v>1306</v>
-      </c>
+      <c r="C40" s="172"/>
+      <c r="D40" s="172"/>
     </row>
     <row r="41" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C41" s="172" t="s">
-        <v>1267</v>
+        <v>1250</v>
       </c>
       <c r="D41" s="172" t="s">
-        <v>1307</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="42" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C42" s="172" t="s">
-        <v>1268</v>
+        <v>1251</v>
       </c>
       <c r="D42" s="172" t="s">
-        <v>1308</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="172" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D43" s="172" t="s">
-        <v>1309</v>
-      </c>
+      <c r="C43" s="172"/>
+      <c r="D43" s="172"/>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="172" t="s">
-        <v>1270</v>
-      </c>
-      <c r="D44" s="172" t="s">
-        <v>1310</v>
-      </c>
+      <c r="C44" s="172"/>
+      <c r="D44" s="172"/>
     </row>
   </sheetData>
   <autoFilter ref="C4:D44" xr:uid="{D8BE486B-21A7-4490-8F97-D3E03752BE85}">
@@ -7248,84 +7111,44 @@
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{24A3FC07-2B3E-41B9-82E8-5C2F44B9267E}"/>
     <hyperlink ref="D6" r:id="rId2" xr:uid="{73EC62DF-C02A-4782-B471-9F691E74A1EF}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{C1A247F4-2020-4324-9618-8823467FA804}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{7F96361E-BE27-477C-80DE-EF4B9564C15D}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{CF46B446-36CA-4F3A-AAB3-44C778BDAA0E}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{D949C3CA-7C2C-4A83-A650-DFCD242F7D13}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{04B0FD9F-546F-493E-8749-506629DB17B9}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{847FCB18-0DE0-4013-AA68-EE105151EF3A}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{331123FD-4DAC-47AD-A46B-6FE9D7B7A1D0}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{17A8567F-F9DD-42FF-BFF1-ED0BB7DDB568}"/>
-    <hyperlink ref="D15" r:id="rId11" xr:uid="{A1F3C67E-EFD3-45DE-BE19-D92C88ABB233}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{1827F064-1C44-4D39-ACCA-C660267114D9}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{4FFF90C3-04A9-4E70-9DD2-7E4E2E8CEE9C}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{7CBA4E0B-4519-454D-A2DB-6A9133CBB177}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{1D783AA9-91C2-4E19-B5F8-00F1525A155F}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{E26898F8-F7DF-43D0-B636-11E8AD628889}"/>
-    <hyperlink ref="D21" r:id="rId17" xr:uid="{2A347431-1326-44E6-BBBE-E286B23640BD}"/>
-    <hyperlink ref="D22" r:id="rId18" xr:uid="{B01E4515-F885-4724-B68B-DD9BF6E0347F}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{D665D0F0-B751-4D82-89E8-8EBB492300FD}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{B4F7A3F8-75CB-4F83-9865-9018FF525F29}"/>
-    <hyperlink ref="D25" r:id="rId21" xr:uid="{2FCB0A69-5A0A-43AF-ABBD-5B7D6368C914}"/>
-    <hyperlink ref="D26" r:id="rId22" xr:uid="{1F580B66-558C-40B7-91A8-626F65D3FB8E}"/>
-    <hyperlink ref="D27" r:id="rId23" xr:uid="{C7C56B69-4D15-466E-93BA-4589D78D1529}"/>
-    <hyperlink ref="D28" r:id="rId24" xr:uid="{328A3C27-1F1A-4466-92D7-15372A363936}"/>
-    <hyperlink ref="D29" r:id="rId25" xr:uid="{9B5E1E00-B07A-4CEA-B7B1-0FCCD86DD566}"/>
-    <hyperlink ref="D30" r:id="rId26" xr:uid="{7DBB030B-B824-4C84-AEA7-499E9EFC6A3F}"/>
-    <hyperlink ref="D31" r:id="rId27" xr:uid="{8CDB0753-5087-4B20-9509-F5EFA1348A77}"/>
-    <hyperlink ref="D32" r:id="rId28" xr:uid="{B60A00F3-6C5C-47F8-B0F3-F80735893FB1}"/>
-    <hyperlink ref="D33" r:id="rId29" xr:uid="{3D6239B8-8890-428C-A6A2-4568AEB2C521}"/>
-    <hyperlink ref="D34" r:id="rId30" xr:uid="{46F92808-965A-48C4-A944-F0EA4800B102}"/>
-    <hyperlink ref="D35" r:id="rId31" xr:uid="{36574F29-7C54-494F-9463-668F70AED03D}"/>
-    <hyperlink ref="D36" r:id="rId32" xr:uid="{3ADA1F9E-DB80-46F9-8706-882A8D262DB7}"/>
-    <hyperlink ref="D37" r:id="rId33" xr:uid="{88114F59-3FA6-48BA-BE51-340376FAAD7F}"/>
-    <hyperlink ref="D38" r:id="rId34" xr:uid="{47756E9C-57CB-4896-B246-253C2C1C2017}"/>
-    <hyperlink ref="D39" r:id="rId35" xr:uid="{CF56DD27-12DF-480F-A7F4-71ED5A14745C}"/>
-    <hyperlink ref="D40" r:id="rId36" xr:uid="{5E47345F-7C78-4E29-9C1A-FD081DACC99F}"/>
-    <hyperlink ref="D41" r:id="rId37" xr:uid="{1813BC59-9985-46DF-825C-8338894D171F}"/>
-    <hyperlink ref="D42" r:id="rId38" xr:uid="{7809BBD7-56DD-4BC2-9CC5-DCF099CD88F0}"/>
-    <hyperlink ref="D43" r:id="rId39" xr:uid="{2C40B6B2-CDAB-49BA-9440-808DF0865DFC}"/>
-    <hyperlink ref="D44" r:id="rId40" xr:uid="{16C49EB5-7449-442F-BAA2-3BF8E973DA68}"/>
-    <hyperlink ref="C5" r:id="rId41" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-intro/video" xr:uid="{2257EBB5-FD27-4AC2-89EF-CC04AB9005FE}"/>
-    <hyperlink ref="C6" r:id="rId42" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-constructor/video" xr:uid="{566EBBBE-1A96-41A1-8FA6-29482273D1D5}"/>
-    <hyperlink ref="C7" r:id="rId43" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_constructor/topic" xr:uid="{226496AB-CB3E-4D17-8462-47D2055A2F1F}"/>
-    <hyperlink ref="C8" r:id="rId44" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-display/video" xr:uid="{97F642FD-661A-4EDA-B8D5-5535154E5AD2}"/>
-    <hyperlink ref="C9" r:id="rId45" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/display_a_binary_tree/topic" xr:uid="{A20CC5D9-052A-4E61-9D84-BDB89F1C3CFC}"/>
-    <hyperlink ref="C10" r:id="rId46" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size_sum_max_and_height/topic" xr:uid="{C7A2092C-4E46-46E3-B3DA-30F200C132CD}"/>
-    <hyperlink ref="C11" r:id="rId47" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size-sum-max-height-binarytree-official/ojquestion" xr:uid="{14507403-3885-4955-9E17-D5BDE6DE7728}"/>
-    <hyperlink ref="C12" r:id="rId48" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-traversals/video" xr:uid="{2EE1D873-6F95-48D7-9111-DB8C3B7BC31F}"/>
-    <hyperlink ref="C13" r:id="rId49" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/traversals_in_a_binary_tree/topic" xr:uid="{E853193E-63F6-46A8-B90D-B32E87AD0AB3}"/>
-    <hyperlink ref="C14" r:id="rId50" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/level_order_transversal_in_a_binary_tree/topic" xr:uid="{33BFE810-3BB8-47F3-A434-592B3BC75843}"/>
-    <hyperlink ref="C15" r:id="rId51" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/levelorder-binarytree-official/ojquestion" xr:uid="{F9EE5B4D-EABF-49EC-986F-F0B28A2B6D2C}"/>
-    <hyperlink ref="C16" r:id="rId52" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative_pre_post_and_inorder_traversals_in_binary_tree/topic" xr:uid="{D218A2F7-2F01-443D-BBB8-3DCE9ADD14E8}"/>
-    <hyperlink ref="C17" r:id="rId53" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion" xr:uid="{A4E917DA-DFD4-4EBC-883B-BBCB61D603C0}"/>
-    <hyperlink ref="C18" r:id="rId54" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find_node_to_root_path_in_binary_tree/topic" xr:uid="{3D8BDF83-2F06-48DD-9208-04E723079449}"/>
-    <hyperlink ref="C19" r:id="rId55" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion" xr:uid="{0429E290-46F4-4BB3-845A-01B5C0218F72}"/>
-    <hyperlink ref="C20" r:id="rId56" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Print_k_levels_down/topic" xr:uid="{D59498E8-9A91-408D-92F3-F8D520A2A858}"/>
-    <hyperlink ref="C21" r:id="rId57" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-k-levels-down-official/ojquestion" xr:uid="{2F8E188F-9634-4938-AB7A-2189DF71BE2B}"/>
-    <hyperlink ref="C22" r:id="rId58" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_nodes_k_distance_away/topic" xr:uid="{7AD93CD4-4544-4E4F-8B57-FC3CACBDE174}"/>
-    <hyperlink ref="C23" r:id="rId59" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion" xr:uid="{418A4EB0-BFB3-4AC5-918B-600F7D9F387A}"/>
-    <hyperlink ref="C24" r:id="rId60" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/Path to leaf from root in range/topic" xr:uid="{AA557FE0-57AE-4D82-BEB6-1979141A2218}"/>
-    <hyperlink ref="C25" r:id="rId61" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion" xr:uid="{26B5940F-C6CE-4D1F-B20B-FE1A70018BC7}"/>
-    <hyperlink ref="C26" r:id="rId62" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_left_cloned_tree/topic" xr:uid="{B3702F57-4733-4A1B-ACF2-2E8E2B248862}"/>
-    <hyperlink ref="C27" r:id="rId63" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-left-cloned-tree-official/ojquestion" xr:uid="{1DB1B16E-9B3A-4066-AD61-B57CACB832B9}"/>
-    <hyperlink ref="C28" r:id="rId64" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform_to_normal_from_left_cloned_tree/topic" xr:uid="{E6C902FE-1521-4D23-BA28-801399BCD608}"/>
-    <hyperlink ref="C29" r:id="rId65" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion" xr:uid="{E4563485-1F55-40E8-8DE1-BD4D5D6E139F}"/>
-    <hyperlink ref="C30" r:id="rId66" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print_single_child_nodes/topic" xr:uid="{D8537BA8-7305-4C91-AD84-E7BE8167DDCD}"/>
-    <hyperlink ref="C31" r:id="rId67" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-single-child-nodes-official/ojquestion" xr:uid="{48368993-C6A2-4CBE-91AA-005123D9E846}"/>
-    <hyperlink ref="C32" r:id="rId68" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove_leaves_in_binary_tree/topic" xr:uid="{D8415E7F-65B8-4AFE-B5F3-E634A8D076E2}"/>
-    <hyperlink ref="C33" r:id="rId69" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove-leaves-binary-tree-official/ojquestion" xr:uid="{3106EDB1-C55C-4544-962F-2BE31D31DBBE}"/>
-    <hyperlink ref="C34" r:id="rId70" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter_of_a_binary tree /topic" xr:uid="{D16C8E4F-4DDE-4F5A-B8D9-0D16974E293E}"/>
-    <hyperlink ref="C35" r:id="rId71" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter-of-binary-tree-official/ojquestion" xr:uid="{F3EAF4E4-5711-4771-A51F-464FF0CAF0B6}"/>
-    <hyperlink ref="C36" r:id="rId72" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt_of_a_binary_tree /topic" xr:uid="{8D1495CA-C805-4101-8450-DEB08C1FBC32}"/>
-    <hyperlink ref="C37" r:id="rId73" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt-of-binary-tree/ojquestion" xr:uid="{7A4647B8-C080-42FD-99ED-6150A16F791E}"/>
-    <hyperlink ref="C38" r:id="rId74" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_a_binary_search_tree/topic" xr:uid="{4A1F1342-24C4-4B75-A985-97B5747FC0F6}"/>
-    <hyperlink ref="C39" r:id="rId75" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-bst-official/ojquestion" xr:uid="{F4964919-BB83-4655-B8BD-5F0CA28BF484}"/>
-    <hyperlink ref="C40" r:id="rId76" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is_balanced_tree/topic" xr:uid="{DD4D01D2-AA02-428D-AC56-5C220C46ACD9}"/>
-    <hyperlink ref="C41" r:id="rId77" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-balanced-binary-tree-official/ojquestion" xr:uid="{86121917-7142-45F3-9D8C-C2ED668DA9B9}"/>
-    <hyperlink ref="C42" r:id="rId78" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest-bst-subtree-official/ojquestion" xr:uid="{6371934C-BF33-42F7-96C2-DB685AA0AC6B}"/>
-    <hyperlink ref="C43" r:id="rId79" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest_bst_subtree/topic" xr:uid="{4CC4C2B8-A378-451E-AAEB-11F88E112D9F}"/>
-    <hyperlink ref="C44" r:id="rId80" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary_tree_introduction /topic" xr:uid="{CEC37375-5ED6-4102-961E-FE3DAD562DC7}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{7F96361E-BE27-477C-80DE-EF4B9564C15D}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{04B0FD9F-546F-493E-8749-506629DB17B9}"/>
+    <hyperlink ref="D12" r:id="rId5" xr:uid="{847FCB18-0DE0-4013-AA68-EE105151EF3A}"/>
+    <hyperlink ref="D15" r:id="rId6" xr:uid="{A1F3C67E-EFD3-45DE-BE19-D92C88ABB233}"/>
+    <hyperlink ref="D17" r:id="rId7" xr:uid="{4FFF90C3-04A9-4E70-9DD2-7E4E2E8CEE9C}"/>
+    <hyperlink ref="D19" r:id="rId8" xr:uid="{1D783AA9-91C2-4E19-B5F8-00F1525A155F}"/>
+    <hyperlink ref="D21" r:id="rId9" xr:uid="{2A347431-1326-44E6-BBBE-E286B23640BD}"/>
+    <hyperlink ref="D23" r:id="rId10" xr:uid="{D665D0F0-B751-4D82-89E8-8EBB492300FD}"/>
+    <hyperlink ref="D25" r:id="rId11" xr:uid="{2FCB0A69-5A0A-43AF-ABBD-5B7D6368C914}"/>
+    <hyperlink ref="D27" r:id="rId12" xr:uid="{C7C56B69-4D15-466E-93BA-4589D78D1529}"/>
+    <hyperlink ref="D29" r:id="rId13" xr:uid="{9B5E1E00-B07A-4CEA-B7B1-0FCCD86DD566}"/>
+    <hyperlink ref="D31" r:id="rId14" xr:uid="{8CDB0753-5087-4B20-9509-F5EFA1348A77}"/>
+    <hyperlink ref="D33" r:id="rId15" xr:uid="{3D6239B8-8890-428C-A6A2-4568AEB2C521}"/>
+    <hyperlink ref="D35" r:id="rId16" xr:uid="{36574F29-7C54-494F-9463-668F70AED03D}"/>
+    <hyperlink ref="D37" r:id="rId17" xr:uid="{88114F59-3FA6-48BA-BE51-340376FAAD7F}"/>
+    <hyperlink ref="D39" r:id="rId18" xr:uid="{CF56DD27-12DF-480F-A7F4-71ED5A14745C}"/>
+    <hyperlink ref="D41" r:id="rId19" xr:uid="{1813BC59-9985-46DF-825C-8338894D171F}"/>
+    <hyperlink ref="D42" r:id="rId20" xr:uid="{7809BBD7-56DD-4BC2-9CC5-DCF099CD88F0}"/>
+    <hyperlink ref="C5" r:id="rId21" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-intro/video" xr:uid="{2257EBB5-FD27-4AC2-89EF-CC04AB9005FE}"/>
+    <hyperlink ref="C6" r:id="rId22" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-constructor/video" xr:uid="{566EBBBE-1A96-41A1-8FA6-29482273D1D5}"/>
+    <hyperlink ref="C8" r:id="rId23" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-display/video" xr:uid="{97F642FD-661A-4EDA-B8D5-5535154E5AD2}"/>
+    <hyperlink ref="C11" r:id="rId24" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/size-sum-max-height-binarytree-official/ojquestion" xr:uid="{14507403-3885-4955-9E17-D5BDE6DE7728}"/>
+    <hyperlink ref="C12" r:id="rId25" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-traversals/video" xr:uid="{2EE1D873-6F95-48D7-9111-DB8C3B7BC31F}"/>
+    <hyperlink ref="C15" r:id="rId26" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/levelorder-binarytree-official/ojquestion" xr:uid="{F9EE5B4D-EABF-49EC-986F-F0B28A2B6D2C}"/>
+    <hyperlink ref="C17" r:id="rId27" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/iterative-pre-post-in-binary-tree-official/ojquestion" xr:uid="{A4E917DA-DFD4-4EBC-883B-BBCB61D603C0}"/>
+    <hyperlink ref="C19" r:id="rId28" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/find-nodetorootpath-binary-tree-official/ojquestion" xr:uid="{0429E290-46F4-4BB3-845A-01B5C0218F72}"/>
+    <hyperlink ref="C21" r:id="rId29" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-k-levels-down-official/ojquestion" xr:uid="{2F8E188F-9634-4938-AB7A-2189DF71BE2B}"/>
+    <hyperlink ref="C23" r:id="rId30" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-nodes-k-away-binary-tree-official/ojquestion" xr:uid="{418A4EB0-BFB3-4AC5-918B-600F7D9F387A}"/>
+    <hyperlink ref="C25" r:id="rId31" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/binary-tree-path-to-leaves-from-root-official/ojquestion" xr:uid="{26B5940F-C6CE-4D1F-B20B-FE1A70018BC7}"/>
+    <hyperlink ref="C27" r:id="rId32" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-left-cloned-tree-official/ojquestion" xr:uid="{1DB1B16E-9B3A-4066-AD61-B57CACB832B9}"/>
+    <hyperlink ref="C29" r:id="rId33" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/transform-to-normal-from-left-cloned-tree-official/ojquestion" xr:uid="{E4563485-1F55-40E8-8DE1-BD4D5D6E139F}"/>
+    <hyperlink ref="C31" r:id="rId34" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/print-single-child-nodes-official/ojquestion" xr:uid="{48368993-C6A2-4CBE-91AA-005123D9E846}"/>
+    <hyperlink ref="C33" r:id="rId35" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/remove-leaves-binary-tree-official/ojquestion" xr:uid="{3106EDB1-C55C-4544-962F-2BE31D31DBBE}"/>
+    <hyperlink ref="C35" r:id="rId36" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/diameter-of-binary-tree-official/ojquestion" xr:uid="{F3EAF4E4-5711-4771-A51F-464FF0CAF0B6}"/>
+    <hyperlink ref="C37" r:id="rId37" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/tilt-of-binary-tree/ojquestion" xr:uid="{7A4647B8-C080-42FD-99ED-6150A16F791E}"/>
+    <hyperlink ref="C39" r:id="rId38" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-bst-official/ojquestion" xr:uid="{F4964919-BB83-4655-B8BD-5F0CA28BF484}"/>
+    <hyperlink ref="C41" r:id="rId39" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/is-balanced-binary-tree-official/ojquestion" xr:uid="{86121917-7142-45F3-9D8C-C2ED668DA9B9}"/>
+    <hyperlink ref="C42" r:id="rId40" display="https://www.pepcoding.com/resources/online-java-foundation/binary-tree/largest-bst-subtree-official/ojquestion" xr:uid="{6371934C-BF33-42F7-96C2-DB685AA0AC6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   04-11-2021 - 21:45:11.20
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C79D7B-48C7-43AE-A756-923BABBB54B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED77D8-03F8-43C1-90B8-EB209512F7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" tabRatio="852" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Linked List" sheetId="5" r:id="rId8"/>
     <sheet name="Generic Tree" sheetId="6" r:id="rId9"/>
     <sheet name="Binary Tree" sheetId="7" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="15" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="15" state="hidden" r:id="rId11"/>
     <sheet name="Binary Search Tree" sheetId="8" r:id="rId12"/>
     <sheet name="Hashmap and Heaps" sheetId="9" r:id="rId13"/>
     <sheet name="Sheet1" sheetId="14" state="hidden" r:id="rId14"/>
@@ -6045,7 +6045,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -6824,7 +6824,7 @@
   <sheetPr codeName="Sheet15" filterMode="1"/>
   <dimension ref="C4:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:D44"/>
     </sheetView>
   </sheetViews>
@@ -7159,8 +7159,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   16-01-2022 -  1:03:08.48
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED77D8-03F8-43C1-90B8-EB209512F7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B45D69-4AD2-4369-992D-438EF8751A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" tabRatio="852" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="1291">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2770,12 +2770,6 @@
   </si>
   <si>
     <t>dp5</t>
-  </si>
-  <si>
-    <t>sun morning</t>
-  </si>
-  <si>
-    <t>sum eve</t>
   </si>
   <si>
     <t>Notes</t>
@@ -6045,7 +6039,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -6089,7 +6083,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>10</v>
@@ -6115,11 +6109,11 @@
         <v>232</v>
       </c>
       <c r="D4" s="150" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E4" s="12"/>
       <c r="G4" s="172" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="H4" t="s">
         <v>71</v>
@@ -6128,7 +6122,7 @@
         <v>607</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",L4,")|[Articles](",G4,")")</f>
@@ -6146,11 +6140,11 @@
         <v>233</v>
       </c>
       <c r="D5" s="150" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="172" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="H5" t="s">
         <v>71</v>
@@ -6159,7 +6153,7 @@
         <v>607</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M23" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",L5,")|[Articles](",G5,")")</f>
@@ -6177,11 +6171,11 @@
         <v>234</v>
       </c>
       <c r="D6" s="150" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="E6" s="12"/>
       <c r="G6" s="172" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="H6" t="s">
         <v>71</v>
@@ -6190,7 +6184,7 @@
         <v>607</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -6205,14 +6199,14 @@
         <v>235</v>
       </c>
       <c r="D7" s="172" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="172" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="H7" t="s">
         <v>71</v>
@@ -6221,7 +6215,7 @@
         <v>608</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
@@ -6239,14 +6233,14 @@
         <v>236</v>
       </c>
       <c r="D8" s="172" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="172" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="H8" t="s">
         <v>71</v>
@@ -6255,7 +6249,7 @@
         <v>609</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
@@ -6270,14 +6264,14 @@
         <v>237</v>
       </c>
       <c r="D9" s="172" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="172" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="H9" t="s">
         <v>71</v>
@@ -6286,7 +6280,7 @@
         <v>530</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
@@ -6301,14 +6295,14 @@
         <v>238</v>
       </c>
       <c r="D10" s="172" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="172" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="H10" t="s">
         <v>71</v>
@@ -6317,7 +6311,7 @@
         <v>610</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
@@ -6332,14 +6326,14 @@
         <v>239</v>
       </c>
       <c r="D11" s="172" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="172" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="H11" t="s">
         <v>71</v>
@@ -6348,7 +6342,7 @@
         <v>600</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
@@ -6363,14 +6357,14 @@
         <v>240</v>
       </c>
       <c r="D12" s="172" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="172" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="H12" t="s">
         <v>71</v>
@@ -6379,7 +6373,7 @@
         <v>611</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
@@ -6394,14 +6388,14 @@
         <v>241</v>
       </c>
       <c r="D13" s="172" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="172" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>585</v>
@@ -6410,7 +6404,7 @@
         <v>647</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
@@ -6425,14 +6419,14 @@
         <v>242</v>
       </c>
       <c r="D14" s="172" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="172" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="H14" t="s">
         <v>612</v>
@@ -6441,7 +6435,7 @@
         <v>613</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -6456,14 +6450,14 @@
         <v>243</v>
       </c>
       <c r="D15" s="172" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="172" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>620</v>
@@ -6472,7 +6466,7 @@
         <v>619</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
@@ -6487,20 +6481,20 @@
         <v>244</v>
       </c>
       <c r="D16" s="172" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="172" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>621</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -6515,14 +6509,14 @@
         <v>245</v>
       </c>
       <c r="D17" s="172" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="172" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="H17" t="s">
         <v>617</v>
@@ -6534,7 +6528,7 @@
         <v>616</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -6549,20 +6543,20 @@
         <v>246</v>
       </c>
       <c r="D18" s="172" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="172" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>624</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -6577,14 +6571,14 @@
         <v>248</v>
       </c>
       <c r="D19" s="172" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="172" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="H19" t="s">
         <v>623</v>
@@ -6593,7 +6587,7 @@
         <v>625</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -6608,20 +6602,20 @@
         <v>249</v>
       </c>
       <c r="D20" s="172" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="172" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>643</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -6636,20 +6630,20 @@
         <v>250</v>
       </c>
       <c r="D21" s="172" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="172" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>644</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -6664,20 +6658,20 @@
         <v>251</v>
       </c>
       <c r="D22" s="172" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="172" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>645</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
@@ -6692,20 +6686,20 @@
         <v>247</v>
       </c>
       <c r="D23" s="172" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="172" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>622</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -6838,23 +6832,23 @@
         <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="5" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C5" s="172" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="D5" s="172" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="6" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C6" s="172" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="D6" s="172" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
@@ -6863,10 +6857,10 @@
     </row>
     <row r="8" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" s="172" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="D8" s="172" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
@@ -6879,18 +6873,18 @@
     </row>
     <row r="11" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" s="172" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="D11" s="172" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="12" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="172" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="D12" s="172" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
@@ -6903,10 +6897,10 @@
     </row>
     <row r="15" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="172" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="D15" s="172" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
@@ -6915,10 +6909,10 @@
     </row>
     <row r="17" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C17" s="172" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="D17" s="172" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
@@ -6927,10 +6921,10 @@
     </row>
     <row r="19" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C19" s="172" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="D19" s="172" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
@@ -6939,10 +6933,10 @@
     </row>
     <row r="21" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="172" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="D21" s="172" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
@@ -6951,10 +6945,10 @@
     </row>
     <row r="23" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C23" s="172" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="D23" s="172" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
@@ -6963,10 +6957,10 @@
     </row>
     <row r="25" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C25" s="172" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="D25" s="172" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
@@ -6975,10 +6969,10 @@
     </row>
     <row r="27" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C27" s="172" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="D27" s="172" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -6987,10 +6981,10 @@
     </row>
     <row r="29" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C29" s="172" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D29" s="172" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
@@ -6999,10 +6993,10 @@
     </row>
     <row r="31" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C31" s="172" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D31" s="172" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
@@ -7011,10 +7005,10 @@
     </row>
     <row r="33" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C33" s="172" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D33" s="172" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
@@ -7023,10 +7017,10 @@
     </row>
     <row r="35" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35" s="172" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="D35" s="172" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
@@ -7035,10 +7029,10 @@
     </row>
     <row r="37" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C37" s="172" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="D37" s="172" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
@@ -7047,10 +7041,10 @@
     </row>
     <row r="39" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C39" s="172" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="D39" s="172" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
@@ -7059,18 +7053,18 @@
     </row>
     <row r="41" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C41" s="172" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="D41" s="172" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="42" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C42" s="172" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="D42" s="172" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
@@ -7225,7 +7219,7 @@
         <v>252</v>
       </c>
       <c r="D4" s="150" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -7246,7 +7240,7 @@
         <v>253</v>
       </c>
       <c r="D5" s="150" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -7264,7 +7258,7 @@
         <v>254</v>
       </c>
       <c r="D6" s="150" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -7273,7 +7267,7 @@
         <v>664</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="L6" t="str">
         <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|")</f>
@@ -7288,7 +7282,7 @@
         <v>255</v>
       </c>
       <c r="D7" s="150" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -7297,7 +7291,7 @@
         <v>661</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L13" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|")</f>
@@ -7312,7 +7306,7 @@
         <v>257</v>
       </c>
       <c r="D8" s="150" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -7327,7 +7321,7 @@
         <v>258</v>
       </c>
       <c r="D9" s="150" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -7336,7 +7330,7 @@
         <v>663</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -7351,7 +7345,7 @@
         <v>259</v>
       </c>
       <c r="D10" s="150" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -7360,7 +7354,7 @@
         <v>662</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -7375,7 +7369,7 @@
         <v>260</v>
       </c>
       <c r="D11" s="150" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -7384,7 +7378,7 @@
         <v>665</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -7402,7 +7396,7 @@
         <v>261</v>
       </c>
       <c r="D12" s="150" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -7411,7 +7405,7 @@
         <v>446</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -7426,7 +7420,7 @@
         <v>256</v>
       </c>
       <c r="D13" s="150" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -7435,7 +7429,7 @@
         <v>666</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -7519,7 +7513,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>10</v>
@@ -7546,13 +7540,13 @@
         <v>267</v>
       </c>
       <c r="D6" s="150" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="150" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="L6" t="str">
         <f>CONCATENATE("|[",C6,"](",D6,")|[Solution](",K6,")|[Articles](",F6,")")</f>
@@ -7567,19 +7561,19 @@
         <v>268</v>
       </c>
       <c r="D7" s="150" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="150" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>657</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L19" si="0">CONCATENATE("|[",C7,"](",D7,")|[Solution](",K7,")|[Articles](",F7,")")</f>
@@ -7594,19 +7588,19 @@
         <v>269</v>
       </c>
       <c r="D8" s="150" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="150" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>658</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -7621,19 +7615,19 @@
         <v>270</v>
       </c>
       <c r="D9" s="150" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="150" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>659</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -7648,19 +7642,19 @@
         <v>271</v>
       </c>
       <c r="D10" s="150" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="150" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="J10" s="21" t="s">
         <v>668</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -7678,19 +7672,19 @@
         <v>262</v>
       </c>
       <c r="D11" s="150" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="150" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>654</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -7705,19 +7699,19 @@
         <v>263</v>
       </c>
       <c r="D12" s="150" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="150" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>655</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -7732,19 +7726,19 @@
         <v>264</v>
       </c>
       <c r="D13" s="150" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="150" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="J13" s="16" t="s">
         <v>652</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -7759,13 +7753,13 @@
         <v>265</v>
       </c>
       <c r="D14" s="150" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="150" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="G14" t="s">
         <v>648</v>
@@ -7774,7 +7768,7 @@
         <v>653</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -7789,13 +7783,13 @@
         <v>266</v>
       </c>
       <c r="D15" s="150" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="150" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>651</v>
@@ -7804,7 +7798,7 @@
         <v>656</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -7819,19 +7813,19 @@
         <v>272</v>
       </c>
       <c r="D16" s="150" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="150" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>667</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -7846,19 +7840,19 @@
         <v>273</v>
       </c>
       <c r="D17" s="150" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="150" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>660</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -7876,10 +7870,10 @@
         <v>274</v>
       </c>
       <c r="D18" s="150" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="F18" s="150" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -7897,10 +7891,10 @@
         <v>275</v>
       </c>
       <c r="D19" s="150" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="F19" s="150" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="G19" t="s">
         <v>681</v>
@@ -7985,482 +7979,482 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="B1" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="172" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="B2" s="172" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="172" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B3" s="172" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="172" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="B4" s="172" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="172" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B5" s="172" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="172" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B6" s="172" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="172" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B7" s="172" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="172" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B8" s="172" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="172" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="B9" s="172" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="172" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="B10" s="172" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="172" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B11" s="172" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="172" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="B12" s="172" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="172" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B13" s="172" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="172" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B14" s="172" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="172" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="B15" s="172" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="172" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="B16" s="172" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="172" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B17" s="172" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="172" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="B18" s="172" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="172" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="B19" s="172" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="172" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="B20" s="172" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="172" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="B21" s="172" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="172" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="B22" s="172" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="172" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="B23" s="172" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="172" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B24" s="172" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="172" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="B25" s="172" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="172" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="B26" s="172" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="172" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="B27" s="172" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="172" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="B28" s="172" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="172" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="B29" s="172" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="172" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B30" s="172" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="172" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B31" s="172" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="172" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="B32" s="172" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="172" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B33" s="172" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="172" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="B34" s="172" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="172" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="B35" s="172" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="172" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="B36" s="172" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="172" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="B37" s="172" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="172" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="B38" s="172" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="172" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="B39" s="172" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="172" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B40" s="172" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="172" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B41" s="172" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="172" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="B42" s="172" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="172" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B43" s="172" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="172" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="B44" s="172" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="172" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B45" s="172" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="172" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B46" s="172" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="172" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="B47" s="172" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="172" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B48" s="172" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="172" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="B49" s="172" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="172" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B50" s="172" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="172" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="B51" s="172" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="172" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="B52" s="172" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="172" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B53" s="172" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="172" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B54" s="172" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="172" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B55" s="172" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="172" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B56" s="172" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="172" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="B57" s="172" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="172" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B58" s="172" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="172" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B59" s="172" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="172" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B60" s="172" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -8696,7 +8690,7 @@
         <v>276</v>
       </c>
       <c r="D4" s="150" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",K4,")|")</f>
@@ -8714,7 +8708,7 @@
         <v>278</v>
       </c>
       <c r="D5" s="150" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="G5" t="s">
         <v>669</v>
@@ -8726,7 +8720,7 @@
         <v>674</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L25" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",K5,")|")</f>
@@ -8744,7 +8738,7 @@
         <v>279</v>
       </c>
       <c r="D6" s="150" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>671</v>
@@ -8756,7 +8750,7 @@
         <v>675</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -8774,13 +8768,13 @@
         <v>280</v>
       </c>
       <c r="D7" s="150" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>699</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -8798,13 +8792,13 @@
         <v>281</v>
       </c>
       <c r="D8" s="150" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>700</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -8822,13 +8816,13 @@
         <v>282</v>
       </c>
       <c r="D9" s="150" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>701</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -8846,13 +8840,13 @@
         <v>283</v>
       </c>
       <c r="D10" s="150" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>702</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -8870,13 +8864,13 @@
         <v>284</v>
       </c>
       <c r="D11" s="150" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>703</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -8894,13 +8888,13 @@
         <v>285</v>
       </c>
       <c r="D12" s="150" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>704</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -8918,13 +8912,13 @@
         <v>286</v>
       </c>
       <c r="D13" s="150" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="J13" s="16" t="s">
         <v>705</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -8942,13 +8936,13 @@
         <v>287</v>
       </c>
       <c r="D14" s="150" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="J14" s="16" t="s">
         <v>706</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -8966,7 +8960,7 @@
         <v>288</v>
       </c>
       <c r="D15" s="150" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="G15" t="s">
         <v>698</v>
@@ -8975,7 +8969,7 @@
         <v>707</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -8993,7 +8987,7 @@
         <v>289</v>
       </c>
       <c r="D16" s="150" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="G16" t="s">
         <v>697</v>
@@ -9002,7 +8996,7 @@
         <v>708</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -9020,7 +9014,7 @@
         <v>290</v>
       </c>
       <c r="D17" s="150" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="G17" t="s">
         <v>687</v>
@@ -9029,7 +9023,7 @@
         <v>709</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -9047,7 +9041,7 @@
         <v>692</v>
       </c>
       <c r="D18" s="150" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="G18" t="s">
         <v>688</v>
@@ -9062,7 +9056,7 @@
         <v>710</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -9080,7 +9074,7 @@
         <v>691</v>
       </c>
       <c r="D19" s="150" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="G19" t="s">
         <v>689</v>
@@ -9092,7 +9086,7 @@
         <v>711</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -9110,7 +9104,7 @@
         <v>291</v>
       </c>
       <c r="D20" s="150" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="G20" t="s">
         <v>695</v>
@@ -9122,7 +9116,7 @@
         <v>718</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -9140,7 +9134,7 @@
         <v>277</v>
       </c>
       <c r="D21" s="150" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="G21" t="s">
         <v>716</v>
@@ -9152,7 +9146,7 @@
         <v>719</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -9161,10 +9155,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C22" s="16" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
@@ -9176,7 +9170,7 @@
         <v>721</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
@@ -9188,7 +9182,7 @@
         <v>722</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
@@ -9200,7 +9194,7 @@
         <v>723</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
@@ -9632,10 +9626,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="144" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E4" s="164" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>5</v>
@@ -9656,7 +9650,7 @@
         <v>47</v>
       </c>
       <c r="M4" s="147" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="N4" t="str">
         <f>CONCATENATE("|[",D4,"](",E4,")|[Solution](",M4,")|")</f>
@@ -9671,10 +9665,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="139" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E5" s="165" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>5</v>
@@ -9695,7 +9689,7 @@
         <v>48</v>
       </c>
       <c r="M5" s="148" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N34" si="0">CONCATENATE("|[",D5,"](",E5,")|[Solution](",M5,")|")</f>
@@ -9710,10 +9704,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="139" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E6" s="165" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>5</v>
@@ -9734,7 +9728,7 @@
         <v>53</v>
       </c>
       <c r="M6" s="148" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
@@ -9749,10 +9743,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="139" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E7" s="165" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>5</v>
@@ -9773,7 +9767,7 @@
         <v>54</v>
       </c>
       <c r="M7" s="148" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
@@ -9788,10 +9782,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="139" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E8" s="165" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>5</v>
@@ -9812,7 +9806,7 @@
         <v>55</v>
       </c>
       <c r="M8" s="148" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
@@ -9824,10 +9818,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="139" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E9" s="165" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>6</v>
@@ -9845,7 +9839,7 @@
         <v>62</v>
       </c>
       <c r="M9" s="148" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
@@ -9860,10 +9854,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="139" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E10" s="165" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>5</v>
@@ -9887,7 +9881,7 @@
         <v>58</v>
       </c>
       <c r="M10" s="148" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
@@ -9902,10 +9896,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="139" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E11" s="165" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>5</v>
@@ -9929,7 +9923,7 @@
         <v>61</v>
       </c>
       <c r="M11" s="148" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
@@ -9944,10 +9938,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="140" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E12" s="166" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>5</v>
@@ -9965,7 +9959,7 @@
         <v>65</v>
       </c>
       <c r="M12" s="148" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
@@ -9980,10 +9974,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="140" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E13" s="166" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>5</v>
@@ -10004,7 +9998,7 @@
         <v>67</v>
       </c>
       <c r="M13" s="148" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
@@ -10019,10 +10013,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="140" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E14" s="166" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>5</v>
@@ -10043,7 +10037,7 @@
         <v>69</v>
       </c>
       <c r="M14" s="148" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
@@ -10058,10 +10052,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="140" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E15" s="166" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>5</v>
@@ -10076,7 +10070,7 @@
         <v>402</v>
       </c>
       <c r="M15" s="148" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
@@ -10091,10 +10085,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="140" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E16" s="166" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>5</v>
@@ -10109,7 +10103,7 @@
         <v>403</v>
       </c>
       <c r="M16" s="148" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
@@ -10124,10 +10118,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="140" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E17" s="166" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>5</v>
@@ -10145,7 +10139,7 @@
         <v>404</v>
       </c>
       <c r="M17" s="148" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
@@ -10160,10 +10154,10 @@
         <v>4</v>
       </c>
       <c r="D18" s="142" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E18" s="167" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>5</v>
@@ -10181,7 +10175,7 @@
         <v>641</v>
       </c>
       <c r="M18" s="148" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
@@ -10196,10 +10190,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="142" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E19" s="167" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>5</v>
@@ -10214,7 +10208,7 @@
         <v>642</v>
       </c>
       <c r="M19" s="148" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="0"/>
@@ -10229,10 +10223,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="142" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E20" s="167" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
@@ -10247,7 +10241,7 @@
         <v>640</v>
       </c>
       <c r="M20" s="148" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="0"/>
@@ -10262,10 +10256,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="142" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E21" s="167" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
@@ -10280,7 +10274,7 @@
         <v>638</v>
       </c>
       <c r="M21" s="148" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="0"/>
@@ -10295,10 +10289,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="142" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E22" s="167" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
@@ -10313,7 +10307,7 @@
         <v>639</v>
       </c>
       <c r="M22" s="148" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="0"/>
@@ -10328,10 +10322,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="141" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E23" s="168" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -10352,7 +10346,7 @@
         <v>637</v>
       </c>
       <c r="M23" s="148" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="0"/>
@@ -10367,10 +10361,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="141" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E24" s="168" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -10391,7 +10385,7 @@
         <v>632</v>
       </c>
       <c r="M24" s="148" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="0"/>
@@ -10406,10 +10400,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="141" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E25" s="168" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>5</v>
@@ -10427,7 +10421,7 @@
         <v>633</v>
       </c>
       <c r="M25" s="148" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="0"/>
@@ -10442,10 +10436,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="141" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E26" s="168" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>5</v>
@@ -10463,7 +10457,7 @@
         <v>634</v>
       </c>
       <c r="M26" s="148" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="0"/>
@@ -10478,10 +10472,10 @@
         <v>4</v>
       </c>
       <c r="D27" s="141" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E27" s="168" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>5</v>
@@ -10502,7 +10496,7 @@
         <v>635</v>
       </c>
       <c r="M27" s="148" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="0"/>
@@ -10517,10 +10511,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="141" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E28" s="168" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>5</v>
@@ -10538,7 +10532,7 @@
         <v>636</v>
       </c>
       <c r="M28" s="148" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="0"/>
@@ -10553,10 +10547,10 @@
         <v>4</v>
       </c>
       <c r="D29" s="141" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E29" s="168" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>5</v>
@@ -10577,7 +10571,7 @@
         <v>631</v>
       </c>
       <c r="M29" s="148" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="0"/>
@@ -10592,10 +10586,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="143" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E30" s="169" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>5</v>
@@ -10616,7 +10610,7 @@
         <v>626</v>
       </c>
       <c r="M30" s="148" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="0"/>
@@ -10631,10 +10625,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="143" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E31" s="169" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>5</v>
@@ -10655,7 +10649,7 @@
         <v>630</v>
       </c>
       <c r="M31" s="148" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="0"/>
@@ -10670,10 +10664,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="143" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E32" s="169" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>5</v>
@@ -10694,7 +10688,7 @@
         <v>629</v>
       </c>
       <c r="M32" s="148" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="0"/>
@@ -10703,10 +10697,10 @@
     </row>
     <row r="33" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="143" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E33" s="169" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="H33" s="2">
         <v>2</v>
@@ -10718,7 +10712,7 @@
         <v>628</v>
       </c>
       <c r="M33" s="148" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="0"/>
@@ -10733,10 +10727,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="143" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E34" s="169" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>5</v>
@@ -10757,7 +10751,7 @@
         <v>627</v>
       </c>
       <c r="M34" s="149" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="0"/>
@@ -11545,7 +11539,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="150" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
@@ -11560,7 +11554,7 @@
         <v>298</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="L5" t="str">
         <f>CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
@@ -11575,7 +11569,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -11590,7 +11584,7 @@
         <v>297</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ref="L6:L21" si="0">CONCATENATE("|[",B6,"](",C6,")|[Solution](",K6,")|")</f>
@@ -11605,7 +11599,7 @@
         <v>302</v>
       </c>
       <c r="C7" s="150" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -11620,7 +11614,7 @@
         <v>504</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -11635,7 +11629,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="150" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -11650,7 +11644,7 @@
         <v>306</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -11665,7 +11659,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="150" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -11677,7 +11671,7 @@
         <v>308</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -11692,7 +11686,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="150" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>5</v>
@@ -11706,7 +11700,7 @@
         <v>317</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -11721,7 +11715,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="150" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
@@ -11739,7 +11733,7 @@
         <v>392</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -11754,7 +11748,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="150" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -11769,7 +11763,7 @@
         <v>393</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -11784,7 +11778,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="150" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -11799,7 +11793,7 @@
         <v>390</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -11814,7 +11808,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="150" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>5</v>
@@ -11831,7 +11825,7 @@
         <v>391</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -11846,7 +11840,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="150" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -11861,7 +11855,7 @@
         <v>388</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -11876,7 +11870,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="150" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -11888,7 +11882,7 @@
         <v>389</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -11903,7 +11897,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="150" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
@@ -11915,7 +11909,7 @@
         <v>394</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -11930,7 +11924,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="150" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -11942,7 +11936,7 @@
         <v>395</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -11957,7 +11951,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="150" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
@@ -11966,7 +11960,7 @@
         <v>396</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -11981,7 +11975,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="150" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
@@ -11999,7 +11993,7 @@
         <v>397</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -12014,7 +12008,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="150" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D21" s="53" t="s">
         <v>5</v>
@@ -12028,7 +12022,7 @@
         <v>398</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -12599,7 +12593,7 @@
         <v>379</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -12615,7 +12609,7 @@
         <v>382</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",B4,"](",C4,")|[Solution](",K4,")|")</f>
@@ -12630,7 +12624,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="158" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -12642,7 +12636,7 @@
         <v>381</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L11" si="0">CONCATENATE("|[",B5,"](",C5,")|[Solution](",K5,")|")</f>
@@ -12657,7 +12651,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="158" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -12671,7 +12665,7 @@
         <v>407</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -12686,7 +12680,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="158" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -12700,7 +12694,7 @@
         <v>406</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -12715,7 +12709,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -12729,7 +12723,7 @@
         <v>410</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -12744,7 +12738,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="158" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -12758,7 +12752,7 @@
         <v>409</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -12773,7 +12767,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
@@ -12789,7 +12783,7 @@
         <v>408</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -12822,7 +12816,7 @@
         <v>377</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -12884,8 +12878,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12923,7 +12917,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>455</v>
@@ -12958,7 +12952,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -12978,7 +12972,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -12998,7 +12992,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -13018,7 +13012,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -13038,7 +13032,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13058,7 +13052,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -13085,9 +13079,6 @@
       <c r="B11" s="89" t="s">
         <v>727</v>
       </c>
-      <c r="C11" t="s">
-        <v>729</v>
-      </c>
       <c r="D11" s="136" t="s">
         <v>154</v>
       </c>
@@ -13105,9 +13096,6 @@
       <c r="B12" s="89" t="s">
         <v>727</v>
       </c>
-      <c r="C12" t="s">
-        <v>729</v>
-      </c>
       <c r="D12" s="136" t="s">
         <v>155</v>
       </c>
@@ -13125,9 +13113,6 @@
       <c r="B13" s="134" t="s">
         <v>728</v>
       </c>
-      <c r="C13" t="s">
-        <v>730</v>
-      </c>
       <c r="D13" s="136" t="s">
         <v>156</v>
       </c>
@@ -13148,9 +13133,6 @@
       <c r="B14" s="134" t="s">
         <v>728</v>
       </c>
-      <c r="C14" t="s">
-        <v>730</v>
-      </c>
       <c r="D14" s="136" t="s">
         <v>157</v>
       </c>
@@ -13171,9 +13153,6 @@
       <c r="B15" s="134" t="s">
         <v>728</v>
       </c>
-      <c r="C15" t="s">
-        <v>730</v>
-      </c>
       <c r="D15" s="137" t="s">
         <v>158</v>
       </c>
@@ -13192,7 +13171,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D16" s="84" t="s">
         <v>159</v>
@@ -13209,7 +13188,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="89" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D17" s="84" t="s">
         <v>160</v>
@@ -13226,7 +13205,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="89" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D18" s="84" t="s">
         <v>161</v>
@@ -13243,7 +13222,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="89" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D19" s="84" t="s">
         <v>162</v>
@@ -13260,7 +13239,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="89" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D20" s="84" t="s">
         <v>163</v>
@@ -13277,7 +13256,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="89" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D21" s="72" t="s">
         <v>164</v>
@@ -13294,7 +13273,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="89" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D22" s="72" t="s">
         <v>165</v>
@@ -13311,7 +13290,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D23" s="72" t="s">
         <v>166</v>
@@ -13328,7 +13307,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="134" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D24" s="73" t="s">
         <v>167</v>
@@ -13345,7 +13324,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="134" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D25" s="73" t="s">
         <v>168</v>
@@ -13362,7 +13341,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="134" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D26" s="73" t="s">
         <v>169</v>
@@ -13379,7 +13358,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="134" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D27" s="73" t="s">
         <v>170</v>
@@ -13396,7 +13375,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="134" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D28" s="71" t="s">
         <v>171</v>
@@ -13413,7 +13392,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="134" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D29" s="71" t="s">
         <v>172</v>
@@ -13430,7 +13409,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="134" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D30" s="71" t="s">
         <v>173</v>
@@ -13604,7 +13583,7 @@
         <v>209</v>
       </c>
       <c r="D9" s="158" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -13613,7 +13592,7 @@
         <v>416</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M9" t="str">
         <f>CONCATENATE("|[",C9,"](",D9,")|[Solution](",L9,")|")</f>
@@ -13628,7 +13607,7 @@
         <v>210</v>
       </c>
       <c r="D10" s="158" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -13637,7 +13616,7 @@
         <v>416</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ref="M10:M34" si="0">CONCATENATE("|[",C10,"](",D10,")|[Solution](",L10,")|")</f>
@@ -13652,7 +13631,7 @@
         <v>211</v>
       </c>
       <c r="D11" s="158" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -13661,7 +13640,7 @@
         <v>416</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
@@ -13676,7 +13655,7 @@
         <v>212</v>
       </c>
       <c r="D12" s="158" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -13685,7 +13664,7 @@
         <v>416</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
@@ -13700,7 +13679,7 @@
         <v>213</v>
       </c>
       <c r="D13" s="158" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -13709,7 +13688,7 @@
         <v>416</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
@@ -13724,7 +13703,7 @@
         <v>214</v>
       </c>
       <c r="D14" s="158" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -13733,7 +13712,7 @@
         <v>416</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -13748,7 +13727,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="158" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -13757,7 +13736,7 @@
         <v>416</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
@@ -13772,7 +13751,7 @@
         <v>216</v>
       </c>
       <c r="D16" s="158" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -13781,7 +13760,7 @@
         <v>416</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -13796,7 +13775,7 @@
         <v>217</v>
       </c>
       <c r="D17" s="158" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -13811,7 +13790,7 @@
         <v>487</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -13826,7 +13805,7 @@
         <v>218</v>
       </c>
       <c r="D18" s="158" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -13838,7 +13817,7 @@
         <v>488</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -13853,7 +13832,7 @@
         <v>219</v>
       </c>
       <c r="D19" s="158" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -13865,7 +13844,7 @@
         <v>483</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -13880,7 +13859,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="158" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -13892,7 +13871,7 @@
         <v>484</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -13907,7 +13886,7 @@
         <v>221</v>
       </c>
       <c r="D21" s="158" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -13919,7 +13898,7 @@
         <v>485</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -13934,7 +13913,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="158" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -13946,7 +13925,7 @@
         <v>486</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
@@ -13961,7 +13940,7 @@
         <v>223</v>
       </c>
       <c r="D23" s="158" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -13979,7 +13958,7 @@
         <v>466</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -13994,7 +13973,7 @@
         <v>224</v>
       </c>
       <c r="D24" s="158" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -14003,7 +13982,7 @@
         <v>468</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
@@ -14018,7 +13997,7 @@
         <v>225</v>
       </c>
       <c r="D25" s="158" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -14030,7 +14009,7 @@
         <v>482</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
@@ -14045,7 +14024,7 @@
         <v>178</v>
       </c>
       <c r="D26" s="158" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -14054,7 +14033,7 @@
         <v>481</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
@@ -14069,7 +14048,7 @@
         <v>226</v>
       </c>
       <c r="D27" s="158" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -14078,7 +14057,7 @@
         <v>489</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
@@ -14093,7 +14072,7 @@
         <v>227</v>
       </c>
       <c r="D28" s="158" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
@@ -14102,7 +14081,7 @@
         <v>499</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
@@ -14117,7 +14096,7 @@
         <v>228</v>
       </c>
       <c r="D29" s="158" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -14126,7 +14105,7 @@
         <v>500</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
@@ -14141,7 +14120,7 @@
         <v>229</v>
       </c>
       <c r="D30" s="158" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -14153,7 +14132,7 @@
         <v>501</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
@@ -14168,7 +14147,7 @@
         <v>230</v>
       </c>
       <c r="D31" s="158" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -14186,7 +14165,7 @@
         <v>503</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
@@ -14201,7 +14180,7 @@
         <v>231</v>
       </c>
       <c r="D32" s="158" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -14216,7 +14195,7 @@
         <v>515</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
@@ -14231,7 +14210,7 @@
         <v>179</v>
       </c>
       <c r="D33" s="158" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -14243,7 +14222,7 @@
         <v>519</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
@@ -14261,7 +14240,7 @@
         <v>505</v>
       </c>
       <c r="D34" s="158" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -14273,7 +14252,7 @@
         <v>520</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="0"/>
@@ -14556,7 +14535,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>10</v>
@@ -14582,10 +14561,10 @@
         <v>180</v>
       </c>
       <c r="D4" s="150" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F4" s="172" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -14594,7 +14573,7 @@
         <v>521</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("|[",C4,"](",D4,")|[Solution](",K4,")|[Articles](",F4,")")</f>
@@ -14612,16 +14591,16 @@
         <v>181</v>
       </c>
       <c r="D5" s="150" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F5" s="172" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>521</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L33" si="0">CONCATENATE("|[",C5,"](",D5,")|[Solution](",K5,")|[Articles](",F5,")")</f>
@@ -14636,13 +14615,13 @@
         <v>182</v>
       </c>
       <c r="D6" s="150" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="172" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="G6" s="93" t="s">
         <v>527</v>
@@ -14657,7 +14636,7 @@
         <v>521</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -14672,13 +14651,13 @@
         <v>183</v>
       </c>
       <c r="D7" s="150" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="172" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="G7" t="s">
         <v>463</v>
@@ -14690,7 +14669,7 @@
         <v>523</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -14705,13 +14684,13 @@
         <v>184</v>
       </c>
       <c r="D8" s="150" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="172" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="G8" t="s">
         <v>463</v>
@@ -14723,7 +14702,7 @@
         <v>524</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -14738,13 +14717,13 @@
         <v>185</v>
       </c>
       <c r="D9" s="150" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="172" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="G9" t="s">
         <v>463</v>
@@ -14756,7 +14735,7 @@
         <v>522</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -14771,13 +14750,13 @@
         <v>186</v>
       </c>
       <c r="D10" s="150" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="172" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="G10" s="95" t="s">
         <v>463</v>
@@ -14792,7 +14771,7 @@
         <v>529</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -14807,13 +14786,13 @@
         <v>187</v>
       </c>
       <c r="D11" s="150" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="172" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="G11" s="94" t="s">
         <v>534</v>
@@ -14828,7 +14807,7 @@
         <v>530</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -14846,13 +14825,13 @@
         <v>188</v>
       </c>
       <c r="D12" s="150" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="172" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="G12" t="s">
         <v>535</v>
@@ -14867,7 +14846,7 @@
         <v>531</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -14882,13 +14861,13 @@
         <v>189</v>
       </c>
       <c r="D13" s="150" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="172" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="G13" t="s">
         <v>543</v>
@@ -14900,7 +14879,7 @@
         <v>532</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -14918,17 +14897,17 @@
         <v>190</v>
       </c>
       <c r="D14" s="150" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F14" s="172" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="G14" s="18"/>
       <c r="J14" s="16" t="s">
         <v>531</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -14943,19 +14922,19 @@
         <v>191</v>
       </c>
       <c r="D15" s="150" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="172" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>587</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -14970,19 +14949,19 @@
         <v>192</v>
       </c>
       <c r="D16" s="150" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="172" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>602</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -14997,19 +14976,19 @@
         <v>193</v>
       </c>
       <c r="D17" s="150" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="172" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>603</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -15024,19 +15003,19 @@
         <v>194</v>
       </c>
       <c r="D18" s="150" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="172" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>603</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -15051,13 +15030,13 @@
         <v>545</v>
       </c>
       <c r="D19" s="150" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="172" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="G19" t="s">
         <v>565</v>
@@ -15066,7 +15045,7 @@
         <v>601</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -15081,13 +15060,13 @@
         <v>195</v>
       </c>
       <c r="D20" s="150" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="172" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="G20" t="s">
         <v>566</v>
@@ -15096,7 +15075,7 @@
         <v>600</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -15111,13 +15090,13 @@
         <v>196</v>
       </c>
       <c r="D21" s="150" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="172" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="G21" t="s">
         <v>567</v>
@@ -15126,7 +15105,7 @@
         <v>599</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -15141,13 +15120,13 @@
         <v>197</v>
       </c>
       <c r="D22" s="150" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="172" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="G22" t="s">
         <v>568</v>
@@ -15159,7 +15138,7 @@
         <v>598</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
@@ -15174,13 +15153,13 @@
         <v>198</v>
       </c>
       <c r="D23" s="150" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="172" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="G23" t="s">
         <v>546</v>
@@ -15192,7 +15171,7 @@
         <v>597</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
@@ -15207,13 +15186,13 @@
         <v>199</v>
       </c>
       <c r="D24" s="150" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="G24" t="s">
         <v>547</v>
@@ -15222,7 +15201,7 @@
         <v>596</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
@@ -15237,13 +15216,13 @@
         <v>200</v>
       </c>
       <c r="D25" s="150" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="172" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="G25" t="s">
         <v>548</v>
@@ -15252,7 +15231,7 @@
         <v>595</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
@@ -15267,13 +15246,13 @@
         <v>201</v>
       </c>
       <c r="D26" s="150" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E26" t="s">
         <v>606</v>
       </c>
       <c r="F26" s="172" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="G26" t="s">
         <v>549</v>
@@ -15285,7 +15264,7 @@
         <v>592</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="0"/>
@@ -15300,13 +15279,13 @@
         <v>202</v>
       </c>
       <c r="D27" s="150" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="172" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>550</v>
@@ -15318,7 +15297,7 @@
         <v>588</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="0"/>
@@ -15333,13 +15312,13 @@
         <v>203</v>
       </c>
       <c r="D28" s="150" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="172" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>552</v>
@@ -15348,7 +15327,7 @@
         <v>589</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="0"/>
@@ -15363,13 +15342,13 @@
         <v>204</v>
       </c>
       <c r="D29" s="150" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="172" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="G29" t="s">
         <v>553</v>
@@ -15378,7 +15357,7 @@
         <v>590</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="0"/>
@@ -15393,13 +15372,13 @@
         <v>205</v>
       </c>
       <c r="D30" s="150" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="172" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>554</v>
@@ -15408,7 +15387,7 @@
         <v>593</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="0"/>
@@ -15423,13 +15402,13 @@
         <v>206</v>
       </c>
       <c r="D31" s="150" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>604</v>
       </c>
       <c r="F31" s="172" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>555</v>
@@ -15441,7 +15420,7 @@
         <v>591</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="0"/>
@@ -15456,13 +15435,13 @@
         <v>207</v>
       </c>
       <c r="D32" s="150" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E32" t="s">
         <v>605</v>
       </c>
       <c r="F32" s="172" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>556</v>
@@ -15474,7 +15453,7 @@
         <v>594</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="0"/>
@@ -15492,16 +15471,16 @@
         <v>208</v>
       </c>
       <c r="D33" s="150" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F33" s="172" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   25-01-2022 - 21:29:54.22
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B45D69-4AD2-4369-992D-438EF8751A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29208A5-D150-4D8F-B092-1F070B72B95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
     <sheet name="Leet" sheetId="13" r:id="rId2"/>
     <sheet name="Recursion&amp; BackTracking" sheetId="1" r:id="rId3"/>
-    <sheet name="Time and Space" sheetId="4" r:id="rId4"/>
-    <sheet name="Stack" sheetId="3" r:id="rId5"/>
-    <sheet name="Queue" sheetId="12" r:id="rId6"/>
-    <sheet name="DP" sheetId="2" r:id="rId7"/>
+    <sheet name="DP" sheetId="2" r:id="rId4"/>
+    <sheet name="Time and Space" sheetId="4" r:id="rId5"/>
+    <sheet name="Stack" sheetId="3" r:id="rId6"/>
+    <sheet name="Queue" sheetId="12" r:id="rId7"/>
     <sheet name="Linked List" sheetId="5" r:id="rId8"/>
     <sheet name="Generic Tree" sheetId="6" r:id="rId9"/>
     <sheet name="Binary Tree" sheetId="7" r:id="rId10"/>
@@ -7472,8 +7472,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7531,7 +7531,7 @@
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" s="89" t="s">
         <v>564</v>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C7" s="98" t="s">
         <v>268</v>
@@ -7582,7 +7582,7 @@
     </row>
     <row r="8" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C8" s="98" t="s">
         <v>269</v>
@@ -7609,7 +7609,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C9" s="98" t="s">
         <v>270</v>
@@ -7636,7 +7636,7 @@
     </row>
     <row r="10" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="120" t="s">
         <v>271</v>
@@ -7663,7 +7663,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B11" s="89" t="s">
         <v>564</v>
@@ -7693,7 +7693,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12" s="127" t="s">
         <v>263</v>
@@ -7720,7 +7720,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C13" s="127" t="s">
         <v>264</v>
@@ -7747,7 +7747,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C14" s="127" t="s">
         <v>265</v>
@@ -7777,7 +7777,7 @@
     </row>
     <row r="15" spans="1:12" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C15" s="127" t="s">
         <v>266</v>
@@ -8623,8 +8623,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10912,6 +10912,603 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="51.85546875" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="52.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>724</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>725</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>725</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>7</v>
+      </c>
+      <c r="B10" s="89" t="s">
+        <v>726</v>
+      </c>
+      <c r="D10" s="135" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>8</v>
+      </c>
+      <c r="B11" s="89" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>9</v>
+      </c>
+      <c r="B12" s="89" t="s">
+        <v>727</v>
+      </c>
+      <c r="D12" s="136" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>10</v>
+      </c>
+      <c r="B13" s="134" t="s">
+        <v>728</v>
+      </c>
+      <c r="D13" s="136" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>11</v>
+      </c>
+      <c r="B14" s="134" t="s">
+        <v>728</v>
+      </c>
+      <c r="D14" s="136" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
+        <v>12</v>
+      </c>
+      <c r="B15" s="134" t="s">
+        <v>728</v>
+      </c>
+      <c r="D15" s="137" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>13</v>
+      </c>
+      <c r="B16" s="89" t="s">
+        <v>730</v>
+      </c>
+      <c r="D16" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>14</v>
+      </c>
+      <c r="B17" s="89" t="s">
+        <v>730</v>
+      </c>
+      <c r="D17" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>15</v>
+      </c>
+      <c r="B18" s="89" t="s">
+        <v>730</v>
+      </c>
+      <c r="D18" s="84" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>16</v>
+      </c>
+      <c r="B19" s="89" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" s="84" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>17</v>
+      </c>
+      <c r="B20" s="89" t="s">
+        <v>731</v>
+      </c>
+      <c r="D20" s="84" t="s">
+        <v>163</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>18</v>
+      </c>
+      <c r="B21" s="89" t="s">
+        <v>731</v>
+      </c>
+      <c r="D21" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>19</v>
+      </c>
+      <c r="B22" s="89" t="s">
+        <v>731</v>
+      </c>
+      <c r="D22" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>20</v>
+      </c>
+      <c r="B23" s="134" t="s">
+        <v>732</v>
+      </c>
+      <c r="D23" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>21</v>
+      </c>
+      <c r="B24" s="134" t="s">
+        <v>732</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>22</v>
+      </c>
+      <c r="B25" s="134" t="s">
+        <v>732</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>23</v>
+      </c>
+      <c r="B26" s="134" t="s">
+        <v>733</v>
+      </c>
+      <c r="D26" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <v>24</v>
+      </c>
+      <c r="B27" s="134" t="s">
+        <v>733</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="29">
+        <v>25</v>
+      </c>
+      <c r="B28" s="134" t="s">
+        <v>733</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="134" t="s">
+        <v>733</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <v>27</v>
+      </c>
+      <c r="B30" s="134" t="s">
+        <v>733</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="29">
+        <v>28</v>
+      </c>
+      <c r="D31" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" t="s">
+        <v>177</v>
+      </c>
+      <c r="G31" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="29">
+        <v>29</v>
+      </c>
+      <c r="D32" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="29">
+        <v>30</v>
+      </c>
+      <c r="D33" s="71" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/longest-string-chain/" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I27"/>
@@ -11441,7 +12038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L51"/>
@@ -12513,7 +13110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L15"/>
@@ -12873,609 +13470,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:K38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="52.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>455</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>724</v>
-      </c>
-      <c r="D4" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>724</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>724</v>
-      </c>
-      <c r="D6" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>725</v>
-      </c>
-      <c r="D7" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>725</v>
-      </c>
-      <c r="D8" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>726</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
-        <v>7</v>
-      </c>
-      <c r="B10" s="89" t="s">
-        <v>726</v>
-      </c>
-      <c r="D10" s="135" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
-      </c>
-      <c r="G10" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
-        <v>8</v>
-      </c>
-      <c r="B11" s="89" t="s">
-        <v>727</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>9</v>
-      </c>
-      <c r="B12" s="89" t="s">
-        <v>727</v>
-      </c>
-      <c r="D12" s="136" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" t="s">
-        <v>177</v>
-      </c>
-      <c r="G12" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
-        <v>10</v>
-      </c>
-      <c r="B13" s="134" t="s">
-        <v>728</v>
-      </c>
-      <c r="D13" s="136" t="s">
-        <v>156</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
-        <v>11</v>
-      </c>
-      <c r="B14" s="134" t="s">
-        <v>728</v>
-      </c>
-      <c r="D14" s="136" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
-        <v>12</v>
-      </c>
-      <c r="B15" s="134" t="s">
-        <v>728</v>
-      </c>
-      <c r="D15" s="137" t="s">
-        <v>158</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
-        <v>13</v>
-      </c>
-      <c r="B16" s="89" t="s">
-        <v>730</v>
-      </c>
-      <c r="D16" s="84" t="s">
-        <v>159</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
-        <v>14</v>
-      </c>
-      <c r="B17" s="89" t="s">
-        <v>730</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
-        <v>15</v>
-      </c>
-      <c r="B18" s="89" t="s">
-        <v>730</v>
-      </c>
-      <c r="D18" s="84" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
-        <v>16</v>
-      </c>
-      <c r="B19" s="89" t="s">
-        <v>731</v>
-      </c>
-      <c r="D19" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
-        <v>17</v>
-      </c>
-      <c r="B20" s="89" t="s">
-        <v>731</v>
-      </c>
-      <c r="D20" s="84" t="s">
-        <v>163</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
-        <v>18</v>
-      </c>
-      <c r="B21" s="89" t="s">
-        <v>731</v>
-      </c>
-      <c r="D21" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>19</v>
-      </c>
-      <c r="B22" s="89" t="s">
-        <v>731</v>
-      </c>
-      <c r="D22" s="72" t="s">
-        <v>165</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
-        <v>20</v>
-      </c>
-      <c r="B23" s="134" t="s">
-        <v>732</v>
-      </c>
-      <c r="D23" s="72" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>21</v>
-      </c>
-      <c r="B24" s="134" t="s">
-        <v>732</v>
-      </c>
-      <c r="D24" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
-        <v>22</v>
-      </c>
-      <c r="B25" s="134" t="s">
-        <v>732</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>23</v>
-      </c>
-      <c r="B26" s="134" t="s">
-        <v>733</v>
-      </c>
-      <c r="D26" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
-        <v>24</v>
-      </c>
-      <c r="B27" s="134" t="s">
-        <v>733</v>
-      </c>
-      <c r="D27" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>25</v>
-      </c>
-      <c r="B28" s="134" t="s">
-        <v>733</v>
-      </c>
-      <c r="D28" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
-        <v>26</v>
-      </c>
-      <c r="B29" s="134" t="s">
-        <v>733</v>
-      </c>
-      <c r="D29" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>27</v>
-      </c>
-      <c r="B30" s="134" t="s">
-        <v>733</v>
-      </c>
-      <c r="D30" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="E30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
-        <v>28</v>
-      </c>
-      <c r="D31" s="71" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
-        <v>29</v>
-      </c>
-      <c r="D32" s="71" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
-        <v>30</v>
-      </c>
-      <c r="D33" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
-        <v>456</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/longest-string-chain/" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -14487,7 +14487,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   Sat 01/04/2025 - 10:55:29.89
</commit_message>
<xml_diff>
--- a/Level1.xlsx
+++ b/Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="852" activeTab="9"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -6449,7 +6449,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -7568,18 +7568,21 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K$1:L$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="4" width="41.2857142857143" style="29" customWidth="1"/>
-    <col min="6" max="6" width="24.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="47.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="39.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="42.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="41.2857142857143" style="29" customWidth="1"/>
+    <col min="4" max="4" width="41.2857142857143" style="29" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7142857142857" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="47.7142857142857" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="39.8571428571429" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="42.4285714285714" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="42.1428571428571" customWidth="1"/>
+    <col min="11" max="12" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4">

</xml_diff>